<commit_message>
1st day round of 16 results
</commit_message>
<xml_diff>
--- a/2025 FIVB Women's Volleyball World Championship.xlsx
+++ b/2025 FIVB Women's Volleyball World Championship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72CA0183-BB33-4970-AA14-02B60B0F886D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8AA3544-59FD-4827-8403-BC02A947CAAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC01" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="2" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
@@ -863,28 +863,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -912,22 +906,28 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5393,11 +5393,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:X1"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
@@ -5406,6 +5401,11 @@
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:X1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5478,74 +5478,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:67" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="56"/>
-      <c r="AW2" s="56"/>
-      <c r="AX2" s="56"/>
-      <c r="AY2" s="56"/>
-      <c r="AZ2" s="56"/>
-      <c r="BA2" s="56"/>
-      <c r="BB2" s="56"/>
-      <c r="BC2" s="56"/>
-      <c r="BD2" s="56"/>
-      <c r="BE2" s="56"/>
-      <c r="BF2" s="56"/>
-      <c r="BG2" s="56"/>
-      <c r="BH2" s="56"/>
-      <c r="BI2" s="56"/>
-      <c r="BJ2" s="56"/>
-      <c r="BK2" s="56"/>
-      <c r="BL2" s="56"/>
-      <c r="BM2" s="56"/>
-      <c r="BN2" s="56"/>
-      <c r="BO2" s="56"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="75"/>
+      <c r="AW2" s="75"/>
+      <c r="AX2" s="75"/>
+      <c r="AY2" s="75"/>
+      <c r="AZ2" s="75"/>
+      <c r="BA2" s="75"/>
+      <c r="BB2" s="75"/>
+      <c r="BC2" s="75"/>
+      <c r="BD2" s="75"/>
+      <c r="BE2" s="75"/>
+      <c r="BF2" s="75"/>
+      <c r="BG2" s="75"/>
+      <c r="BH2" s="75"/>
+      <c r="BI2" s="75"/>
+      <c r="BJ2" s="75"/>
+      <c r="BK2" s="75"/>
+      <c r="BL2" s="75"/>
+      <c r="BM2" s="75"/>
+      <c r="BN2" s="75"/>
+      <c r="BO2" s="75"/>
     </row>
     <row r="3" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AX3" s="33"/>
@@ -5568,116 +5568,116 @@
       <c r="BO3" s="33"/>
     </row>
     <row r="4" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="57"/>
-      <c r="AO4" s="57"/>
-      <c r="AP4" s="57"/>
-      <c r="AQ4" s="57"/>
-      <c r="AR4" s="57"/>
-      <c r="AS4" s="57"/>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="57"/>
-      <c r="AV4" s="57"/>
-      <c r="AW4" s="57"/>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="57"/>
-      <c r="AZ4" s="57"/>
-      <c r="BA4" s="57"/>
-      <c r="BB4" s="57"/>
-      <c r="BC4" s="57"/>
-      <c r="BD4" s="57"/>
-      <c r="BE4" s="57"/>
-      <c r="BF4" s="57"/>
-      <c r="BG4" s="57"/>
-      <c r="BH4" s="57"/>
-      <c r="BI4" s="57"/>
-      <c r="BJ4" s="57"/>
-      <c r="BK4" s="57"/>
-      <c r="BL4" s="57"/>
-      <c r="BM4" s="57"/>
-      <c r="BN4" s="57"/>
-      <c r="BO4" s="57"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="76"/>
+      <c r="BF4" s="76"/>
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="76"/>
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="76"/>
+      <c r="BM4" s="76"/>
+      <c r="BN4" s="76"/>
+      <c r="BO4" s="76"/>
     </row>
     <row r="5" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75" t="s">
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="75" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="75" t="s">
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
       <c r="AD5" s="12" t="s">
         <v>23</v>
       </c>
@@ -5735,34 +5735,34 @@
       <c r="AW5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX5" s="61" t="s">
+      <c r="AX5" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="AY5" s="62"/>
-      <c r="AZ5" s="63"/>
-      <c r="BA5" s="61" t="s">
+      <c r="AY5" s="73"/>
+      <c r="AZ5" s="74"/>
+      <c r="BA5" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="BB5" s="62"/>
-      <c r="BC5" s="63"/>
-      <c r="BD5" s="61" t="s">
+      <c r="BB5" s="73"/>
+      <c r="BC5" s="74"/>
+      <c r="BD5" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="BE5" s="62"/>
-      <c r="BF5" s="62"/>
-      <c r="BG5" s="62"/>
-      <c r="BH5" s="62"/>
-      <c r="BI5" s="63"/>
-      <c r="BJ5" s="61" t="s">
+      <c r="BE5" s="73"/>
+      <c r="BF5" s="73"/>
+      <c r="BG5" s="73"/>
+      <c r="BH5" s="73"/>
+      <c r="BI5" s="74"/>
+      <c r="BJ5" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="BK5" s="62"/>
-      <c r="BL5" s="63"/>
-      <c r="BM5" s="61" t="s">
+      <c r="BK5" s="73"/>
+      <c r="BL5" s="74"/>
+      <c r="BM5" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="BN5" s="62"/>
-      <c r="BO5" s="63"/>
+      <c r="BN5" s="73"/>
+      <c r="BO5" s="74"/>
     </row>
     <row r="6" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B6" s="23">
@@ -7031,116 +7031,116 @@
       </c>
     </row>
     <row r="12" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="57"/>
-      <c r="AA12" s="57"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="57"/>
-      <c r="AD12" s="57"/>
-      <c r="AE12" s="57"/>
-      <c r="AF12" s="57"/>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="57"/>
-      <c r="AJ12" s="57"/>
-      <c r="AK12" s="57"/>
-      <c r="AL12" s="57"/>
-      <c r="AM12" s="57"/>
-      <c r="AN12" s="57"/>
-      <c r="AO12" s="57"/>
-      <c r="AP12" s="57"/>
-      <c r="AQ12" s="57"/>
-      <c r="AR12" s="57"/>
-      <c r="AS12" s="57"/>
-      <c r="AT12" s="57"/>
-      <c r="AU12" s="57"/>
-      <c r="AV12" s="57"/>
-      <c r="AW12" s="57"/>
-      <c r="AX12" s="57"/>
-      <c r="AY12" s="57"/>
-      <c r="AZ12" s="57"/>
-      <c r="BA12" s="57"/>
-      <c r="BB12" s="57"/>
-      <c r="BC12" s="57"/>
-      <c r="BD12" s="57"/>
-      <c r="BE12" s="57"/>
-      <c r="BF12" s="57"/>
-      <c r="BG12" s="57"/>
-      <c r="BH12" s="57"/>
-      <c r="BI12" s="57"/>
-      <c r="BJ12" s="57"/>
-      <c r="BK12" s="57"/>
-      <c r="BL12" s="57"/>
-      <c r="BM12" s="57"/>
-      <c r="BN12" s="57"/>
-      <c r="BO12" s="57"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="76"/>
+      <c r="R12" s="76"/>
+      <c r="S12" s="76"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="76"/>
+      <c r="V12" s="76"/>
+      <c r="W12" s="76"/>
+      <c r="X12" s="76"/>
+      <c r="Y12" s="76"/>
+      <c r="Z12" s="76"/>
+      <c r="AA12" s="76"/>
+      <c r="AB12" s="76"/>
+      <c r="AC12" s="76"/>
+      <c r="AD12" s="76"/>
+      <c r="AE12" s="76"/>
+      <c r="AF12" s="76"/>
+      <c r="AG12" s="76"/>
+      <c r="AH12" s="76"/>
+      <c r="AI12" s="76"/>
+      <c r="AJ12" s="76"/>
+      <c r="AK12" s="76"/>
+      <c r="AL12" s="76"/>
+      <c r="AM12" s="76"/>
+      <c r="AN12" s="76"/>
+      <c r="AO12" s="76"/>
+      <c r="AP12" s="76"/>
+      <c r="AQ12" s="76"/>
+      <c r="AR12" s="76"/>
+      <c r="AS12" s="76"/>
+      <c r="AT12" s="76"/>
+      <c r="AU12" s="76"/>
+      <c r="AV12" s="76"/>
+      <c r="AW12" s="76"/>
+      <c r="AX12" s="76"/>
+      <c r="AY12" s="76"/>
+      <c r="AZ12" s="76"/>
+      <c r="BA12" s="76"/>
+      <c r="BB12" s="76"/>
+      <c r="BC12" s="76"/>
+      <c r="BD12" s="76"/>
+      <c r="BE12" s="76"/>
+      <c r="BF12" s="76"/>
+      <c r="BG12" s="76"/>
+      <c r="BH12" s="76"/>
+      <c r="BI12" s="76"/>
+      <c r="BJ12" s="76"/>
+      <c r="BK12" s="76"/>
+      <c r="BL12" s="76"/>
+      <c r="BM12" s="76"/>
+      <c r="BN12" s="76"/>
+      <c r="BO12" s="76"/>
     </row>
     <row r="13" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="21"/>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="72" t="s">
+      <c r="H13" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="72" t="s">
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="72" t="s">
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="72" t="s">
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R13" s="73"/>
-      <c r="S13" s="73"/>
-      <c r="T13" s="72" t="s">
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U13" s="73"/>
-      <c r="V13" s="73"/>
-      <c r="W13" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X13" s="73"/>
-      <c r="Y13" s="73"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="59"/>
       <c r="AD13" s="12" t="s">
         <v>23</v>
       </c>
@@ -7198,34 +7198,34 @@
       <c r="AW13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX13" s="58" t="s">
+      <c r="AX13" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY13" s="59"/>
-      <c r="AZ13" s="60"/>
-      <c r="BA13" s="58" t="s">
+      <c r="AY13" s="70"/>
+      <c r="AZ13" s="71"/>
+      <c r="BA13" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB13" s="59"/>
-      <c r="BC13" s="60"/>
-      <c r="BD13" s="58" t="s">
+      <c r="BB13" s="70"/>
+      <c r="BC13" s="71"/>
+      <c r="BD13" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE13" s="59"/>
-      <c r="BF13" s="59"/>
-      <c r="BG13" s="59"/>
-      <c r="BH13" s="59"/>
-      <c r="BI13" s="60"/>
-      <c r="BJ13" s="58" t="s">
+      <c r="BE13" s="70"/>
+      <c r="BF13" s="70"/>
+      <c r="BG13" s="70"/>
+      <c r="BH13" s="70"/>
+      <c r="BI13" s="71"/>
+      <c r="BJ13" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK13" s="59"/>
-      <c r="BL13" s="60"/>
-      <c r="BM13" s="58" t="s">
+      <c r="BK13" s="70"/>
+      <c r="BL13" s="71"/>
+      <c r="BM13" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN13" s="59"/>
-      <c r="BO13" s="60"/>
+      <c r="BN13" s="70"/>
+      <c r="BO13" s="71"/>
     </row>
     <row r="14" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -8478,116 +8478,116 @@
       </c>
     </row>
     <row r="20" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="57"/>
-      <c r="V20" s="57"/>
-      <c r="W20" s="57"/>
-      <c r="X20" s="57"/>
-      <c r="Y20" s="57"/>
-      <c r="Z20" s="57"/>
-      <c r="AA20" s="57"/>
-      <c r="AB20" s="57"/>
-      <c r="AC20" s="57"/>
-      <c r="AD20" s="57"/>
-      <c r="AE20" s="57"/>
-      <c r="AF20" s="57"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="57"/>
-      <c r="AK20" s="57"/>
-      <c r="AL20" s="57"/>
-      <c r="AM20" s="57"/>
-      <c r="AN20" s="57"/>
-      <c r="AO20" s="57"/>
-      <c r="AP20" s="57"/>
-      <c r="AQ20" s="57"/>
-      <c r="AR20" s="57"/>
-      <c r="AS20" s="57"/>
-      <c r="AT20" s="57"/>
-      <c r="AU20" s="57"/>
-      <c r="AV20" s="57"/>
-      <c r="AW20" s="57"/>
-      <c r="AX20" s="57"/>
-      <c r="AY20" s="57"/>
-      <c r="AZ20" s="57"/>
-      <c r="BA20" s="57"/>
-      <c r="BB20" s="57"/>
-      <c r="BC20" s="57"/>
-      <c r="BD20" s="57"/>
-      <c r="BE20" s="57"/>
-      <c r="BF20" s="57"/>
-      <c r="BG20" s="57"/>
-      <c r="BH20" s="57"/>
-      <c r="BI20" s="57"/>
-      <c r="BJ20" s="57"/>
-      <c r="BK20" s="57"/>
-      <c r="BL20" s="57"/>
-      <c r="BM20" s="57"/>
-      <c r="BN20" s="57"/>
-      <c r="BO20" s="57"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
+      <c r="P20" s="76"/>
+      <c r="Q20" s="76"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
+      <c r="T20" s="76"/>
+      <c r="U20" s="76"/>
+      <c r="V20" s="76"/>
+      <c r="W20" s="76"/>
+      <c r="X20" s="76"/>
+      <c r="Y20" s="76"/>
+      <c r="Z20" s="76"/>
+      <c r="AA20" s="76"/>
+      <c r="AB20" s="76"/>
+      <c r="AC20" s="76"/>
+      <c r="AD20" s="76"/>
+      <c r="AE20" s="76"/>
+      <c r="AF20" s="76"/>
+      <c r="AG20" s="76"/>
+      <c r="AH20" s="76"/>
+      <c r="AI20" s="76"/>
+      <c r="AJ20" s="76"/>
+      <c r="AK20" s="76"/>
+      <c r="AL20" s="76"/>
+      <c r="AM20" s="76"/>
+      <c r="AN20" s="76"/>
+      <c r="AO20" s="76"/>
+      <c r="AP20" s="76"/>
+      <c r="AQ20" s="76"/>
+      <c r="AR20" s="76"/>
+      <c r="AS20" s="76"/>
+      <c r="AT20" s="76"/>
+      <c r="AU20" s="76"/>
+      <c r="AV20" s="76"/>
+      <c r="AW20" s="76"/>
+      <c r="AX20" s="76"/>
+      <c r="AY20" s="76"/>
+      <c r="AZ20" s="76"/>
+      <c r="BA20" s="76"/>
+      <c r="BB20" s="76"/>
+      <c r="BC20" s="76"/>
+      <c r="BD20" s="76"/>
+      <c r="BE20" s="76"/>
+      <c r="BF20" s="76"/>
+      <c r="BG20" s="76"/>
+      <c r="BH20" s="76"/>
+      <c r="BI20" s="76"/>
+      <c r="BJ20" s="76"/>
+      <c r="BK20" s="76"/>
+      <c r="BL20" s="76"/>
+      <c r="BM20" s="76"/>
+      <c r="BN20" s="76"/>
+      <c r="BO20" s="76"/>
     </row>
     <row r="21" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="71" t="s">
+      <c r="D21" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="72" t="s">
+      <c r="H21" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="72" t="s">
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="72" t="s">
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O21" s="73"/>
-      <c r="P21" s="73"/>
-      <c r="Q21" s="72" t="s">
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R21" s="73"/>
-      <c r="S21" s="73"/>
-      <c r="T21" s="72" t="s">
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U21" s="73"/>
-      <c r="V21" s="73"/>
-      <c r="W21" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X21" s="73"/>
-      <c r="Y21" s="73"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="59"/>
+      <c r="Y21" s="59"/>
       <c r="AD21" s="12" t="s">
         <v>23</v>
       </c>
@@ -8645,34 +8645,34 @@
       <c r="AW21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX21" s="58" t="s">
+      <c r="AX21" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY21" s="59"/>
-      <c r="AZ21" s="60"/>
-      <c r="BA21" s="58" t="s">
+      <c r="AY21" s="70"/>
+      <c r="AZ21" s="71"/>
+      <c r="BA21" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB21" s="59"/>
-      <c r="BC21" s="60"/>
-      <c r="BD21" s="58" t="s">
+      <c r="BB21" s="70"/>
+      <c r="BC21" s="71"/>
+      <c r="BD21" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE21" s="59"/>
-      <c r="BF21" s="59"/>
-      <c r="BG21" s="59"/>
-      <c r="BH21" s="59"/>
-      <c r="BI21" s="60"/>
-      <c r="BJ21" s="58" t="s">
+      <c r="BE21" s="70"/>
+      <c r="BF21" s="70"/>
+      <c r="BG21" s="70"/>
+      <c r="BH21" s="70"/>
+      <c r="BI21" s="71"/>
+      <c r="BJ21" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK21" s="59"/>
-      <c r="BL21" s="60"/>
-      <c r="BM21" s="58" t="s">
+      <c r="BK21" s="70"/>
+      <c r="BL21" s="71"/>
+      <c r="BM21" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN21" s="59"/>
-      <c r="BO21" s="60"/>
+      <c r="BN21" s="70"/>
+      <c r="BO21" s="71"/>
     </row>
     <row r="22" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
@@ -9937,116 +9937,116 @@
       </c>
     </row>
     <row r="28" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
-      <c r="V28" s="57"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="57"/>
-      <c r="Y28" s="57"/>
-      <c r="Z28" s="57"/>
-      <c r="AA28" s="57"/>
-      <c r="AB28" s="57"/>
-      <c r="AC28" s="57"/>
-      <c r="AD28" s="57"/>
-      <c r="AE28" s="57"/>
-      <c r="AF28" s="57"/>
-      <c r="AG28" s="57"/>
-      <c r="AH28" s="57"/>
-      <c r="AI28" s="57"/>
-      <c r="AJ28" s="57"/>
-      <c r="AK28" s="57"/>
-      <c r="AL28" s="57"/>
-      <c r="AM28" s="57"/>
-      <c r="AN28" s="57"/>
-      <c r="AO28" s="57"/>
-      <c r="AP28" s="57"/>
-      <c r="AQ28" s="57"/>
-      <c r="AR28" s="57"/>
-      <c r="AS28" s="57"/>
-      <c r="AT28" s="57"/>
-      <c r="AU28" s="57"/>
-      <c r="AV28" s="57"/>
-      <c r="AW28" s="57"/>
-      <c r="AX28" s="57"/>
-      <c r="AY28" s="57"/>
-      <c r="AZ28" s="57"/>
-      <c r="BA28" s="57"/>
-      <c r="BB28" s="57"/>
-      <c r="BC28" s="57"/>
-      <c r="BD28" s="57"/>
-      <c r="BE28" s="57"/>
-      <c r="BF28" s="57"/>
-      <c r="BG28" s="57"/>
-      <c r="BH28" s="57"/>
-      <c r="BI28" s="57"/>
-      <c r="BJ28" s="57"/>
-      <c r="BK28" s="57"/>
-      <c r="BL28" s="57"/>
-      <c r="BM28" s="57"/>
-      <c r="BN28" s="57"/>
-      <c r="BO28" s="57"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="76"/>
+      <c r="P28" s="76"/>
+      <c r="Q28" s="76"/>
+      <c r="R28" s="76"/>
+      <c r="S28" s="76"/>
+      <c r="T28" s="76"/>
+      <c r="U28" s="76"/>
+      <c r="V28" s="76"/>
+      <c r="W28" s="76"/>
+      <c r="X28" s="76"/>
+      <c r="Y28" s="76"/>
+      <c r="Z28" s="76"/>
+      <c r="AA28" s="76"/>
+      <c r="AB28" s="76"/>
+      <c r="AC28" s="76"/>
+      <c r="AD28" s="76"/>
+      <c r="AE28" s="76"/>
+      <c r="AF28" s="76"/>
+      <c r="AG28" s="76"/>
+      <c r="AH28" s="76"/>
+      <c r="AI28" s="76"/>
+      <c r="AJ28" s="76"/>
+      <c r="AK28" s="76"/>
+      <c r="AL28" s="76"/>
+      <c r="AM28" s="76"/>
+      <c r="AN28" s="76"/>
+      <c r="AO28" s="76"/>
+      <c r="AP28" s="76"/>
+      <c r="AQ28" s="76"/>
+      <c r="AR28" s="76"/>
+      <c r="AS28" s="76"/>
+      <c r="AT28" s="76"/>
+      <c r="AU28" s="76"/>
+      <c r="AV28" s="76"/>
+      <c r="AW28" s="76"/>
+      <c r="AX28" s="76"/>
+      <c r="AY28" s="76"/>
+      <c r="AZ28" s="76"/>
+      <c r="BA28" s="76"/>
+      <c r="BB28" s="76"/>
+      <c r="BC28" s="76"/>
+      <c r="BD28" s="76"/>
+      <c r="BE28" s="76"/>
+      <c r="BF28" s="76"/>
+      <c r="BG28" s="76"/>
+      <c r="BH28" s="76"/>
+      <c r="BI28" s="76"/>
+      <c r="BJ28" s="76"/>
+      <c r="BK28" s="76"/>
+      <c r="BL28" s="76"/>
+      <c r="BM28" s="76"/>
+      <c r="BN28" s="76"/>
+      <c r="BO28" s="76"/>
     </row>
     <row r="29" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="21"/>
-      <c r="D29" s="71" t="s">
+      <c r="D29" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="72" t="s">
+      <c r="H29" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="72" t="s">
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="72" t="s">
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="72" t="s">
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="73"/>
-      <c r="S29" s="73"/>
-      <c r="T29" s="72" t="s">
+      <c r="R29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U29" s="73"/>
-      <c r="V29" s="73"/>
-      <c r="W29" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="73"/>
-      <c r="Y29" s="73"/>
+      <c r="U29" s="59"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="59"/>
+      <c r="Y29" s="59"/>
       <c r="AD29" s="12" t="s">
         <v>23</v>
       </c>
@@ -10104,34 +10104,34 @@
       <c r="AW29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX29" s="58" t="s">
+      <c r="AX29" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY29" s="59"/>
-      <c r="AZ29" s="60"/>
-      <c r="BA29" s="58" t="s">
+      <c r="AY29" s="70"/>
+      <c r="AZ29" s="71"/>
+      <c r="BA29" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB29" s="59"/>
-      <c r="BC29" s="60"/>
-      <c r="BD29" s="58" t="s">
+      <c r="BB29" s="70"/>
+      <c r="BC29" s="71"/>
+      <c r="BD29" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE29" s="59"/>
-      <c r="BF29" s="59"/>
-      <c r="BG29" s="59"/>
-      <c r="BH29" s="59"/>
-      <c r="BI29" s="60"/>
-      <c r="BJ29" s="58" t="s">
+      <c r="BE29" s="70"/>
+      <c r="BF29" s="70"/>
+      <c r="BG29" s="70"/>
+      <c r="BH29" s="70"/>
+      <c r="BI29" s="71"/>
+      <c r="BJ29" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK29" s="59"/>
-      <c r="BL29" s="60"/>
-      <c r="BM29" s="58" t="s">
+      <c r="BK29" s="70"/>
+      <c r="BL29" s="71"/>
+      <c r="BM29" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN29" s="59"/>
-      <c r="BO29" s="60"/>
+      <c r="BN29" s="70"/>
+      <c r="BO29" s="71"/>
     </row>
     <row r="30" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
@@ -11396,120 +11396,120 @@
       </c>
     </row>
     <row r="36" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
-      <c r="S36" s="57"/>
-      <c r="T36" s="57"/>
-      <c r="U36" s="57"/>
-      <c r="V36" s="57"/>
-      <c r="W36" s="57"/>
-      <c r="X36" s="57"/>
-      <c r="Y36" s="57"/>
-      <c r="Z36" s="57"/>
-      <c r="AA36" s="57"/>
-      <c r="AB36" s="57"/>
-      <c r="AC36" s="57"/>
-      <c r="AD36" s="57"/>
-      <c r="AE36" s="57"/>
-      <c r="AF36" s="57"/>
-      <c r="AG36" s="57"/>
-      <c r="AH36" s="57"/>
-      <c r="AI36" s="57"/>
-      <c r="AJ36" s="57"/>
-      <c r="AK36" s="57"/>
-      <c r="AL36" s="57"/>
-      <c r="AM36" s="57"/>
-      <c r="AN36" s="57"/>
-      <c r="AO36" s="57"/>
-      <c r="AP36" s="57"/>
-      <c r="AQ36" s="57"/>
-      <c r="AR36" s="57"/>
-      <c r="AS36" s="57"/>
-      <c r="AT36" s="57"/>
-      <c r="AU36" s="57"/>
-      <c r="AV36" s="57"/>
-      <c r="AW36" s="57"/>
-      <c r="AX36" s="57"/>
-      <c r="AY36" s="57"/>
-      <c r="AZ36" s="57"/>
-      <c r="BA36" s="57"/>
-      <c r="BB36" s="57"/>
-      <c r="BC36" s="57"/>
-      <c r="BD36" s="57"/>
-      <c r="BE36" s="57"/>
-      <c r="BF36" s="57"/>
-      <c r="BG36" s="57"/>
-      <c r="BH36" s="57"/>
-      <c r="BI36" s="57"/>
-      <c r="BJ36" s="57"/>
-      <c r="BK36" s="57"/>
-      <c r="BL36" s="57"/>
-      <c r="BM36" s="57"/>
-      <c r="BN36" s="57"/>
-      <c r="BO36" s="57"/>
-      <c r="BQ36" s="64" t="s">
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="76"/>
+      <c r="O36" s="76"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="76"/>
+      <c r="R36" s="76"/>
+      <c r="S36" s="76"/>
+      <c r="T36" s="76"/>
+      <c r="U36" s="76"/>
+      <c r="V36" s="76"/>
+      <c r="W36" s="76"/>
+      <c r="X36" s="76"/>
+      <c r="Y36" s="76"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="76"/>
+      <c r="AB36" s="76"/>
+      <c r="AC36" s="76"/>
+      <c r="AD36" s="76"/>
+      <c r="AE36" s="76"/>
+      <c r="AF36" s="76"/>
+      <c r="AG36" s="76"/>
+      <c r="AH36" s="76"/>
+      <c r="AI36" s="76"/>
+      <c r="AJ36" s="76"/>
+      <c r="AK36" s="76"/>
+      <c r="AL36" s="76"/>
+      <c r="AM36" s="76"/>
+      <c r="AN36" s="76"/>
+      <c r="AO36" s="76"/>
+      <c r="AP36" s="76"/>
+      <c r="AQ36" s="76"/>
+      <c r="AR36" s="76"/>
+      <c r="AS36" s="76"/>
+      <c r="AT36" s="76"/>
+      <c r="AU36" s="76"/>
+      <c r="AV36" s="76"/>
+      <c r="AW36" s="76"/>
+      <c r="AX36" s="76"/>
+      <c r="AY36" s="76"/>
+      <c r="AZ36" s="76"/>
+      <c r="BA36" s="76"/>
+      <c r="BB36" s="76"/>
+      <c r="BC36" s="76"/>
+      <c r="BD36" s="76"/>
+      <c r="BE36" s="76"/>
+      <c r="BF36" s="76"/>
+      <c r="BG36" s="76"/>
+      <c r="BH36" s="76"/>
+      <c r="BI36" s="76"/>
+      <c r="BJ36" s="76"/>
+      <c r="BK36" s="76"/>
+      <c r="BL36" s="76"/>
+      <c r="BM36" s="76"/>
+      <c r="BN36" s="76"/>
+      <c r="BO36" s="76"/>
+      <c r="BQ36" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="BR36" s="64"/>
+      <c r="BR36" s="62"/>
     </row>
     <row r="37" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="21"/>
-      <c r="D37" s="71" t="s">
+      <c r="D37" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="72" t="s">
+      <c r="H37" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="73"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="72" t="s">
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L37" s="73"/>
-      <c r="M37" s="73"/>
-      <c r="N37" s="72" t="s">
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O37" s="73"/>
-      <c r="P37" s="73"/>
-      <c r="Q37" s="72" t="s">
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R37" s="73"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="72" t="s">
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X37" s="73"/>
-      <c r="Y37" s="73"/>
+      <c r="U37" s="59"/>
+      <c r="V37" s="59"/>
+      <c r="W37" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
       <c r="AD37" s="12" t="s">
         <v>23</v>
       </c>
@@ -11567,38 +11567,38 @@
       <c r="AW37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX37" s="58" t="s">
+      <c r="AX37" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY37" s="59"/>
-      <c r="AZ37" s="60"/>
-      <c r="BA37" s="58" t="s">
+      <c r="AY37" s="70"/>
+      <c r="AZ37" s="71"/>
+      <c r="BA37" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB37" s="59"/>
-      <c r="BC37" s="60"/>
-      <c r="BD37" s="58" t="s">
+      <c r="BB37" s="70"/>
+      <c r="BC37" s="71"/>
+      <c r="BD37" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE37" s="59"/>
-      <c r="BF37" s="59"/>
-      <c r="BG37" s="59"/>
-      <c r="BH37" s="59"/>
-      <c r="BI37" s="60"/>
-      <c r="BJ37" s="58" t="s">
+      <c r="BE37" s="70"/>
+      <c r="BF37" s="70"/>
+      <c r="BG37" s="70"/>
+      <c r="BH37" s="70"/>
+      <c r="BI37" s="71"/>
+      <c r="BJ37" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK37" s="59"/>
-      <c r="BL37" s="60"/>
-      <c r="BM37" s="58" t="s">
+      <c r="BK37" s="70"/>
+      <c r="BL37" s="71"/>
+      <c r="BM37" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN37" s="59"/>
-      <c r="BO37" s="60"/>
-      <c r="BQ37" s="65" t="s">
+      <c r="BN37" s="70"/>
+      <c r="BO37" s="71"/>
+      <c r="BQ37" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="BR37" s="66"/>
+      <c r="BR37" s="64"/>
     </row>
     <row r="38" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B38" s="23">
@@ -11809,10 +11809,10 @@
       <c r="BO38" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="BQ38" s="67" t="s">
+      <c r="BQ38" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="BR38" s="68"/>
+      <c r="BR38" s="66"/>
     </row>
     <row r="39" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B39" s="23">
@@ -12036,10 +12036,10 @@
         <f>VLOOKUP($AX39,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>1297.1428571428571</v>
       </c>
-      <c r="BQ39" s="67" t="s">
+      <c r="BQ39" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="BR39" s="68"/>
+      <c r="BR39" s="66"/>
     </row>
     <row r="40" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B40" s="23">
@@ -12271,10 +12271,10 @@
         <f>VLOOKUP($AX40,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>1026.5151515151515</v>
       </c>
-      <c r="BQ40" s="67" t="s">
+      <c r="BQ40" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="BR40" s="68"/>
+      <c r="BR40" s="66"/>
     </row>
     <row r="41" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B41" s="23">
@@ -12498,10 +12498,10 @@
         <f>VLOOKUP($AX41,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>973.88059701492534</v>
       </c>
-      <c r="BQ41" s="69" t="s">
+      <c r="BQ41" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="BR41" s="70"/>
+      <c r="BR41" s="68"/>
     </row>
     <row r="42" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B42" s="23">
@@ -12875,116 +12875,116 @@
       </c>
     </row>
     <row r="44" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="57"/>
-      <c r="U44" s="57"/>
-      <c r="V44" s="57"/>
-      <c r="W44" s="57"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="57"/>
-      <c r="Z44" s="57"/>
-      <c r="AA44" s="57"/>
-      <c r="AB44" s="57"/>
-      <c r="AC44" s="57"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="57"/>
-      <c r="AF44" s="57"/>
-      <c r="AG44" s="57"/>
-      <c r="AH44" s="57"/>
-      <c r="AI44" s="57"/>
-      <c r="AJ44" s="57"/>
-      <c r="AK44" s="57"/>
-      <c r="AL44" s="57"/>
-      <c r="AM44" s="57"/>
-      <c r="AN44" s="57"/>
-      <c r="AO44" s="57"/>
-      <c r="AP44" s="57"/>
-      <c r="AQ44" s="57"/>
-      <c r="AR44" s="57"/>
-      <c r="AS44" s="57"/>
-      <c r="AT44" s="57"/>
-      <c r="AU44" s="57"/>
-      <c r="AV44" s="57"/>
-      <c r="AW44" s="57"/>
-      <c r="AX44" s="57"/>
-      <c r="AY44" s="57"/>
-      <c r="AZ44" s="57"/>
-      <c r="BA44" s="57"/>
-      <c r="BB44" s="57"/>
-      <c r="BC44" s="57"/>
-      <c r="BD44" s="57"/>
-      <c r="BE44" s="57"/>
-      <c r="BF44" s="57"/>
-      <c r="BG44" s="57"/>
-      <c r="BH44" s="57"/>
-      <c r="BI44" s="57"/>
-      <c r="BJ44" s="57"/>
-      <c r="BK44" s="57"/>
-      <c r="BL44" s="57"/>
-      <c r="BM44" s="57"/>
-      <c r="BN44" s="57"/>
-      <c r="BO44" s="57"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="76"/>
+      <c r="P44" s="76"/>
+      <c r="Q44" s="76"/>
+      <c r="R44" s="76"/>
+      <c r="S44" s="76"/>
+      <c r="T44" s="76"/>
+      <c r="U44" s="76"/>
+      <c r="V44" s="76"/>
+      <c r="W44" s="76"/>
+      <c r="X44" s="76"/>
+      <c r="Y44" s="76"/>
+      <c r="Z44" s="76"/>
+      <c r="AA44" s="76"/>
+      <c r="AB44" s="76"/>
+      <c r="AC44" s="76"/>
+      <c r="AD44" s="76"/>
+      <c r="AE44" s="76"/>
+      <c r="AF44" s="76"/>
+      <c r="AG44" s="76"/>
+      <c r="AH44" s="76"/>
+      <c r="AI44" s="76"/>
+      <c r="AJ44" s="76"/>
+      <c r="AK44" s="76"/>
+      <c r="AL44" s="76"/>
+      <c r="AM44" s="76"/>
+      <c r="AN44" s="76"/>
+      <c r="AO44" s="76"/>
+      <c r="AP44" s="76"/>
+      <c r="AQ44" s="76"/>
+      <c r="AR44" s="76"/>
+      <c r="AS44" s="76"/>
+      <c r="AT44" s="76"/>
+      <c r="AU44" s="76"/>
+      <c r="AV44" s="76"/>
+      <c r="AW44" s="76"/>
+      <c r="AX44" s="76"/>
+      <c r="AY44" s="76"/>
+      <c r="AZ44" s="76"/>
+      <c r="BA44" s="76"/>
+      <c r="BB44" s="76"/>
+      <c r="BC44" s="76"/>
+      <c r="BD44" s="76"/>
+      <c r="BE44" s="76"/>
+      <c r="BF44" s="76"/>
+      <c r="BG44" s="76"/>
+      <c r="BH44" s="76"/>
+      <c r="BI44" s="76"/>
+      <c r="BJ44" s="76"/>
+      <c r="BK44" s="76"/>
+      <c r="BL44" s="76"/>
+      <c r="BM44" s="76"/>
+      <c r="BN44" s="76"/>
+      <c r="BO44" s="76"/>
     </row>
     <row r="45" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B45" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C45" s="21"/>
-      <c r="D45" s="71" t="s">
+      <c r="D45" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="71"/>
-      <c r="F45" s="71"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
       <c r="G45" s="22"/>
-      <c r="H45" s="72" t="s">
+      <c r="H45" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="72" t="s">
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L45" s="73"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="72" t="s">
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O45" s="73"/>
-      <c r="P45" s="73"/>
-      <c r="Q45" s="72" t="s">
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73"/>
-      <c r="T45" s="72" t="s">
+      <c r="R45" s="59"/>
+      <c r="S45" s="59"/>
+      <c r="T45" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U45" s="73"/>
-      <c r="V45" s="73"/>
-      <c r="W45" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X45" s="73"/>
-      <c r="Y45" s="73"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="59"/>
+      <c r="W45" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
       <c r="AD45" s="12" t="s">
         <v>23</v>
       </c>
@@ -13042,34 +13042,34 @@
       <c r="AW45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX45" s="58" t="s">
+      <c r="AX45" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY45" s="59"/>
-      <c r="AZ45" s="60"/>
-      <c r="BA45" s="58" t="s">
+      <c r="AY45" s="70"/>
+      <c r="AZ45" s="71"/>
+      <c r="BA45" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB45" s="59"/>
-      <c r="BC45" s="60"/>
-      <c r="BD45" s="58" t="s">
+      <c r="BB45" s="70"/>
+      <c r="BC45" s="71"/>
+      <c r="BD45" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE45" s="59"/>
-      <c r="BF45" s="59"/>
-      <c r="BG45" s="59"/>
-      <c r="BH45" s="59"/>
-      <c r="BI45" s="60"/>
-      <c r="BJ45" s="58" t="s">
+      <c r="BE45" s="70"/>
+      <c r="BF45" s="70"/>
+      <c r="BG45" s="70"/>
+      <c r="BH45" s="70"/>
+      <c r="BI45" s="71"/>
+      <c r="BJ45" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK45" s="59"/>
-      <c r="BL45" s="60"/>
-      <c r="BM45" s="58" t="s">
+      <c r="BK45" s="70"/>
+      <c r="BL45" s="71"/>
+      <c r="BM45" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN45" s="59"/>
-      <c r="BO45" s="60"/>
+      <c r="BN45" s="70"/>
+      <c r="BO45" s="71"/>
     </row>
     <row r="46" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
@@ -14330,116 +14330,116 @@
       </c>
     </row>
     <row r="52" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="57"/>
-      <c r="Q52" s="57"/>
-      <c r="R52" s="57"/>
-      <c r="S52" s="57"/>
-      <c r="T52" s="57"/>
-      <c r="U52" s="57"/>
-      <c r="V52" s="57"/>
-      <c r="W52" s="57"/>
-      <c r="X52" s="57"/>
-      <c r="Y52" s="57"/>
-      <c r="Z52" s="57"/>
-      <c r="AA52" s="57"/>
-      <c r="AB52" s="57"/>
-      <c r="AC52" s="57"/>
-      <c r="AD52" s="57"/>
-      <c r="AE52" s="57"/>
-      <c r="AF52" s="57"/>
-      <c r="AG52" s="57"/>
-      <c r="AH52" s="57"/>
-      <c r="AI52" s="57"/>
-      <c r="AJ52" s="57"/>
-      <c r="AK52" s="57"/>
-      <c r="AL52" s="57"/>
-      <c r="AM52" s="57"/>
-      <c r="AN52" s="57"/>
-      <c r="AO52" s="57"/>
-      <c r="AP52" s="57"/>
-      <c r="AQ52" s="57"/>
-      <c r="AR52" s="57"/>
-      <c r="AS52" s="57"/>
-      <c r="AT52" s="57"/>
-      <c r="AU52" s="57"/>
-      <c r="AV52" s="57"/>
-      <c r="AW52" s="57"/>
-      <c r="AX52" s="57"/>
-      <c r="AY52" s="57"/>
-      <c r="AZ52" s="57"/>
-      <c r="BA52" s="57"/>
-      <c r="BB52" s="57"/>
-      <c r="BC52" s="57"/>
-      <c r="BD52" s="57"/>
-      <c r="BE52" s="57"/>
-      <c r="BF52" s="57"/>
-      <c r="BG52" s="57"/>
-      <c r="BH52" s="57"/>
-      <c r="BI52" s="57"/>
-      <c r="BJ52" s="57"/>
-      <c r="BK52" s="57"/>
-      <c r="BL52" s="57"/>
-      <c r="BM52" s="57"/>
-      <c r="BN52" s="57"/>
-      <c r="BO52" s="57"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="76"/>
+      <c r="M52" s="76"/>
+      <c r="N52" s="76"/>
+      <c r="O52" s="76"/>
+      <c r="P52" s="76"/>
+      <c r="Q52" s="76"/>
+      <c r="R52" s="76"/>
+      <c r="S52" s="76"/>
+      <c r="T52" s="76"/>
+      <c r="U52" s="76"/>
+      <c r="V52" s="76"/>
+      <c r="W52" s="76"/>
+      <c r="X52" s="76"/>
+      <c r="Y52" s="76"/>
+      <c r="Z52" s="76"/>
+      <c r="AA52" s="76"/>
+      <c r="AB52" s="76"/>
+      <c r="AC52" s="76"/>
+      <c r="AD52" s="76"/>
+      <c r="AE52" s="76"/>
+      <c r="AF52" s="76"/>
+      <c r="AG52" s="76"/>
+      <c r="AH52" s="76"/>
+      <c r="AI52" s="76"/>
+      <c r="AJ52" s="76"/>
+      <c r="AK52" s="76"/>
+      <c r="AL52" s="76"/>
+      <c r="AM52" s="76"/>
+      <c r="AN52" s="76"/>
+      <c r="AO52" s="76"/>
+      <c r="AP52" s="76"/>
+      <c r="AQ52" s="76"/>
+      <c r="AR52" s="76"/>
+      <c r="AS52" s="76"/>
+      <c r="AT52" s="76"/>
+      <c r="AU52" s="76"/>
+      <c r="AV52" s="76"/>
+      <c r="AW52" s="76"/>
+      <c r="AX52" s="76"/>
+      <c r="AY52" s="76"/>
+      <c r="AZ52" s="76"/>
+      <c r="BA52" s="76"/>
+      <c r="BB52" s="76"/>
+      <c r="BC52" s="76"/>
+      <c r="BD52" s="76"/>
+      <c r="BE52" s="76"/>
+      <c r="BF52" s="76"/>
+      <c r="BG52" s="76"/>
+      <c r="BH52" s="76"/>
+      <c r="BI52" s="76"/>
+      <c r="BJ52" s="76"/>
+      <c r="BK52" s="76"/>
+      <c r="BL52" s="76"/>
+      <c r="BM52" s="76"/>
+      <c r="BN52" s="76"/>
+      <c r="BO52" s="76"/>
     </row>
     <row r="53" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B53" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="71" t="s">
+      <c r="D53" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E53" s="71"/>
-      <c r="F53" s="71"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
       <c r="G53" s="22"/>
-      <c r="H53" s="72" t="s">
+      <c r="H53" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I53" s="73"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="72" t="s">
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L53" s="73"/>
-      <c r="M53" s="73"/>
-      <c r="N53" s="72" t="s">
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O53" s="73"/>
-      <c r="P53" s="73"/>
-      <c r="Q53" s="72" t="s">
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R53" s="73"/>
-      <c r="S53" s="73"/>
-      <c r="T53" s="72" t="s">
+      <c r="R53" s="59"/>
+      <c r="S53" s="59"/>
+      <c r="T53" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U53" s="73"/>
-      <c r="V53" s="73"/>
-      <c r="W53" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X53" s="73"/>
-      <c r="Y53" s="73"/>
+      <c r="U53" s="59"/>
+      <c r="V53" s="59"/>
+      <c r="W53" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X53" s="59"/>
+      <c r="Y53" s="59"/>
       <c r="AD53" s="12" t="s">
         <v>23</v>
       </c>
@@ -14497,34 +14497,34 @@
       <c r="AW53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX53" s="58" t="s">
+      <c r="AX53" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY53" s="59"/>
-      <c r="AZ53" s="60"/>
-      <c r="BA53" s="58" t="s">
+      <c r="AY53" s="70"/>
+      <c r="AZ53" s="71"/>
+      <c r="BA53" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB53" s="59"/>
-      <c r="BC53" s="60"/>
-      <c r="BD53" s="58" t="s">
+      <c r="BB53" s="70"/>
+      <c r="BC53" s="71"/>
+      <c r="BD53" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE53" s="59"/>
-      <c r="BF53" s="59"/>
-      <c r="BG53" s="59"/>
-      <c r="BH53" s="59"/>
-      <c r="BI53" s="60"/>
-      <c r="BJ53" s="58" t="s">
+      <c r="BE53" s="70"/>
+      <c r="BF53" s="70"/>
+      <c r="BG53" s="70"/>
+      <c r="BH53" s="70"/>
+      <c r="BI53" s="71"/>
+      <c r="BJ53" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK53" s="59"/>
-      <c r="BL53" s="60"/>
-      <c r="BM53" s="58" t="s">
+      <c r="BK53" s="70"/>
+      <c r="BL53" s="71"/>
+      <c r="BM53" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN53" s="59"/>
-      <c r="BO53" s="60"/>
+      <c r="BN53" s="70"/>
+      <c r="BO53" s="71"/>
     </row>
     <row r="54" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B54" s="23">
@@ -15785,116 +15785,116 @@
       </c>
     </row>
     <row r="60" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="57" t="s">
+      <c r="B60" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="57"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="57"/>
-      <c r="R60" s="57"/>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
-      <c r="U60" s="57"/>
-      <c r="V60" s="57"/>
-      <c r="W60" s="57"/>
-      <c r="X60" s="57"/>
-      <c r="Y60" s="57"/>
-      <c r="Z60" s="57"/>
-      <c r="AA60" s="57"/>
-      <c r="AB60" s="57"/>
-      <c r="AC60" s="57"/>
-      <c r="AD60" s="57"/>
-      <c r="AE60" s="57"/>
-      <c r="AF60" s="57"/>
-      <c r="AG60" s="57"/>
-      <c r="AH60" s="57"/>
-      <c r="AI60" s="57"/>
-      <c r="AJ60" s="57"/>
-      <c r="AK60" s="57"/>
-      <c r="AL60" s="57"/>
-      <c r="AM60" s="57"/>
-      <c r="AN60" s="57"/>
-      <c r="AO60" s="57"/>
-      <c r="AP60" s="57"/>
-      <c r="AQ60" s="57"/>
-      <c r="AR60" s="57"/>
-      <c r="AS60" s="57"/>
-      <c r="AT60" s="57"/>
-      <c r="AU60" s="57"/>
-      <c r="AV60" s="57"/>
-      <c r="AW60" s="57"/>
-      <c r="AX60" s="57"/>
-      <c r="AY60" s="57"/>
-      <c r="AZ60" s="57"/>
-      <c r="BA60" s="57"/>
-      <c r="BB60" s="57"/>
-      <c r="BC60" s="57"/>
-      <c r="BD60" s="57"/>
-      <c r="BE60" s="57"/>
-      <c r="BF60" s="57"/>
-      <c r="BG60" s="57"/>
-      <c r="BH60" s="57"/>
-      <c r="BI60" s="57"/>
-      <c r="BJ60" s="57"/>
-      <c r="BK60" s="57"/>
-      <c r="BL60" s="57"/>
-      <c r="BM60" s="57"/>
-      <c r="BN60" s="57"/>
-      <c r="BO60" s="57"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="76"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="76"/>
+      <c r="O60" s="76"/>
+      <c r="P60" s="76"/>
+      <c r="Q60" s="76"/>
+      <c r="R60" s="76"/>
+      <c r="S60" s="76"/>
+      <c r="T60" s="76"/>
+      <c r="U60" s="76"/>
+      <c r="V60" s="76"/>
+      <c r="W60" s="76"/>
+      <c r="X60" s="76"/>
+      <c r="Y60" s="76"/>
+      <c r="Z60" s="76"/>
+      <c r="AA60" s="76"/>
+      <c r="AB60" s="76"/>
+      <c r="AC60" s="76"/>
+      <c r="AD60" s="76"/>
+      <c r="AE60" s="76"/>
+      <c r="AF60" s="76"/>
+      <c r="AG60" s="76"/>
+      <c r="AH60" s="76"/>
+      <c r="AI60" s="76"/>
+      <c r="AJ60" s="76"/>
+      <c r="AK60" s="76"/>
+      <c r="AL60" s="76"/>
+      <c r="AM60" s="76"/>
+      <c r="AN60" s="76"/>
+      <c r="AO60" s="76"/>
+      <c r="AP60" s="76"/>
+      <c r="AQ60" s="76"/>
+      <c r="AR60" s="76"/>
+      <c r="AS60" s="76"/>
+      <c r="AT60" s="76"/>
+      <c r="AU60" s="76"/>
+      <c r="AV60" s="76"/>
+      <c r="AW60" s="76"/>
+      <c r="AX60" s="76"/>
+      <c r="AY60" s="76"/>
+      <c r="AZ60" s="76"/>
+      <c r="BA60" s="76"/>
+      <c r="BB60" s="76"/>
+      <c r="BC60" s="76"/>
+      <c r="BD60" s="76"/>
+      <c r="BE60" s="76"/>
+      <c r="BF60" s="76"/>
+      <c r="BG60" s="76"/>
+      <c r="BH60" s="76"/>
+      <c r="BI60" s="76"/>
+      <c r="BJ60" s="76"/>
+      <c r="BK60" s="76"/>
+      <c r="BL60" s="76"/>
+      <c r="BM60" s="76"/>
+      <c r="BN60" s="76"/>
+      <c r="BO60" s="76"/>
     </row>
     <row r="61" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B61" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="21"/>
-      <c r="D61" s="71" t="s">
+      <c r="D61" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E61" s="71"/>
-      <c r="F61" s="71"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="72" t="s">
+      <c r="H61" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I61" s="73"/>
-      <c r="J61" s="73"/>
-      <c r="K61" s="72" t="s">
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L61" s="73"/>
-      <c r="M61" s="73"/>
-      <c r="N61" s="72" t="s">
+      <c r="L61" s="59"/>
+      <c r="M61" s="59"/>
+      <c r="N61" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O61" s="73"/>
-      <c r="P61" s="73"/>
-      <c r="Q61" s="72" t="s">
+      <c r="O61" s="59"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R61" s="73"/>
-      <c r="S61" s="73"/>
-      <c r="T61" s="72" t="s">
+      <c r="R61" s="59"/>
+      <c r="S61" s="59"/>
+      <c r="T61" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U61" s="73"/>
-      <c r="V61" s="73"/>
-      <c r="W61" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X61" s="73"/>
-      <c r="Y61" s="73"/>
+      <c r="U61" s="59"/>
+      <c r="V61" s="59"/>
+      <c r="W61" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X61" s="59"/>
+      <c r="Y61" s="59"/>
       <c r="AD61" s="12" t="s">
         <v>23</v>
       </c>
@@ -15952,34 +15952,34 @@
       <c r="AW61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX61" s="58" t="s">
+      <c r="AX61" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY61" s="59"/>
-      <c r="AZ61" s="60"/>
-      <c r="BA61" s="58" t="s">
+      <c r="AY61" s="70"/>
+      <c r="AZ61" s="71"/>
+      <c r="BA61" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB61" s="59"/>
-      <c r="BC61" s="60"/>
-      <c r="BD61" s="58" t="s">
+      <c r="BB61" s="70"/>
+      <c r="BC61" s="71"/>
+      <c r="BD61" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE61" s="59"/>
-      <c r="BF61" s="59"/>
-      <c r="BG61" s="59"/>
-      <c r="BH61" s="59"/>
-      <c r="BI61" s="60"/>
-      <c r="BJ61" s="58" t="s">
+      <c r="BE61" s="70"/>
+      <c r="BF61" s="70"/>
+      <c r="BG61" s="70"/>
+      <c r="BH61" s="70"/>
+      <c r="BI61" s="71"/>
+      <c r="BJ61" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK61" s="59"/>
-      <c r="BL61" s="60"/>
-      <c r="BM61" s="58" t="s">
+      <c r="BK61" s="70"/>
+      <c r="BL61" s="71"/>
+      <c r="BM61" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN61" s="59"/>
-      <c r="BO61" s="60"/>
+      <c r="BN61" s="70"/>
+      <c r="BO61" s="71"/>
     </row>
     <row r="62" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B62" s="11">
@@ -17238,93 +17238,6 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="111">
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:Y21"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="Q37:S37"/>
-    <mergeCell ref="T37:V37"/>
-    <mergeCell ref="W37:Y37"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="T61:V61"/>
-    <mergeCell ref="W61:Y61"/>
-    <mergeCell ref="W45:Y45"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="T53:V53"/>
-    <mergeCell ref="W53:Y53"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="T45:V45"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BQ37:BR37"/>
-    <mergeCell ref="BQ38:BR38"/>
-    <mergeCell ref="BQ39:BR39"/>
-    <mergeCell ref="BQ40:BR40"/>
-    <mergeCell ref="BQ41:BR41"/>
-    <mergeCell ref="AX29:AZ29"/>
-    <mergeCell ref="BA29:BC29"/>
-    <mergeCell ref="BD29:BI29"/>
-    <mergeCell ref="BJ29:BL29"/>
-    <mergeCell ref="BM29:BO29"/>
-    <mergeCell ref="AX37:AZ37"/>
-    <mergeCell ref="BA37:BC37"/>
-    <mergeCell ref="BD37:BI37"/>
-    <mergeCell ref="BJ37:BL37"/>
-    <mergeCell ref="BM37:BO37"/>
-    <mergeCell ref="BJ21:BL21"/>
-    <mergeCell ref="BM21:BO21"/>
-    <mergeCell ref="AX61:AZ61"/>
-    <mergeCell ref="BA61:BC61"/>
-    <mergeCell ref="BD61:BI61"/>
-    <mergeCell ref="BJ61:BL61"/>
-    <mergeCell ref="BM61:BO61"/>
-    <mergeCell ref="AX45:AZ45"/>
-    <mergeCell ref="BA5:BC5"/>
-    <mergeCell ref="BD5:BI5"/>
-    <mergeCell ref="BJ5:BL5"/>
-    <mergeCell ref="BM5:BO5"/>
-    <mergeCell ref="AX5:AZ5"/>
-    <mergeCell ref="BA13:BC13"/>
-    <mergeCell ref="BD13:BI13"/>
     <mergeCell ref="B2:BO2"/>
     <mergeCell ref="B4:BO4"/>
     <mergeCell ref="B12:BO12"/>
@@ -17349,6 +17262,93 @@
     <mergeCell ref="AX21:AZ21"/>
     <mergeCell ref="BA21:BC21"/>
     <mergeCell ref="BD21:BI21"/>
+    <mergeCell ref="BJ21:BL21"/>
+    <mergeCell ref="BM21:BO21"/>
+    <mergeCell ref="AX61:AZ61"/>
+    <mergeCell ref="BA61:BC61"/>
+    <mergeCell ref="BD61:BI61"/>
+    <mergeCell ref="BJ61:BL61"/>
+    <mergeCell ref="BM61:BO61"/>
+    <mergeCell ref="AX45:AZ45"/>
+    <mergeCell ref="BA5:BC5"/>
+    <mergeCell ref="BD5:BI5"/>
+    <mergeCell ref="BJ5:BL5"/>
+    <mergeCell ref="BM5:BO5"/>
+    <mergeCell ref="AX5:AZ5"/>
+    <mergeCell ref="BA13:BC13"/>
+    <mergeCell ref="BD13:BI13"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BQ37:BR37"/>
+    <mergeCell ref="BQ38:BR38"/>
+    <mergeCell ref="BQ39:BR39"/>
+    <mergeCell ref="BQ40:BR40"/>
+    <mergeCell ref="BQ41:BR41"/>
+    <mergeCell ref="AX29:AZ29"/>
+    <mergeCell ref="BA29:BC29"/>
+    <mergeCell ref="BD29:BI29"/>
+    <mergeCell ref="BJ29:BL29"/>
+    <mergeCell ref="BM29:BO29"/>
+    <mergeCell ref="AX37:AZ37"/>
+    <mergeCell ref="BA37:BC37"/>
+    <mergeCell ref="BD37:BI37"/>
+    <mergeCell ref="BJ37:BL37"/>
+    <mergeCell ref="BM37:BO37"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="T61:V61"/>
+    <mergeCell ref="W61:Y61"/>
+    <mergeCell ref="W45:Y45"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="T53:V53"/>
+    <mergeCell ref="W53:Y53"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="T45:V45"/>
+    <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="T37:V37"/>
+    <mergeCell ref="W37:Y37"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T13:V13"/>
   </mergeCells>
   <conditionalFormatting sqref="T6:V11 T22:V27 T54:V59">
     <cfRule type="expression" dxfId="95" priority="472">
@@ -17687,7 +17687,7 @@
   <dimension ref="B1:BO48"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17756,55 +17756,55 @@
       <c r="Y1" s="18"/>
     </row>
     <row r="2" spans="2:67" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="56"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="75"/>
       <c r="AW2" s="46"/>
       <c r="AX2" s="46"/>
       <c r="AY2" s="46"/>
@@ -17858,42 +17858,42 @@
         <v>86</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75" t="s">
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="75" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="75" t="s">
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
       <c r="AA5" s="12" t="s">
         <v>23</v>
       </c>
@@ -17960,70 +17960,94 @@
         <f>IF(Preliminary!BA7&lt;3,"Winner of Pool A",Preliminary!AY7)</f>
         <v> Netherlands</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="48">
+        <v>3</v>
+      </c>
       <c r="E6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="47"/>
+      <c r="F6" s="47">
+        <v>2</v>
+      </c>
       <c r="G6" s="25" t="str">
         <f>IF(Preliminary!BA64&lt;3,"Runners-up of Pool H",Preliminary!AY64)</f>
         <v> Serbia</v>
       </c>
-      <c r="H6" s="28"/>
+      <c r="H6" s="28">
+        <v>27</v>
+      </c>
       <c r="I6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="28"/>
+      <c r="J6" s="30">
+        <v>25</v>
+      </c>
+      <c r="K6" s="28">
+        <v>26</v>
+      </c>
       <c r="L6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="28"/>
+      <c r="M6" s="30">
+        <v>24</v>
+      </c>
+      <c r="N6" s="28">
+        <v>22</v>
+      </c>
       <c r="O6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="28"/>
+      <c r="P6" s="30">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>20</v>
+      </c>
       <c r="R6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S6" s="30"/>
-      <c r="T6" s="28"/>
+      <c r="S6" s="30">
+        <v>25</v>
+      </c>
+      <c r="T6" s="28">
+        <v>15</v>
+      </c>
       <c r="U6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="V6" s="30"/>
+      <c r="V6" s="30">
+        <v>11</v>
+      </c>
       <c r="W6" s="31">
         <f t="shared" ref="W6:W13" si="0">SUM(H6,K6,N6,Q6,T6)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="X6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y6" s="32">
         <f t="shared" ref="Y6:Y13" si="1">SUM(J6,M6,P6,S6,V6)</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AA6" s="12">
         <f>AD6+AE6</f>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="12" t="str">
         <f>IF(OR(D6="",F6=""),0,IF(D6&gt;F6,C6,G6))</f>
-        <v>0</v>
+        <v> Netherlands</v>
       </c>
       <c r="AC6" s="12">
         <f>IF(OR(D6="",F6=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="12">
         <f>IF(OR(D6="",F6=""),0,IF(D6&gt;F6,D6,F6))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE6" s="12">
         <f>IF(OR(D6="",F6=""),0,IF(D6&gt;F6,F6,D6))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF6" s="12">
         <f>IF(AND(AD6=3,AE6=0),1,0)</f>
@@ -18035,35 +18059,35 @@
       </c>
       <c r="AH6" s="12">
         <f>IF(AND(AD6=3,AE6=2),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" s="12">
         <f>IF(D6&gt;F6,SUM(H6,K6,N6,Q6,T6,),SUM(J6,M6,P6,S6,V6))</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AJ6" s="12">
         <f>IF(D6&gt;F6,SUM(J6,M6,P6,S6,V6),SUM(H6,K6,N6,Q6,T6))</f>
-        <v>0</v>
-      </c>
-      <c r="AL6" s="12">
+        <v>110</v>
+      </c>
+      <c r="AL6" s="12" t="str">
         <f>IF(OR(D6="",F6=""),0,IF(D6&lt;F6,C6,G6))</f>
-        <v>0</v>
+        <v> Serbia</v>
       </c>
       <c r="AM6" s="12">
         <f>IF(OR(D6="",F6=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="12">
         <f>IF(OR(D6="",F6=""),0,IF(D6&lt;F6,D6,F6))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO6" s="12">
         <f>IF(OR(D6="",F6=""),0,IF(D6&lt;F6,F6,D6))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP6" s="12">
         <f>IF(AND(AN6=2,AO6=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="12">
         <f>IF(AND(AN6=1,AO6=3),1,0)</f>
@@ -18075,11 +18099,11 @@
       </c>
       <c r="AS6" s="12">
         <f>IF(D6&lt;F6,SUM(H6,K6,N6,Q6,T6,),SUM(J6,M6,P6,S6,V6))</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AT6" s="12">
         <f>IF(D6&lt;F6,SUM(J6,M6,P6,S6,V6),SUM(H6,K6,N6,Q6,T6))</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="AX6" s="14"/>
     </row>
@@ -18091,30 +18115,46 @@
         <f>IF(Preliminary!BA63&lt;3,"Winner of Pool H",Preliminary!AY63)</f>
         <v> Japan</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="48">
+        <v>3</v>
+      </c>
       <c r="E7" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="47"/>
+      <c r="F7" s="47">
+        <v>0</v>
+      </c>
       <c r="G7" s="25" t="str">
         <f>IF(Preliminary!BA8&lt;3,"Runners-up of Pool A",Preliminary!AY8)</f>
         <v> Thailand</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="28">
+        <v>25</v>
+      </c>
       <c r="I7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="30">
+        <v>20</v>
+      </c>
+      <c r="K7" s="28">
+        <v>25</v>
+      </c>
       <c r="L7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="28"/>
+      <c r="M7" s="30">
+        <v>23</v>
+      </c>
+      <c r="N7" s="28">
+        <v>25</v>
+      </c>
       <c r="O7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="30"/>
+      <c r="P7" s="30">
+        <v>23</v>
+      </c>
       <c r="Q7" s="28"/>
       <c r="R7" s="29" t="s">
         <v>0</v>
@@ -18127,30 +18167,30 @@
       <c r="V7" s="30"/>
       <c r="W7" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y7" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AA7" s="12">
         <f t="shared" ref="AA7:AA13" si="2">AD7+AE7</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="12" t="str">
         <f t="shared" ref="AB7:AB13" si="3">IF(OR(D7="",F7=""),0,IF(D7&gt;F7,C7,G7))</f>
-        <v>0</v>
+        <v> Japan</v>
       </c>
       <c r="AC7" s="12">
         <f t="shared" ref="AC7:AC13" si="4">IF(OR(D7="",F7=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" s="12">
         <f t="shared" ref="AD7:AD13" si="5">IF(OR(D7="",F7=""),0,IF(D7&gt;F7,D7,F7))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" ref="AE7:AE13" si="6">IF(OR(D7="",F7=""),0,IF(D7&gt;F7,F7,D7))</f>
@@ -18158,7 +18198,7 @@
       </c>
       <c r="AF7" s="12">
         <f t="shared" ref="AF7:AF13" si="7">IF(AND(AD7=3,AE7=0),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" ref="AG7:AG13" si="8">IF(AND(AD7=3,AE7=1),1,0)</f>
@@ -18170,19 +18210,19 @@
       </c>
       <c r="AI7" s="12">
         <f t="shared" ref="AI7:AI13" si="10">IF(D7&gt;F7,SUM(H7,K7,N7,Q7,T7,),SUM(J7,M7,P7,S7,V7))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AJ7" s="12">
         <f t="shared" ref="AJ7:AJ13" si="11">IF(D7&gt;F7,SUM(J7,M7,P7,S7,V7),SUM(H7,K7,N7,Q7,T7))</f>
-        <v>0</v>
-      </c>
-      <c r="AL7" s="12">
+        <v>66</v>
+      </c>
+      <c r="AL7" s="12" t="str">
         <f t="shared" ref="AL7:AL13" si="12">IF(OR(D7="",F7=""),0,IF(D7&lt;F7,C7,G7))</f>
-        <v>0</v>
+        <v> Thailand</v>
       </c>
       <c r="AM7" s="12">
         <f t="shared" ref="AM7:AM13" si="13">IF(OR(D7="",F7=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN7" s="12">
         <f t="shared" ref="AN7:AN13" si="14">IF(OR(D7="",F7=""),0,IF(D7&lt;F7,D7,F7))</f>
@@ -18190,7 +18230,7 @@
       </c>
       <c r="AO7" s="12">
         <f t="shared" ref="AO7:AO13" si="15">IF(OR(D7="",F7=""),0,IF(D7&lt;F7,F7,D7))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP7" s="12">
         <f t="shared" ref="AP7:AP13" si="16">IF(AND(AN7=2,AO7=3),1,0)</f>
@@ -18202,15 +18242,15 @@
       </c>
       <c r="AR7" s="12">
         <f t="shared" ref="AR7:AR13" si="18">IF(AND(AN7=0,AO7=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS7" s="12">
         <f t="shared" ref="AS7:AS13" si="19">IF(D7&lt;F7,SUM(H7,K7,N7,Q7,T7,),SUM(J7,M7,P7,S7,V7))</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="AT7" s="12">
         <f t="shared" ref="AT7:AT13" si="20">IF(D7&lt;F7,SUM(J7,M7,P7,S7,V7),SUM(H7,K7,N7,Q7,T7))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:67" x14ac:dyDescent="0.25">
@@ -19086,52 +19126,52 @@
       <c r="W15" s="77"/>
       <c r="X15" s="77"/>
       <c r="Y15" s="77"/>
-      <c r="AU15" s="64" t="s">
+      <c r="AU15" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="AV15" s="64"/>
+      <c r="AV15" s="62"/>
     </row>
     <row r="16" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
       <c r="G16" s="36"/>
-      <c r="H16" s="75" t="s">
+      <c r="H16" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="75" t="s">
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="75" t="s">
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="75" t="s">
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R16" s="74"/>
-      <c r="S16" s="74"/>
-      <c r="T16" s="75" t="s">
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
       <c r="AA16" s="12" t="s">
         <v>23</v>
       </c>
@@ -19189,10 +19229,10 @@
       <c r="AT16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AU16" s="65" t="s">
+      <c r="AU16" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AV16" s="66"/>
+      <c r="AV16" s="64"/>
     </row>
     <row r="17" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23">
@@ -19200,7 +19240,7 @@
       </c>
       <c r="C17" s="24" t="str">
         <f>IF(AB6=0,"Winner R1",AB6)</f>
-        <v>Winner R1</v>
+        <v> Netherlands</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="49" t="s">
@@ -19209,7 +19249,7 @@
       <c r="F17" s="47"/>
       <c r="G17" s="25" t="str">
         <f>IF(AB7=0,"Winner R2",AB7)</f>
-        <v>Winner R2</v>
+        <v> Japan</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="29" t="s">
@@ -19323,10 +19363,10 @@
         <f>IF(D17&lt;F17,SUM(J17,M17,P17,S17,V17),SUM(H17,K17,N17,Q17,T17))</f>
         <v>0</v>
       </c>
-      <c r="AU17" s="67" t="s">
+      <c r="AU17" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="AV17" s="68"/>
+      <c r="AV17" s="66"/>
     </row>
     <row r="18" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
@@ -19457,10 +19497,10 @@
         <f t="shared" ref="AT18:AT20" si="39">IF(D18&lt;F18,SUM(J18,M18,P18,S18,V18),SUM(H18,K18,N18,Q18,T18))</f>
         <v>0</v>
       </c>
-      <c r="AU18" s="67" t="s">
+      <c r="AU18" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="AV18" s="68"/>
+      <c r="AV18" s="66"/>
     </row>
     <row r="19" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23">
@@ -19591,10 +19631,10 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AU19" s="67" t="s">
+      <c r="AU19" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="AV19" s="68"/>
+      <c r="AV19" s="66"/>
     </row>
     <row r="20" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23">
@@ -19725,10 +19765,10 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AU20" s="69" t="s">
+      <c r="AU20" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="AV20" s="70"/>
+      <c r="AV20" s="68"/>
     </row>
     <row r="21" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -19764,42 +19804,42 @@
         <v>86</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="76" t="s">
+      <c r="D23" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="75" t="s">
+      <c r="H23" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="75" t="s">
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="75" t="s">
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="75" t="s">
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R23" s="74"/>
-      <c r="S23" s="74"/>
-      <c r="T23" s="75" t="s">
+      <c r="R23" s="56"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U23" s="74"/>
-      <c r="V23" s="74"/>
-      <c r="W23" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X23" s="74"/>
-      <c r="Y23" s="74"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="56"/>
       <c r="AA23" s="12" t="s">
         <v>23</v>
       </c>
@@ -20171,42 +20211,42 @@
         <v>86</v>
       </c>
       <c r="C29" s="35"/>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
       <c r="G29" s="36"/>
-      <c r="H29" s="75" t="s">
+      <c r="H29" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75" t="s">
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="75" t="s">
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="75" t="s">
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="74"/>
-      <c r="S29" s="74"/>
-      <c r="T29" s="75" t="s">
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U29" s="74"/>
-      <c r="V29" s="74"/>
-      <c r="W29" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="74"/>
-      <c r="Y29" s="74"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="56"/>
+      <c r="Y29" s="56"/>
       <c r="AA29" s="12" t="s">
         <v>23</v>
       </c>
@@ -20468,42 +20508,42 @@
         <v>86</v>
       </c>
       <c r="C34" s="35"/>
-      <c r="D34" s="76" t="s">
+      <c r="D34" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="75" t="s">
+      <c r="H34" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75" t="s">
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75" t="s">
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O34" s="74"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75" t="s">
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="75" t="s">
+      <c r="R34" s="56"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X34" s="74"/>
-      <c r="Y34" s="74"/>
+      <c r="U34" s="56"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X34" s="56"/>
+      <c r="Y34" s="56"/>
       <c r="AA34" s="12" t="s">
         <v>23</v>
       </c>
@@ -20821,6 +20861,38 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="48">
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="W34:Y34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="B33:Y33"/>
+    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="AU16:AV16"/>
+    <mergeCell ref="AU17:AV17"/>
     <mergeCell ref="B2:AV2"/>
     <mergeCell ref="T16:V16"/>
     <mergeCell ref="W16:Y16"/>
@@ -20837,38 +20909,6 @@
     <mergeCell ref="AU18:AV18"/>
     <mergeCell ref="AU19:AV19"/>
     <mergeCell ref="AU20:AV20"/>
-    <mergeCell ref="B33:Y33"/>
-    <mergeCell ref="AU15:AV15"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="AU16:AV16"/>
-    <mergeCell ref="AU17:AV17"/>
-    <mergeCell ref="W34:Y34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <conditionalFormatting sqref="BM18:XFD18 BM22:XFD23 BM20:XFD20 A18:A20 Z18:Z20 A41:A1048576 B53:Y1048576 B38:Y47 B37 D37:Y37 Z41:AT1048576 BM41:XFD1048576 A3:XFD3 BM6:XFD15 A4:A15 B4:XFD4 Z22:AT22 AA5:AT13 Z26:AT28 Z23:Z25 Z29:Z30 B36:AT36 Z34:Z35 BM25:XFD36 A22:A36 Z31:AT33 Z5:XFD5 B14:AT15 B21:Y22 B28:Y28 B33:Y33 Z6:Z13 AW24:BL1048576 AU21:AV1048576">
     <cfRule type="cellIs" dxfId="31" priority="79" operator="equal">
@@ -21043,15 +21083,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -21284,6 +21315,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -21293,14 +21333,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1A4F3B6-8EF3-43FC-AA6E-56F4B11E76F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21319,19 +21351,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att R16 Complete Results
</commit_message>
<xml_diff>
--- a/2025 FIVB Women's Volleyball World Championship.xlsx
+++ b/2025 FIVB Women's Volleyball World Championship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8AA3544-59FD-4827-8403-BC02A947CAAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3FDF2D4-9AB6-4FA5-A737-AA5296B46BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC01" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="2" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
@@ -863,22 +863,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,28 +912,22 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5393,6 +5393,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:X1"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
@@ -5401,11 +5406,6 @@
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:X1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5478,74 +5478,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:67" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
-      <c r="AC2" s="75"/>
-      <c r="AD2" s="75"/>
-      <c r="AE2" s="75"/>
-      <c r="AF2" s="75"/>
-      <c r="AG2" s="75"/>
-      <c r="AH2" s="75"/>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
-      <c r="AQ2" s="75"/>
-      <c r="AR2" s="75"/>
-      <c r="AS2" s="75"/>
-      <c r="AT2" s="75"/>
-      <c r="AU2" s="75"/>
-      <c r="AV2" s="75"/>
-      <c r="AW2" s="75"/>
-      <c r="AX2" s="75"/>
-      <c r="AY2" s="75"/>
-      <c r="AZ2" s="75"/>
-      <c r="BA2" s="75"/>
-      <c r="BB2" s="75"/>
-      <c r="BC2" s="75"/>
-      <c r="BD2" s="75"/>
-      <c r="BE2" s="75"/>
-      <c r="BF2" s="75"/>
-      <c r="BG2" s="75"/>
-      <c r="BH2" s="75"/>
-      <c r="BI2" s="75"/>
-      <c r="BJ2" s="75"/>
-      <c r="BK2" s="75"/>
-      <c r="BL2" s="75"/>
-      <c r="BM2" s="75"/>
-      <c r="BN2" s="75"/>
-      <c r="BO2" s="75"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
+      <c r="AD2" s="56"/>
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="56"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="56"/>
+      <c r="AJ2" s="56"/>
+      <c r="AK2" s="56"/>
+      <c r="AL2" s="56"/>
+      <c r="AM2" s="56"/>
+      <c r="AN2" s="56"/>
+      <c r="AO2" s="56"/>
+      <c r="AP2" s="56"/>
+      <c r="AQ2" s="56"/>
+      <c r="AR2" s="56"/>
+      <c r="AS2" s="56"/>
+      <c r="AT2" s="56"/>
+      <c r="AU2" s="56"/>
+      <c r="AV2" s="56"/>
+      <c r="AW2" s="56"/>
+      <c r="AX2" s="56"/>
+      <c r="AY2" s="56"/>
+      <c r="AZ2" s="56"/>
+      <c r="BA2" s="56"/>
+      <c r="BB2" s="56"/>
+      <c r="BC2" s="56"/>
+      <c r="BD2" s="56"/>
+      <c r="BE2" s="56"/>
+      <c r="BF2" s="56"/>
+      <c r="BG2" s="56"/>
+      <c r="BH2" s="56"/>
+      <c r="BI2" s="56"/>
+      <c r="BJ2" s="56"/>
+      <c r="BK2" s="56"/>
+      <c r="BL2" s="56"/>
+      <c r="BM2" s="56"/>
+      <c r="BN2" s="56"/>
+      <c r="BO2" s="56"/>
     </row>
     <row r="3" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AX3" s="33"/>
@@ -5568,116 +5568,116 @@
       <c r="BO3" s="33"/>
     </row>
     <row r="4" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="76"/>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="76"/>
-      <c r="AE4" s="76"/>
-      <c r="AF4" s="76"/>
-      <c r="AG4" s="76"/>
-      <c r="AH4" s="76"/>
-      <c r="AI4" s="76"/>
-      <c r="AJ4" s="76"/>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="76"/>
-      <c r="AN4" s="76"/>
-      <c r="AO4" s="76"/>
-      <c r="AP4" s="76"/>
-      <c r="AQ4" s="76"/>
-      <c r="AR4" s="76"/>
-      <c r="AS4" s="76"/>
-      <c r="AT4" s="76"/>
-      <c r="AU4" s="76"/>
-      <c r="AV4" s="76"/>
-      <c r="AW4" s="76"/>
-      <c r="AX4" s="76"/>
-      <c r="AY4" s="76"/>
-      <c r="AZ4" s="76"/>
-      <c r="BA4" s="76"/>
-      <c r="BB4" s="76"/>
-      <c r="BC4" s="76"/>
-      <c r="BD4" s="76"/>
-      <c r="BE4" s="76"/>
-      <c r="BF4" s="76"/>
-      <c r="BG4" s="76"/>
-      <c r="BH4" s="76"/>
-      <c r="BI4" s="76"/>
-      <c r="BJ4" s="76"/>
-      <c r="BK4" s="76"/>
-      <c r="BL4" s="76"/>
-      <c r="BM4" s="76"/>
-      <c r="BN4" s="76"/>
-      <c r="BO4" s="76"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="57"/>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="57"/>
+      <c r="AL4" s="57"/>
+      <c r="AM4" s="57"/>
+      <c r="AN4" s="57"/>
+      <c r="AO4" s="57"/>
+      <c r="AP4" s="57"/>
+      <c r="AQ4" s="57"/>
+      <c r="AR4" s="57"/>
+      <c r="AS4" s="57"/>
+      <c r="AT4" s="57"/>
+      <c r="AU4" s="57"/>
+      <c r="AV4" s="57"/>
+      <c r="AW4" s="57"/>
+      <c r="AX4" s="57"/>
+      <c r="AY4" s="57"/>
+      <c r="AZ4" s="57"/>
+      <c r="BA4" s="57"/>
+      <c r="BB4" s="57"/>
+      <c r="BC4" s="57"/>
+      <c r="BD4" s="57"/>
+      <c r="BE4" s="57"/>
+      <c r="BF4" s="57"/>
+      <c r="BG4" s="57"/>
+      <c r="BH4" s="57"/>
+      <c r="BI4" s="57"/>
+      <c r="BJ4" s="57"/>
+      <c r="BK4" s="57"/>
+      <c r="BL4" s="57"/>
+      <c r="BM4" s="57"/>
+      <c r="BN4" s="57"/>
+      <c r="BO4" s="57"/>
     </row>
     <row r="5" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="57" t="s">
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="57" t="s">
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="57" t="s">
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="57" t="s">
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="56"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
       <c r="AD5" s="12" t="s">
         <v>23</v>
       </c>
@@ -5735,34 +5735,34 @@
       <c r="AW5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX5" s="72" t="s">
+      <c r="AX5" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="74"/>
-      <c r="BA5" s="72" t="s">
+      <c r="AY5" s="62"/>
+      <c r="AZ5" s="63"/>
+      <c r="BA5" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="BB5" s="73"/>
-      <c r="BC5" s="74"/>
-      <c r="BD5" s="72" t="s">
+      <c r="BB5" s="62"/>
+      <c r="BC5" s="63"/>
+      <c r="BD5" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="BE5" s="73"/>
-      <c r="BF5" s="73"/>
-      <c r="BG5" s="73"/>
-      <c r="BH5" s="73"/>
-      <c r="BI5" s="74"/>
-      <c r="BJ5" s="72" t="s">
+      <c r="BE5" s="62"/>
+      <c r="BF5" s="62"/>
+      <c r="BG5" s="62"/>
+      <c r="BH5" s="62"/>
+      <c r="BI5" s="63"/>
+      <c r="BJ5" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="BK5" s="73"/>
-      <c r="BL5" s="74"/>
-      <c r="BM5" s="72" t="s">
+      <c r="BK5" s="62"/>
+      <c r="BL5" s="63"/>
+      <c r="BM5" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="BN5" s="73"/>
-      <c r="BO5" s="74"/>
+      <c r="BN5" s="62"/>
+      <c r="BO5" s="63"/>
     </row>
     <row r="6" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B6" s="23">
@@ -7031,116 +7031,116 @@
       </c>
     </row>
     <row r="12" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="76"/>
-      <c r="S12" s="76"/>
-      <c r="T12" s="76"/>
-      <c r="U12" s="76"/>
-      <c r="V12" s="76"/>
-      <c r="W12" s="76"/>
-      <c r="X12" s="76"/>
-      <c r="Y12" s="76"/>
-      <c r="Z12" s="76"/>
-      <c r="AA12" s="76"/>
-      <c r="AB12" s="76"/>
-      <c r="AC12" s="76"/>
-      <c r="AD12" s="76"/>
-      <c r="AE12" s="76"/>
-      <c r="AF12" s="76"/>
-      <c r="AG12" s="76"/>
-      <c r="AH12" s="76"/>
-      <c r="AI12" s="76"/>
-      <c r="AJ12" s="76"/>
-      <c r="AK12" s="76"/>
-      <c r="AL12" s="76"/>
-      <c r="AM12" s="76"/>
-      <c r="AN12" s="76"/>
-      <c r="AO12" s="76"/>
-      <c r="AP12" s="76"/>
-      <c r="AQ12" s="76"/>
-      <c r="AR12" s="76"/>
-      <c r="AS12" s="76"/>
-      <c r="AT12" s="76"/>
-      <c r="AU12" s="76"/>
-      <c r="AV12" s="76"/>
-      <c r="AW12" s="76"/>
-      <c r="AX12" s="76"/>
-      <c r="AY12" s="76"/>
-      <c r="AZ12" s="76"/>
-      <c r="BA12" s="76"/>
-      <c r="BB12" s="76"/>
-      <c r="BC12" s="76"/>
-      <c r="BD12" s="76"/>
-      <c r="BE12" s="76"/>
-      <c r="BF12" s="76"/>
-      <c r="BG12" s="76"/>
-      <c r="BH12" s="76"/>
-      <c r="BI12" s="76"/>
-      <c r="BJ12" s="76"/>
-      <c r="BK12" s="76"/>
-      <c r="BL12" s="76"/>
-      <c r="BM12" s="76"/>
-      <c r="BN12" s="76"/>
-      <c r="BO12" s="76"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
+      <c r="Y12" s="57"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="57"/>
+      <c r="AF12" s="57"/>
+      <c r="AG12" s="57"/>
+      <c r="AH12" s="57"/>
+      <c r="AI12" s="57"/>
+      <c r="AJ12" s="57"/>
+      <c r="AK12" s="57"/>
+      <c r="AL12" s="57"/>
+      <c r="AM12" s="57"/>
+      <c r="AN12" s="57"/>
+      <c r="AO12" s="57"/>
+      <c r="AP12" s="57"/>
+      <c r="AQ12" s="57"/>
+      <c r="AR12" s="57"/>
+      <c r="AS12" s="57"/>
+      <c r="AT12" s="57"/>
+      <c r="AU12" s="57"/>
+      <c r="AV12" s="57"/>
+      <c r="AW12" s="57"/>
+      <c r="AX12" s="57"/>
+      <c r="AY12" s="57"/>
+      <c r="AZ12" s="57"/>
+      <c r="BA12" s="57"/>
+      <c r="BB12" s="57"/>
+      <c r="BC12" s="57"/>
+      <c r="BD12" s="57"/>
+      <c r="BE12" s="57"/>
+      <c r="BF12" s="57"/>
+      <c r="BG12" s="57"/>
+      <c r="BH12" s="57"/>
+      <c r="BI12" s="57"/>
+      <c r="BJ12" s="57"/>
+      <c r="BK12" s="57"/>
+      <c r="BL12" s="57"/>
+      <c r="BM12" s="57"/>
+      <c r="BN12" s="57"/>
+      <c r="BO12" s="57"/>
     </row>
     <row r="13" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="21"/>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="61" t="s">
+      <c r="H13" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="61" t="s">
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="61" t="s">
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="61" t="s">
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="61" t="s">
+      <c r="R13" s="73"/>
+      <c r="S13" s="73"/>
+      <c r="T13" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U13" s="59"/>
-      <c r="V13" s="59"/>
-      <c r="W13" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X13" s="59"/>
-      <c r="Y13" s="59"/>
+      <c r="U13" s="73"/>
+      <c r="V13" s="73"/>
+      <c r="W13" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="73"/>
+      <c r="Y13" s="73"/>
       <c r="AD13" s="12" t="s">
         <v>23</v>
       </c>
@@ -7198,34 +7198,34 @@
       <c r="AW13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX13" s="69" t="s">
+      <c r="AX13" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY13" s="70"/>
-      <c r="AZ13" s="71"/>
-      <c r="BA13" s="69" t="s">
+      <c r="AY13" s="59"/>
+      <c r="AZ13" s="60"/>
+      <c r="BA13" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB13" s="70"/>
-      <c r="BC13" s="71"/>
-      <c r="BD13" s="69" t="s">
+      <c r="BB13" s="59"/>
+      <c r="BC13" s="60"/>
+      <c r="BD13" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE13" s="70"/>
-      <c r="BF13" s="70"/>
-      <c r="BG13" s="70"/>
-      <c r="BH13" s="70"/>
-      <c r="BI13" s="71"/>
-      <c r="BJ13" s="69" t="s">
+      <c r="BE13" s="59"/>
+      <c r="BF13" s="59"/>
+      <c r="BG13" s="59"/>
+      <c r="BH13" s="59"/>
+      <c r="BI13" s="60"/>
+      <c r="BJ13" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK13" s="70"/>
-      <c r="BL13" s="71"/>
-      <c r="BM13" s="69" t="s">
+      <c r="BK13" s="59"/>
+      <c r="BL13" s="60"/>
+      <c r="BM13" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN13" s="70"/>
-      <c r="BO13" s="71"/>
+      <c r="BN13" s="59"/>
+      <c r="BO13" s="60"/>
     </row>
     <row r="14" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -8478,116 +8478,116 @@
       </c>
     </row>
     <row r="20" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
-      <c r="T20" s="76"/>
-      <c r="U20" s="76"/>
-      <c r="V20" s="76"/>
-      <c r="W20" s="76"/>
-      <c r="X20" s="76"/>
-      <c r="Y20" s="76"/>
-      <c r="Z20" s="76"/>
-      <c r="AA20" s="76"/>
-      <c r="AB20" s="76"/>
-      <c r="AC20" s="76"/>
-      <c r="AD20" s="76"/>
-      <c r="AE20" s="76"/>
-      <c r="AF20" s="76"/>
-      <c r="AG20" s="76"/>
-      <c r="AH20" s="76"/>
-      <c r="AI20" s="76"/>
-      <c r="AJ20" s="76"/>
-      <c r="AK20" s="76"/>
-      <c r="AL20" s="76"/>
-      <c r="AM20" s="76"/>
-      <c r="AN20" s="76"/>
-      <c r="AO20" s="76"/>
-      <c r="AP20" s="76"/>
-      <c r="AQ20" s="76"/>
-      <c r="AR20" s="76"/>
-      <c r="AS20" s="76"/>
-      <c r="AT20" s="76"/>
-      <c r="AU20" s="76"/>
-      <c r="AV20" s="76"/>
-      <c r="AW20" s="76"/>
-      <c r="AX20" s="76"/>
-      <c r="AY20" s="76"/>
-      <c r="AZ20" s="76"/>
-      <c r="BA20" s="76"/>
-      <c r="BB20" s="76"/>
-      <c r="BC20" s="76"/>
-      <c r="BD20" s="76"/>
-      <c r="BE20" s="76"/>
-      <c r="BF20" s="76"/>
-      <c r="BG20" s="76"/>
-      <c r="BH20" s="76"/>
-      <c r="BI20" s="76"/>
-      <c r="BJ20" s="76"/>
-      <c r="BK20" s="76"/>
-      <c r="BL20" s="76"/>
-      <c r="BM20" s="76"/>
-      <c r="BN20" s="76"/>
-      <c r="BO20" s="76"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="57"/>
+      <c r="AA20" s="57"/>
+      <c r="AB20" s="57"/>
+      <c r="AC20" s="57"/>
+      <c r="AD20" s="57"/>
+      <c r="AE20" s="57"/>
+      <c r="AF20" s="57"/>
+      <c r="AG20" s="57"/>
+      <c r="AH20" s="57"/>
+      <c r="AI20" s="57"/>
+      <c r="AJ20" s="57"/>
+      <c r="AK20" s="57"/>
+      <c r="AL20" s="57"/>
+      <c r="AM20" s="57"/>
+      <c r="AN20" s="57"/>
+      <c r="AO20" s="57"/>
+      <c r="AP20" s="57"/>
+      <c r="AQ20" s="57"/>
+      <c r="AR20" s="57"/>
+      <c r="AS20" s="57"/>
+      <c r="AT20" s="57"/>
+      <c r="AU20" s="57"/>
+      <c r="AV20" s="57"/>
+      <c r="AW20" s="57"/>
+      <c r="AX20" s="57"/>
+      <c r="AY20" s="57"/>
+      <c r="AZ20" s="57"/>
+      <c r="BA20" s="57"/>
+      <c r="BB20" s="57"/>
+      <c r="BC20" s="57"/>
+      <c r="BD20" s="57"/>
+      <c r="BE20" s="57"/>
+      <c r="BF20" s="57"/>
+      <c r="BG20" s="57"/>
+      <c r="BH20" s="57"/>
+      <c r="BI20" s="57"/>
+      <c r="BJ20" s="57"/>
+      <c r="BK20" s="57"/>
+      <c r="BL20" s="57"/>
+      <c r="BM20" s="57"/>
+      <c r="BN20" s="57"/>
+      <c r="BO20" s="57"/>
     </row>
     <row r="21" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="61" t="s">
+      <c r="H21" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="61" t="s">
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="61" t="s">
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="61" t="s">
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R21" s="59"/>
-      <c r="S21" s="59"/>
-      <c r="T21" s="61" t="s">
+      <c r="R21" s="73"/>
+      <c r="S21" s="73"/>
+      <c r="T21" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U21" s="59"/>
-      <c r="V21" s="59"/>
-      <c r="W21" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X21" s="59"/>
-      <c r="Y21" s="59"/>
+      <c r="U21" s="73"/>
+      <c r="V21" s="73"/>
+      <c r="W21" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="73"/>
+      <c r="Y21" s="73"/>
       <c r="AD21" s="12" t="s">
         <v>23</v>
       </c>
@@ -8645,34 +8645,34 @@
       <c r="AW21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX21" s="69" t="s">
+      <c r="AX21" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY21" s="70"/>
-      <c r="AZ21" s="71"/>
-      <c r="BA21" s="69" t="s">
+      <c r="AY21" s="59"/>
+      <c r="AZ21" s="60"/>
+      <c r="BA21" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB21" s="70"/>
-      <c r="BC21" s="71"/>
-      <c r="BD21" s="69" t="s">
+      <c r="BB21" s="59"/>
+      <c r="BC21" s="60"/>
+      <c r="BD21" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE21" s="70"/>
-      <c r="BF21" s="70"/>
-      <c r="BG21" s="70"/>
-      <c r="BH21" s="70"/>
-      <c r="BI21" s="71"/>
-      <c r="BJ21" s="69" t="s">
+      <c r="BE21" s="59"/>
+      <c r="BF21" s="59"/>
+      <c r="BG21" s="59"/>
+      <c r="BH21" s="59"/>
+      <c r="BI21" s="60"/>
+      <c r="BJ21" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK21" s="70"/>
-      <c r="BL21" s="71"/>
-      <c r="BM21" s="69" t="s">
+      <c r="BK21" s="59"/>
+      <c r="BL21" s="60"/>
+      <c r="BM21" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN21" s="70"/>
-      <c r="BO21" s="71"/>
+      <c r="BN21" s="59"/>
+      <c r="BO21" s="60"/>
     </row>
     <row r="22" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
@@ -9937,116 +9937,116 @@
       </c>
     </row>
     <row r="28" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="76"/>
-      <c r="S28" s="76"/>
-      <c r="T28" s="76"/>
-      <c r="U28" s="76"/>
-      <c r="V28" s="76"/>
-      <c r="W28" s="76"/>
-      <c r="X28" s="76"/>
-      <c r="Y28" s="76"/>
-      <c r="Z28" s="76"/>
-      <c r="AA28" s="76"/>
-      <c r="AB28" s="76"/>
-      <c r="AC28" s="76"/>
-      <c r="AD28" s="76"/>
-      <c r="AE28" s="76"/>
-      <c r="AF28" s="76"/>
-      <c r="AG28" s="76"/>
-      <c r="AH28" s="76"/>
-      <c r="AI28" s="76"/>
-      <c r="AJ28" s="76"/>
-      <c r="AK28" s="76"/>
-      <c r="AL28" s="76"/>
-      <c r="AM28" s="76"/>
-      <c r="AN28" s="76"/>
-      <c r="AO28" s="76"/>
-      <c r="AP28" s="76"/>
-      <c r="AQ28" s="76"/>
-      <c r="AR28" s="76"/>
-      <c r="AS28" s="76"/>
-      <c r="AT28" s="76"/>
-      <c r="AU28" s="76"/>
-      <c r="AV28" s="76"/>
-      <c r="AW28" s="76"/>
-      <c r="AX28" s="76"/>
-      <c r="AY28" s="76"/>
-      <c r="AZ28" s="76"/>
-      <c r="BA28" s="76"/>
-      <c r="BB28" s="76"/>
-      <c r="BC28" s="76"/>
-      <c r="BD28" s="76"/>
-      <c r="BE28" s="76"/>
-      <c r="BF28" s="76"/>
-      <c r="BG28" s="76"/>
-      <c r="BH28" s="76"/>
-      <c r="BI28" s="76"/>
-      <c r="BJ28" s="76"/>
-      <c r="BK28" s="76"/>
-      <c r="BL28" s="76"/>
-      <c r="BM28" s="76"/>
-      <c r="BN28" s="76"/>
-      <c r="BO28" s="76"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="57"/>
+      <c r="X28" s="57"/>
+      <c r="Y28" s="57"/>
+      <c r="Z28" s="57"/>
+      <c r="AA28" s="57"/>
+      <c r="AB28" s="57"/>
+      <c r="AC28" s="57"/>
+      <c r="AD28" s="57"/>
+      <c r="AE28" s="57"/>
+      <c r="AF28" s="57"/>
+      <c r="AG28" s="57"/>
+      <c r="AH28" s="57"/>
+      <c r="AI28" s="57"/>
+      <c r="AJ28" s="57"/>
+      <c r="AK28" s="57"/>
+      <c r="AL28" s="57"/>
+      <c r="AM28" s="57"/>
+      <c r="AN28" s="57"/>
+      <c r="AO28" s="57"/>
+      <c r="AP28" s="57"/>
+      <c r="AQ28" s="57"/>
+      <c r="AR28" s="57"/>
+      <c r="AS28" s="57"/>
+      <c r="AT28" s="57"/>
+      <c r="AU28" s="57"/>
+      <c r="AV28" s="57"/>
+      <c r="AW28" s="57"/>
+      <c r="AX28" s="57"/>
+      <c r="AY28" s="57"/>
+      <c r="AZ28" s="57"/>
+      <c r="BA28" s="57"/>
+      <c r="BB28" s="57"/>
+      <c r="BC28" s="57"/>
+      <c r="BD28" s="57"/>
+      <c r="BE28" s="57"/>
+      <c r="BF28" s="57"/>
+      <c r="BG28" s="57"/>
+      <c r="BH28" s="57"/>
+      <c r="BI28" s="57"/>
+      <c r="BJ28" s="57"/>
+      <c r="BK28" s="57"/>
+      <c r="BL28" s="57"/>
+      <c r="BM28" s="57"/>
+      <c r="BN28" s="57"/>
+      <c r="BO28" s="57"/>
     </row>
     <row r="29" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="21"/>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="61" t="s">
+      <c r="H29" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="61" t="s">
+      <c r="I29" s="73"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="61" t="s">
+      <c r="L29" s="73"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="61" t="s">
+      <c r="O29" s="73"/>
+      <c r="P29" s="73"/>
+      <c r="Q29" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="59"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="61" t="s">
+      <c r="R29" s="73"/>
+      <c r="S29" s="73"/>
+      <c r="T29" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U29" s="59"/>
-      <c r="V29" s="59"/>
-      <c r="W29" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="59"/>
-      <c r="Y29" s="59"/>
+      <c r="U29" s="73"/>
+      <c r="V29" s="73"/>
+      <c r="W29" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="73"/>
+      <c r="Y29" s="73"/>
       <c r="AD29" s="12" t="s">
         <v>23</v>
       </c>
@@ -10104,34 +10104,34 @@
       <c r="AW29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX29" s="69" t="s">
+      <c r="AX29" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY29" s="70"/>
-      <c r="AZ29" s="71"/>
-      <c r="BA29" s="69" t="s">
+      <c r="AY29" s="59"/>
+      <c r="AZ29" s="60"/>
+      <c r="BA29" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB29" s="70"/>
-      <c r="BC29" s="71"/>
-      <c r="BD29" s="69" t="s">
+      <c r="BB29" s="59"/>
+      <c r="BC29" s="60"/>
+      <c r="BD29" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE29" s="70"/>
-      <c r="BF29" s="70"/>
-      <c r="BG29" s="70"/>
-      <c r="BH29" s="70"/>
-      <c r="BI29" s="71"/>
-      <c r="BJ29" s="69" t="s">
+      <c r="BE29" s="59"/>
+      <c r="BF29" s="59"/>
+      <c r="BG29" s="59"/>
+      <c r="BH29" s="59"/>
+      <c r="BI29" s="60"/>
+      <c r="BJ29" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK29" s="70"/>
-      <c r="BL29" s="71"/>
-      <c r="BM29" s="69" t="s">
+      <c r="BK29" s="59"/>
+      <c r="BL29" s="60"/>
+      <c r="BM29" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN29" s="70"/>
-      <c r="BO29" s="71"/>
+      <c r="BN29" s="59"/>
+      <c r="BO29" s="60"/>
     </row>
     <row r="30" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
@@ -11396,120 +11396,120 @@
       </c>
     </row>
     <row r="36" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-      <c r="N36" s="76"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
-      <c r="R36" s="76"/>
-      <c r="S36" s="76"/>
-      <c r="T36" s="76"/>
-      <c r="U36" s="76"/>
-      <c r="V36" s="76"/>
-      <c r="W36" s="76"/>
-      <c r="X36" s="76"/>
-      <c r="Y36" s="76"/>
-      <c r="Z36" s="76"/>
-      <c r="AA36" s="76"/>
-      <c r="AB36" s="76"/>
-      <c r="AC36" s="76"/>
-      <c r="AD36" s="76"/>
-      <c r="AE36" s="76"/>
-      <c r="AF36" s="76"/>
-      <c r="AG36" s="76"/>
-      <c r="AH36" s="76"/>
-      <c r="AI36" s="76"/>
-      <c r="AJ36" s="76"/>
-      <c r="AK36" s="76"/>
-      <c r="AL36" s="76"/>
-      <c r="AM36" s="76"/>
-      <c r="AN36" s="76"/>
-      <c r="AO36" s="76"/>
-      <c r="AP36" s="76"/>
-      <c r="AQ36" s="76"/>
-      <c r="AR36" s="76"/>
-      <c r="AS36" s="76"/>
-      <c r="AT36" s="76"/>
-      <c r="AU36" s="76"/>
-      <c r="AV36" s="76"/>
-      <c r="AW36" s="76"/>
-      <c r="AX36" s="76"/>
-      <c r="AY36" s="76"/>
-      <c r="AZ36" s="76"/>
-      <c r="BA36" s="76"/>
-      <c r="BB36" s="76"/>
-      <c r="BC36" s="76"/>
-      <c r="BD36" s="76"/>
-      <c r="BE36" s="76"/>
-      <c r="BF36" s="76"/>
-      <c r="BG36" s="76"/>
-      <c r="BH36" s="76"/>
-      <c r="BI36" s="76"/>
-      <c r="BJ36" s="76"/>
-      <c r="BK36" s="76"/>
-      <c r="BL36" s="76"/>
-      <c r="BM36" s="76"/>
-      <c r="BN36" s="76"/>
-      <c r="BO36" s="76"/>
-      <c r="BQ36" s="62" t="s">
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57"/>
+      <c r="R36" s="57"/>
+      <c r="S36" s="57"/>
+      <c r="T36" s="57"/>
+      <c r="U36" s="57"/>
+      <c r="V36" s="57"/>
+      <c r="W36" s="57"/>
+      <c r="X36" s="57"/>
+      <c r="Y36" s="57"/>
+      <c r="Z36" s="57"/>
+      <c r="AA36" s="57"/>
+      <c r="AB36" s="57"/>
+      <c r="AC36" s="57"/>
+      <c r="AD36" s="57"/>
+      <c r="AE36" s="57"/>
+      <c r="AF36" s="57"/>
+      <c r="AG36" s="57"/>
+      <c r="AH36" s="57"/>
+      <c r="AI36" s="57"/>
+      <c r="AJ36" s="57"/>
+      <c r="AK36" s="57"/>
+      <c r="AL36" s="57"/>
+      <c r="AM36" s="57"/>
+      <c r="AN36" s="57"/>
+      <c r="AO36" s="57"/>
+      <c r="AP36" s="57"/>
+      <c r="AQ36" s="57"/>
+      <c r="AR36" s="57"/>
+      <c r="AS36" s="57"/>
+      <c r="AT36" s="57"/>
+      <c r="AU36" s="57"/>
+      <c r="AV36" s="57"/>
+      <c r="AW36" s="57"/>
+      <c r="AX36" s="57"/>
+      <c r="AY36" s="57"/>
+      <c r="AZ36" s="57"/>
+      <c r="BA36" s="57"/>
+      <c r="BB36" s="57"/>
+      <c r="BC36" s="57"/>
+      <c r="BD36" s="57"/>
+      <c r="BE36" s="57"/>
+      <c r="BF36" s="57"/>
+      <c r="BG36" s="57"/>
+      <c r="BH36" s="57"/>
+      <c r="BI36" s="57"/>
+      <c r="BJ36" s="57"/>
+      <c r="BK36" s="57"/>
+      <c r="BL36" s="57"/>
+      <c r="BM36" s="57"/>
+      <c r="BN36" s="57"/>
+      <c r="BO36" s="57"/>
+      <c r="BQ36" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="BR36" s="62"/>
+      <c r="BR36" s="64"/>
     </row>
     <row r="37" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="21"/>
-      <c r="D37" s="60" t="s">
+      <c r="D37" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="61" t="s">
+      <c r="H37" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="61" t="s">
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L37" s="59"/>
-      <c r="M37" s="59"/>
-      <c r="N37" s="61" t="s">
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="61" t="s">
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R37" s="59"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="61" t="s">
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U37" s="59"/>
-      <c r="V37" s="59"/>
-      <c r="W37" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X37" s="59"/>
-      <c r="Y37" s="59"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
+      <c r="W37" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X37" s="73"/>
+      <c r="Y37" s="73"/>
       <c r="AD37" s="12" t="s">
         <v>23</v>
       </c>
@@ -11567,38 +11567,38 @@
       <c r="AW37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX37" s="69" t="s">
+      <c r="AX37" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY37" s="70"/>
-      <c r="AZ37" s="71"/>
-      <c r="BA37" s="69" t="s">
+      <c r="AY37" s="59"/>
+      <c r="AZ37" s="60"/>
+      <c r="BA37" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB37" s="70"/>
-      <c r="BC37" s="71"/>
-      <c r="BD37" s="69" t="s">
+      <c r="BB37" s="59"/>
+      <c r="BC37" s="60"/>
+      <c r="BD37" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE37" s="70"/>
-      <c r="BF37" s="70"/>
-      <c r="BG37" s="70"/>
-      <c r="BH37" s="70"/>
-      <c r="BI37" s="71"/>
-      <c r="BJ37" s="69" t="s">
+      <c r="BE37" s="59"/>
+      <c r="BF37" s="59"/>
+      <c r="BG37" s="59"/>
+      <c r="BH37" s="59"/>
+      <c r="BI37" s="60"/>
+      <c r="BJ37" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK37" s="70"/>
-      <c r="BL37" s="71"/>
-      <c r="BM37" s="69" t="s">
+      <c r="BK37" s="59"/>
+      <c r="BL37" s="60"/>
+      <c r="BM37" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN37" s="70"/>
-      <c r="BO37" s="71"/>
-      <c r="BQ37" s="63" t="s">
+      <c r="BN37" s="59"/>
+      <c r="BO37" s="60"/>
+      <c r="BQ37" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="BR37" s="64"/>
+      <c r="BR37" s="66"/>
     </row>
     <row r="38" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B38" s="23">
@@ -11809,10 +11809,10 @@
       <c r="BO38" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="BQ38" s="65" t="s">
+      <c r="BQ38" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="BR38" s="66"/>
+      <c r="BR38" s="68"/>
     </row>
     <row r="39" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B39" s="23">
@@ -12036,10 +12036,10 @@
         <f>VLOOKUP($AX39,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>1297.1428571428571</v>
       </c>
-      <c r="BQ39" s="65" t="s">
+      <c r="BQ39" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="BR39" s="66"/>
+      <c r="BR39" s="68"/>
     </row>
     <row r="40" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B40" s="23">
@@ -12271,10 +12271,10 @@
         <f>VLOOKUP($AX40,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>1026.5151515151515</v>
       </c>
-      <c r="BQ40" s="65" t="s">
+      <c r="BQ40" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="BR40" s="66"/>
+      <c r="BR40" s="68"/>
     </row>
     <row r="41" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B41" s="23">
@@ -12498,10 +12498,10 @@
         <f>VLOOKUP($AX41,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>973.88059701492534</v>
       </c>
-      <c r="BQ41" s="67" t="s">
+      <c r="BQ41" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="BR41" s="68"/>
+      <c r="BR41" s="70"/>
     </row>
     <row r="42" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B42" s="23">
@@ -12875,116 +12875,116 @@
       </c>
     </row>
     <row r="44" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76"/>
-      <c r="K44" s="76"/>
-      <c r="L44" s="76"/>
-      <c r="M44" s="76"/>
-      <c r="N44" s="76"/>
-      <c r="O44" s="76"/>
-      <c r="P44" s="76"/>
-      <c r="Q44" s="76"/>
-      <c r="R44" s="76"/>
-      <c r="S44" s="76"/>
-      <c r="T44" s="76"/>
-      <c r="U44" s="76"/>
-      <c r="V44" s="76"/>
-      <c r="W44" s="76"/>
-      <c r="X44" s="76"/>
-      <c r="Y44" s="76"/>
-      <c r="Z44" s="76"/>
-      <c r="AA44" s="76"/>
-      <c r="AB44" s="76"/>
-      <c r="AC44" s="76"/>
-      <c r="AD44" s="76"/>
-      <c r="AE44" s="76"/>
-      <c r="AF44" s="76"/>
-      <c r="AG44" s="76"/>
-      <c r="AH44" s="76"/>
-      <c r="AI44" s="76"/>
-      <c r="AJ44" s="76"/>
-      <c r="AK44" s="76"/>
-      <c r="AL44" s="76"/>
-      <c r="AM44" s="76"/>
-      <c r="AN44" s="76"/>
-      <c r="AO44" s="76"/>
-      <c r="AP44" s="76"/>
-      <c r="AQ44" s="76"/>
-      <c r="AR44" s="76"/>
-      <c r="AS44" s="76"/>
-      <c r="AT44" s="76"/>
-      <c r="AU44" s="76"/>
-      <c r="AV44" s="76"/>
-      <c r="AW44" s="76"/>
-      <c r="AX44" s="76"/>
-      <c r="AY44" s="76"/>
-      <c r="AZ44" s="76"/>
-      <c r="BA44" s="76"/>
-      <c r="BB44" s="76"/>
-      <c r="BC44" s="76"/>
-      <c r="BD44" s="76"/>
-      <c r="BE44" s="76"/>
-      <c r="BF44" s="76"/>
-      <c r="BG44" s="76"/>
-      <c r="BH44" s="76"/>
-      <c r="BI44" s="76"/>
-      <c r="BJ44" s="76"/>
-      <c r="BK44" s="76"/>
-      <c r="BL44" s="76"/>
-      <c r="BM44" s="76"/>
-      <c r="BN44" s="76"/>
-      <c r="BO44" s="76"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="57"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+      <c r="P44" s="57"/>
+      <c r="Q44" s="57"/>
+      <c r="R44" s="57"/>
+      <c r="S44" s="57"/>
+      <c r="T44" s="57"/>
+      <c r="U44" s="57"/>
+      <c r="V44" s="57"/>
+      <c r="W44" s="57"/>
+      <c r="X44" s="57"/>
+      <c r="Y44" s="57"/>
+      <c r="Z44" s="57"/>
+      <c r="AA44" s="57"/>
+      <c r="AB44" s="57"/>
+      <c r="AC44" s="57"/>
+      <c r="AD44" s="57"/>
+      <c r="AE44" s="57"/>
+      <c r="AF44" s="57"/>
+      <c r="AG44" s="57"/>
+      <c r="AH44" s="57"/>
+      <c r="AI44" s="57"/>
+      <c r="AJ44" s="57"/>
+      <c r="AK44" s="57"/>
+      <c r="AL44" s="57"/>
+      <c r="AM44" s="57"/>
+      <c r="AN44" s="57"/>
+      <c r="AO44" s="57"/>
+      <c r="AP44" s="57"/>
+      <c r="AQ44" s="57"/>
+      <c r="AR44" s="57"/>
+      <c r="AS44" s="57"/>
+      <c r="AT44" s="57"/>
+      <c r="AU44" s="57"/>
+      <c r="AV44" s="57"/>
+      <c r="AW44" s="57"/>
+      <c r="AX44" s="57"/>
+      <c r="AY44" s="57"/>
+      <c r="AZ44" s="57"/>
+      <c r="BA44" s="57"/>
+      <c r="BB44" s="57"/>
+      <c r="BC44" s="57"/>
+      <c r="BD44" s="57"/>
+      <c r="BE44" s="57"/>
+      <c r="BF44" s="57"/>
+      <c r="BG44" s="57"/>
+      <c r="BH44" s="57"/>
+      <c r="BI44" s="57"/>
+      <c r="BJ44" s="57"/>
+      <c r="BK44" s="57"/>
+      <c r="BL44" s="57"/>
+      <c r="BM44" s="57"/>
+      <c r="BN44" s="57"/>
+      <c r="BO44" s="57"/>
     </row>
     <row r="45" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B45" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C45" s="21"/>
-      <c r="D45" s="60" t="s">
+      <c r="D45" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
       <c r="G45" s="22"/>
-      <c r="H45" s="61" t="s">
+      <c r="H45" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="61" t="s">
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L45" s="59"/>
-      <c r="M45" s="59"/>
-      <c r="N45" s="61" t="s">
+      <c r="L45" s="73"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O45" s="59"/>
-      <c r="P45" s="59"/>
-      <c r="Q45" s="61" t="s">
+      <c r="O45" s="73"/>
+      <c r="P45" s="73"/>
+      <c r="Q45" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R45" s="59"/>
-      <c r="S45" s="59"/>
-      <c r="T45" s="61" t="s">
+      <c r="R45" s="73"/>
+      <c r="S45" s="73"/>
+      <c r="T45" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U45" s="59"/>
-      <c r="V45" s="59"/>
-      <c r="W45" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X45" s="59"/>
-      <c r="Y45" s="59"/>
+      <c r="U45" s="73"/>
+      <c r="V45" s="73"/>
+      <c r="W45" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X45" s="73"/>
+      <c r="Y45" s="73"/>
       <c r="AD45" s="12" t="s">
         <v>23</v>
       </c>
@@ -13042,34 +13042,34 @@
       <c r="AW45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX45" s="69" t="s">
+      <c r="AX45" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY45" s="70"/>
-      <c r="AZ45" s="71"/>
-      <c r="BA45" s="69" t="s">
+      <c r="AY45" s="59"/>
+      <c r="AZ45" s="60"/>
+      <c r="BA45" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB45" s="70"/>
-      <c r="BC45" s="71"/>
-      <c r="BD45" s="69" t="s">
+      <c r="BB45" s="59"/>
+      <c r="BC45" s="60"/>
+      <c r="BD45" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE45" s="70"/>
-      <c r="BF45" s="70"/>
-      <c r="BG45" s="70"/>
-      <c r="BH45" s="70"/>
-      <c r="BI45" s="71"/>
-      <c r="BJ45" s="69" t="s">
+      <c r="BE45" s="59"/>
+      <c r="BF45" s="59"/>
+      <c r="BG45" s="59"/>
+      <c r="BH45" s="59"/>
+      <c r="BI45" s="60"/>
+      <c r="BJ45" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK45" s="70"/>
-      <c r="BL45" s="71"/>
-      <c r="BM45" s="69" t="s">
+      <c r="BK45" s="59"/>
+      <c r="BL45" s="60"/>
+      <c r="BM45" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN45" s="70"/>
-      <c r="BO45" s="71"/>
+      <c r="BN45" s="59"/>
+      <c r="BO45" s="60"/>
     </row>
     <row r="46" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
@@ -14330,116 +14330,116 @@
       </c>
     </row>
     <row r="52" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="76" t="s">
+      <c r="B52" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="76"/>
-      <c r="I52" s="76"/>
-      <c r="J52" s="76"/>
-      <c r="K52" s="76"/>
-      <c r="L52" s="76"/>
-      <c r="M52" s="76"/>
-      <c r="N52" s="76"/>
-      <c r="O52" s="76"/>
-      <c r="P52" s="76"/>
-      <c r="Q52" s="76"/>
-      <c r="R52" s="76"/>
-      <c r="S52" s="76"/>
-      <c r="T52" s="76"/>
-      <c r="U52" s="76"/>
-      <c r="V52" s="76"/>
-      <c r="W52" s="76"/>
-      <c r="X52" s="76"/>
-      <c r="Y52" s="76"/>
-      <c r="Z52" s="76"/>
-      <c r="AA52" s="76"/>
-      <c r="AB52" s="76"/>
-      <c r="AC52" s="76"/>
-      <c r="AD52" s="76"/>
-      <c r="AE52" s="76"/>
-      <c r="AF52" s="76"/>
-      <c r="AG52" s="76"/>
-      <c r="AH52" s="76"/>
-      <c r="AI52" s="76"/>
-      <c r="AJ52" s="76"/>
-      <c r="AK52" s="76"/>
-      <c r="AL52" s="76"/>
-      <c r="AM52" s="76"/>
-      <c r="AN52" s="76"/>
-      <c r="AO52" s="76"/>
-      <c r="AP52" s="76"/>
-      <c r="AQ52" s="76"/>
-      <c r="AR52" s="76"/>
-      <c r="AS52" s="76"/>
-      <c r="AT52" s="76"/>
-      <c r="AU52" s="76"/>
-      <c r="AV52" s="76"/>
-      <c r="AW52" s="76"/>
-      <c r="AX52" s="76"/>
-      <c r="AY52" s="76"/>
-      <c r="AZ52" s="76"/>
-      <c r="BA52" s="76"/>
-      <c r="BB52" s="76"/>
-      <c r="BC52" s="76"/>
-      <c r="BD52" s="76"/>
-      <c r="BE52" s="76"/>
-      <c r="BF52" s="76"/>
-      <c r="BG52" s="76"/>
-      <c r="BH52" s="76"/>
-      <c r="BI52" s="76"/>
-      <c r="BJ52" s="76"/>
-      <c r="BK52" s="76"/>
-      <c r="BL52" s="76"/>
-      <c r="BM52" s="76"/>
-      <c r="BN52" s="76"/>
-      <c r="BO52" s="76"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="57"/>
+      <c r="S52" s="57"/>
+      <c r="T52" s="57"/>
+      <c r="U52" s="57"/>
+      <c r="V52" s="57"/>
+      <c r="W52" s="57"/>
+      <c r="X52" s="57"/>
+      <c r="Y52" s="57"/>
+      <c r="Z52" s="57"/>
+      <c r="AA52" s="57"/>
+      <c r="AB52" s="57"/>
+      <c r="AC52" s="57"/>
+      <c r="AD52" s="57"/>
+      <c r="AE52" s="57"/>
+      <c r="AF52" s="57"/>
+      <c r="AG52" s="57"/>
+      <c r="AH52" s="57"/>
+      <c r="AI52" s="57"/>
+      <c r="AJ52" s="57"/>
+      <c r="AK52" s="57"/>
+      <c r="AL52" s="57"/>
+      <c r="AM52" s="57"/>
+      <c r="AN52" s="57"/>
+      <c r="AO52" s="57"/>
+      <c r="AP52" s="57"/>
+      <c r="AQ52" s="57"/>
+      <c r="AR52" s="57"/>
+      <c r="AS52" s="57"/>
+      <c r="AT52" s="57"/>
+      <c r="AU52" s="57"/>
+      <c r="AV52" s="57"/>
+      <c r="AW52" s="57"/>
+      <c r="AX52" s="57"/>
+      <c r="AY52" s="57"/>
+      <c r="AZ52" s="57"/>
+      <c r="BA52" s="57"/>
+      <c r="BB52" s="57"/>
+      <c r="BC52" s="57"/>
+      <c r="BD52" s="57"/>
+      <c r="BE52" s="57"/>
+      <c r="BF52" s="57"/>
+      <c r="BG52" s="57"/>
+      <c r="BH52" s="57"/>
+      <c r="BI52" s="57"/>
+      <c r="BJ52" s="57"/>
+      <c r="BK52" s="57"/>
+      <c r="BL52" s="57"/>
+      <c r="BM52" s="57"/>
+      <c r="BN52" s="57"/>
+      <c r="BO52" s="57"/>
     </row>
     <row r="53" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B53" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="60" t="s">
+      <c r="D53" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
       <c r="G53" s="22"/>
-      <c r="H53" s="61" t="s">
+      <c r="H53" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I53" s="59"/>
-      <c r="J53" s="59"/>
-      <c r="K53" s="61" t="s">
+      <c r="I53" s="73"/>
+      <c r="J53" s="73"/>
+      <c r="K53" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L53" s="59"/>
-      <c r="M53" s="59"/>
-      <c r="N53" s="61" t="s">
+      <c r="L53" s="73"/>
+      <c r="M53" s="73"/>
+      <c r="N53" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O53" s="59"/>
-      <c r="P53" s="59"/>
-      <c r="Q53" s="61" t="s">
+      <c r="O53" s="73"/>
+      <c r="P53" s="73"/>
+      <c r="Q53" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R53" s="59"/>
-      <c r="S53" s="59"/>
-      <c r="T53" s="61" t="s">
+      <c r="R53" s="73"/>
+      <c r="S53" s="73"/>
+      <c r="T53" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U53" s="59"/>
-      <c r="V53" s="59"/>
-      <c r="W53" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X53" s="59"/>
-      <c r="Y53" s="59"/>
+      <c r="U53" s="73"/>
+      <c r="V53" s="73"/>
+      <c r="W53" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X53" s="73"/>
+      <c r="Y53" s="73"/>
       <c r="AD53" s="12" t="s">
         <v>23</v>
       </c>
@@ -14497,34 +14497,34 @@
       <c r="AW53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX53" s="69" t="s">
+      <c r="AX53" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY53" s="70"/>
-      <c r="AZ53" s="71"/>
-      <c r="BA53" s="69" t="s">
+      <c r="AY53" s="59"/>
+      <c r="AZ53" s="60"/>
+      <c r="BA53" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB53" s="70"/>
-      <c r="BC53" s="71"/>
-      <c r="BD53" s="69" t="s">
+      <c r="BB53" s="59"/>
+      <c r="BC53" s="60"/>
+      <c r="BD53" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE53" s="70"/>
-      <c r="BF53" s="70"/>
-      <c r="BG53" s="70"/>
-      <c r="BH53" s="70"/>
-      <c r="BI53" s="71"/>
-      <c r="BJ53" s="69" t="s">
+      <c r="BE53" s="59"/>
+      <c r="BF53" s="59"/>
+      <c r="BG53" s="59"/>
+      <c r="BH53" s="59"/>
+      <c r="BI53" s="60"/>
+      <c r="BJ53" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK53" s="70"/>
-      <c r="BL53" s="71"/>
-      <c r="BM53" s="69" t="s">
+      <c r="BK53" s="59"/>
+      <c r="BL53" s="60"/>
+      <c r="BM53" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN53" s="70"/>
-      <c r="BO53" s="71"/>
+      <c r="BN53" s="59"/>
+      <c r="BO53" s="60"/>
     </row>
     <row r="54" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B54" s="23">
@@ -15785,116 +15785,116 @@
       </c>
     </row>
     <row r="60" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="76" t="s">
+      <c r="B60" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="76"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="76"/>
-      <c r="I60" s="76"/>
-      <c r="J60" s="76"/>
-      <c r="K60" s="76"/>
-      <c r="L60" s="76"/>
-      <c r="M60" s="76"/>
-      <c r="N60" s="76"/>
-      <c r="O60" s="76"/>
-      <c r="P60" s="76"/>
-      <c r="Q60" s="76"/>
-      <c r="R60" s="76"/>
-      <c r="S60" s="76"/>
-      <c r="T60" s="76"/>
-      <c r="U60" s="76"/>
-      <c r="V60" s="76"/>
-      <c r="W60" s="76"/>
-      <c r="X60" s="76"/>
-      <c r="Y60" s="76"/>
-      <c r="Z60" s="76"/>
-      <c r="AA60" s="76"/>
-      <c r="AB60" s="76"/>
-      <c r="AC60" s="76"/>
-      <c r="AD60" s="76"/>
-      <c r="AE60" s="76"/>
-      <c r="AF60" s="76"/>
-      <c r="AG60" s="76"/>
-      <c r="AH60" s="76"/>
-      <c r="AI60" s="76"/>
-      <c r="AJ60" s="76"/>
-      <c r="AK60" s="76"/>
-      <c r="AL60" s="76"/>
-      <c r="AM60" s="76"/>
-      <c r="AN60" s="76"/>
-      <c r="AO60" s="76"/>
-      <c r="AP60" s="76"/>
-      <c r="AQ60" s="76"/>
-      <c r="AR60" s="76"/>
-      <c r="AS60" s="76"/>
-      <c r="AT60" s="76"/>
-      <c r="AU60" s="76"/>
-      <c r="AV60" s="76"/>
-      <c r="AW60" s="76"/>
-      <c r="AX60" s="76"/>
-      <c r="AY60" s="76"/>
-      <c r="AZ60" s="76"/>
-      <c r="BA60" s="76"/>
-      <c r="BB60" s="76"/>
-      <c r="BC60" s="76"/>
-      <c r="BD60" s="76"/>
-      <c r="BE60" s="76"/>
-      <c r="BF60" s="76"/>
-      <c r="BG60" s="76"/>
-      <c r="BH60" s="76"/>
-      <c r="BI60" s="76"/>
-      <c r="BJ60" s="76"/>
-      <c r="BK60" s="76"/>
-      <c r="BL60" s="76"/>
-      <c r="BM60" s="76"/>
-      <c r="BN60" s="76"/>
-      <c r="BO60" s="76"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
+      <c r="F60" s="57"/>
+      <c r="G60" s="57"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="57"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="57"/>
+      <c r="L60" s="57"/>
+      <c r="M60" s="57"/>
+      <c r="N60" s="57"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="57"/>
+      <c r="Q60" s="57"/>
+      <c r="R60" s="57"/>
+      <c r="S60" s="57"/>
+      <c r="T60" s="57"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="57"/>
+      <c r="W60" s="57"/>
+      <c r="X60" s="57"/>
+      <c r="Y60" s="57"/>
+      <c r="Z60" s="57"/>
+      <c r="AA60" s="57"/>
+      <c r="AB60" s="57"/>
+      <c r="AC60" s="57"/>
+      <c r="AD60" s="57"/>
+      <c r="AE60" s="57"/>
+      <c r="AF60" s="57"/>
+      <c r="AG60" s="57"/>
+      <c r="AH60" s="57"/>
+      <c r="AI60" s="57"/>
+      <c r="AJ60" s="57"/>
+      <c r="AK60" s="57"/>
+      <c r="AL60" s="57"/>
+      <c r="AM60" s="57"/>
+      <c r="AN60" s="57"/>
+      <c r="AO60" s="57"/>
+      <c r="AP60" s="57"/>
+      <c r="AQ60" s="57"/>
+      <c r="AR60" s="57"/>
+      <c r="AS60" s="57"/>
+      <c r="AT60" s="57"/>
+      <c r="AU60" s="57"/>
+      <c r="AV60" s="57"/>
+      <c r="AW60" s="57"/>
+      <c r="AX60" s="57"/>
+      <c r="AY60" s="57"/>
+      <c r="AZ60" s="57"/>
+      <c r="BA60" s="57"/>
+      <c r="BB60" s="57"/>
+      <c r="BC60" s="57"/>
+      <c r="BD60" s="57"/>
+      <c r="BE60" s="57"/>
+      <c r="BF60" s="57"/>
+      <c r="BG60" s="57"/>
+      <c r="BH60" s="57"/>
+      <c r="BI60" s="57"/>
+      <c r="BJ60" s="57"/>
+      <c r="BK60" s="57"/>
+      <c r="BL60" s="57"/>
+      <c r="BM60" s="57"/>
+      <c r="BN60" s="57"/>
+      <c r="BO60" s="57"/>
     </row>
     <row r="61" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B61" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="21"/>
-      <c r="D61" s="60" t="s">
+      <c r="D61" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="E61" s="60"/>
-      <c r="F61" s="60"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="71"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="61" t="s">
+      <c r="H61" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="I61" s="59"/>
-      <c r="J61" s="59"/>
-      <c r="K61" s="61" t="s">
+      <c r="I61" s="73"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="L61" s="59"/>
-      <c r="M61" s="59"/>
-      <c r="N61" s="61" t="s">
+      <c r="L61" s="73"/>
+      <c r="M61" s="73"/>
+      <c r="N61" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="O61" s="59"/>
-      <c r="P61" s="59"/>
-      <c r="Q61" s="61" t="s">
+      <c r="O61" s="73"/>
+      <c r="P61" s="73"/>
+      <c r="Q61" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="R61" s="59"/>
-      <c r="S61" s="59"/>
-      <c r="T61" s="61" t="s">
+      <c r="R61" s="73"/>
+      <c r="S61" s="73"/>
+      <c r="T61" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="U61" s="59"/>
-      <c r="V61" s="59"/>
-      <c r="W61" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="X61" s="59"/>
-      <c r="Y61" s="59"/>
+      <c r="U61" s="73"/>
+      <c r="V61" s="73"/>
+      <c r="W61" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="X61" s="73"/>
+      <c r="Y61" s="73"/>
       <c r="AD61" s="12" t="s">
         <v>23</v>
       </c>
@@ -15952,34 +15952,34 @@
       <c r="AW61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX61" s="69" t="s">
+      <c r="AX61" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="AY61" s="70"/>
-      <c r="AZ61" s="71"/>
-      <c r="BA61" s="69" t="s">
+      <c r="AY61" s="59"/>
+      <c r="AZ61" s="60"/>
+      <c r="BA61" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="BB61" s="70"/>
-      <c r="BC61" s="71"/>
-      <c r="BD61" s="69" t="s">
+      <c r="BB61" s="59"/>
+      <c r="BC61" s="60"/>
+      <c r="BD61" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="BE61" s="70"/>
-      <c r="BF61" s="70"/>
-      <c r="BG61" s="70"/>
-      <c r="BH61" s="70"/>
-      <c r="BI61" s="71"/>
-      <c r="BJ61" s="69" t="s">
+      <c r="BE61" s="59"/>
+      <c r="BF61" s="59"/>
+      <c r="BG61" s="59"/>
+      <c r="BH61" s="59"/>
+      <c r="BI61" s="60"/>
+      <c r="BJ61" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="BK61" s="70"/>
-      <c r="BL61" s="71"/>
-      <c r="BM61" s="69" t="s">
+      <c r="BK61" s="59"/>
+      <c r="BL61" s="60"/>
+      <c r="BM61" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="BN61" s="70"/>
-      <c r="BO61" s="71"/>
+      <c r="BN61" s="59"/>
+      <c r="BO61" s="60"/>
     </row>
     <row r="62" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B62" s="11">
@@ -17238,6 +17238,93 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="111">
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="T37:V37"/>
+    <mergeCell ref="W37:Y37"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="T61:V61"/>
+    <mergeCell ref="W61:Y61"/>
+    <mergeCell ref="W45:Y45"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="T53:V53"/>
+    <mergeCell ref="W53:Y53"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="T45:V45"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BQ37:BR37"/>
+    <mergeCell ref="BQ38:BR38"/>
+    <mergeCell ref="BQ39:BR39"/>
+    <mergeCell ref="BQ40:BR40"/>
+    <mergeCell ref="BQ41:BR41"/>
+    <mergeCell ref="AX29:AZ29"/>
+    <mergeCell ref="BA29:BC29"/>
+    <mergeCell ref="BD29:BI29"/>
+    <mergeCell ref="BJ29:BL29"/>
+    <mergeCell ref="BM29:BO29"/>
+    <mergeCell ref="AX37:AZ37"/>
+    <mergeCell ref="BA37:BC37"/>
+    <mergeCell ref="BD37:BI37"/>
+    <mergeCell ref="BJ37:BL37"/>
+    <mergeCell ref="BM37:BO37"/>
+    <mergeCell ref="BJ21:BL21"/>
+    <mergeCell ref="BM21:BO21"/>
+    <mergeCell ref="AX61:AZ61"/>
+    <mergeCell ref="BA61:BC61"/>
+    <mergeCell ref="BD61:BI61"/>
+    <mergeCell ref="BJ61:BL61"/>
+    <mergeCell ref="BM61:BO61"/>
+    <mergeCell ref="AX45:AZ45"/>
+    <mergeCell ref="BA5:BC5"/>
+    <mergeCell ref="BD5:BI5"/>
+    <mergeCell ref="BJ5:BL5"/>
+    <mergeCell ref="BM5:BO5"/>
+    <mergeCell ref="AX5:AZ5"/>
+    <mergeCell ref="BA13:BC13"/>
+    <mergeCell ref="BD13:BI13"/>
     <mergeCell ref="B2:BO2"/>
     <mergeCell ref="B4:BO4"/>
     <mergeCell ref="B12:BO12"/>
@@ -17262,93 +17349,6 @@
     <mergeCell ref="AX21:AZ21"/>
     <mergeCell ref="BA21:BC21"/>
     <mergeCell ref="BD21:BI21"/>
-    <mergeCell ref="BJ21:BL21"/>
-    <mergeCell ref="BM21:BO21"/>
-    <mergeCell ref="AX61:AZ61"/>
-    <mergeCell ref="BA61:BC61"/>
-    <mergeCell ref="BD61:BI61"/>
-    <mergeCell ref="BJ61:BL61"/>
-    <mergeCell ref="BM61:BO61"/>
-    <mergeCell ref="AX45:AZ45"/>
-    <mergeCell ref="BA5:BC5"/>
-    <mergeCell ref="BD5:BI5"/>
-    <mergeCell ref="BJ5:BL5"/>
-    <mergeCell ref="BM5:BO5"/>
-    <mergeCell ref="AX5:AZ5"/>
-    <mergeCell ref="BA13:BC13"/>
-    <mergeCell ref="BD13:BI13"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BQ37:BR37"/>
-    <mergeCell ref="BQ38:BR38"/>
-    <mergeCell ref="BQ39:BR39"/>
-    <mergeCell ref="BQ40:BR40"/>
-    <mergeCell ref="BQ41:BR41"/>
-    <mergeCell ref="AX29:AZ29"/>
-    <mergeCell ref="BA29:BC29"/>
-    <mergeCell ref="BD29:BI29"/>
-    <mergeCell ref="BJ29:BL29"/>
-    <mergeCell ref="BM29:BO29"/>
-    <mergeCell ref="AX37:AZ37"/>
-    <mergeCell ref="BA37:BC37"/>
-    <mergeCell ref="BD37:BI37"/>
-    <mergeCell ref="BJ37:BL37"/>
-    <mergeCell ref="BM37:BO37"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="T61:V61"/>
-    <mergeCell ref="W61:Y61"/>
-    <mergeCell ref="W45:Y45"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="T53:V53"/>
-    <mergeCell ref="W53:Y53"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="T45:V45"/>
-    <mergeCell ref="Q37:S37"/>
-    <mergeCell ref="T37:V37"/>
-    <mergeCell ref="W37:Y37"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:Y21"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
   </mergeCells>
   <conditionalFormatting sqref="T6:V11 T22:V27 T54:V59">
     <cfRule type="expression" dxfId="95" priority="472">
@@ -17687,7 +17687,7 @@
   <dimension ref="B1:BO48"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17756,55 +17756,55 @@
       <c r="Y1" s="18"/>
     </row>
     <row r="2" spans="2:67" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
-      <c r="AC2" s="75"/>
-      <c r="AD2" s="75"/>
-      <c r="AE2" s="75"/>
-      <c r="AF2" s="75"/>
-      <c r="AG2" s="75"/>
-      <c r="AH2" s="75"/>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
-      <c r="AQ2" s="75"/>
-      <c r="AR2" s="75"/>
-      <c r="AS2" s="75"/>
-      <c r="AT2" s="75"/>
-      <c r="AU2" s="75"/>
-      <c r="AV2" s="75"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
+      <c r="AD2" s="56"/>
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="56"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="56"/>
+      <c r="AJ2" s="56"/>
+      <c r="AK2" s="56"/>
+      <c r="AL2" s="56"/>
+      <c r="AM2" s="56"/>
+      <c r="AN2" s="56"/>
+      <c r="AO2" s="56"/>
+      <c r="AP2" s="56"/>
+      <c r="AQ2" s="56"/>
+      <c r="AR2" s="56"/>
+      <c r="AS2" s="56"/>
+      <c r="AT2" s="56"/>
+      <c r="AU2" s="56"/>
+      <c r="AV2" s="56"/>
       <c r="AW2" s="46"/>
       <c r="AX2" s="46"/>
       <c r="AY2" s="46"/>
@@ -17858,42 +17858,42 @@
         <v>86</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="57" t="s">
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="57" t="s">
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="57" t="s">
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="57" t="s">
+      <c r="R5" s="74"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="56"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
       <c r="AA5" s="12" t="s">
         <v>23</v>
       </c>
@@ -18261,30 +18261,46 @@
         <f>IF(Preliminary!BA15&lt;3,"Winner of Pool B",Preliminary!AY15)</f>
         <v> Italy</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="48">
+        <v>3</v>
+      </c>
       <c r="E8" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="47"/>
+      <c r="F8" s="47">
+        <v>0</v>
+      </c>
       <c r="G8" s="25" t="str">
         <f>IF(Preliminary!BA56&lt;3,"Runners-up of Pool G",Preliminary!AY56)</f>
         <v> Germany</v>
       </c>
-      <c r="H8" s="28"/>
+      <c r="H8" s="28">
+        <v>25</v>
+      </c>
       <c r="I8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="28"/>
+      <c r="J8" s="30">
+        <v>22</v>
+      </c>
+      <c r="K8" s="28">
+        <v>25</v>
+      </c>
       <c r="L8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="28"/>
+      <c r="M8" s="30">
+        <v>18</v>
+      </c>
+      <c r="N8" s="28">
+        <v>25</v>
+      </c>
       <c r="O8" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P8" s="30"/>
+      <c r="P8" s="30">
+        <v>11</v>
+      </c>
       <c r="Q8" s="28"/>
       <c r="R8" s="29" t="s">
         <v>0</v>
@@ -18297,30 +18313,30 @@
       <c r="V8" s="30"/>
       <c r="W8" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y8" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="AA8" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB8" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v> Italy</v>
       </c>
       <c r="AC8" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="6"/>
@@ -18328,7 +18344,7 @@
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="8"/>
@@ -18340,19 +18356,19 @@
       </c>
       <c r="AI8" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AJ8" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL8" s="12">
+        <v>51</v>
+      </c>
+      <c r="AL8" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v> Germany</v>
       </c>
       <c r="AM8" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="12">
         <f t="shared" si="14"/>
@@ -18360,7 +18376,7 @@
       </c>
       <c r="AO8" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP8" s="12">
         <f t="shared" si="16"/>
@@ -18372,15 +18388,15 @@
       </c>
       <c r="AR8" s="12">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS8" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="AT8" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="2:67" x14ac:dyDescent="0.25">
@@ -18391,70 +18407,94 @@
         <f>IF(Preliminary!BA55&lt;3,"Winner of Pool G",Preliminary!AY55)</f>
         <v> Poland</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="48">
+        <v>3</v>
+      </c>
       <c r="E9" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="47"/>
+      <c r="F9" s="47">
+        <v>2</v>
+      </c>
       <c r="G9" s="25" t="str">
         <f>IF(Preliminary!BA16&lt;3,"Runners-up of Pool B",Preliminary!AY16)</f>
         <v> Belgium</v>
       </c>
-      <c r="H9" s="28"/>
+      <c r="H9" s="28">
+        <v>25</v>
+      </c>
       <c r="I9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="28"/>
+      <c r="J9" s="30">
+        <v>27</v>
+      </c>
+      <c r="K9" s="28">
+        <v>25</v>
+      </c>
       <c r="L9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="28"/>
+      <c r="M9" s="30">
+        <v>20</v>
+      </c>
+      <c r="N9" s="28">
+        <v>25</v>
+      </c>
       <c r="O9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="28"/>
+      <c r="P9" s="30">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="28">
+        <v>22</v>
+      </c>
       <c r="R9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S9" s="30"/>
-      <c r="T9" s="28"/>
+      <c r="S9" s="30">
+        <v>25</v>
+      </c>
+      <c r="T9" s="28">
+        <v>15</v>
+      </c>
       <c r="U9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="V9" s="30"/>
+      <c r="V9" s="30">
+        <v>10</v>
+      </c>
       <c r="W9" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="X9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y9" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AA9" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="12">
+        <v>5</v>
+      </c>
+      <c r="AB9" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v> Poland</v>
       </c>
       <c r="AC9" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="7"/>
@@ -18466,35 +18506,35 @@
       </c>
       <c r="AH9" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="AJ9" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL9" s="12">
+        <v>99</v>
+      </c>
+      <c r="AL9" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v> Belgium</v>
       </c>
       <c r="AM9" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN9" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO9" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP9" s="12">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ9" s="12">
         <f t="shared" si="17"/>
@@ -18506,11 +18546,11 @@
       </c>
       <c r="AS9" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AT9" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:67" x14ac:dyDescent="0.25">
@@ -18521,35 +18561,55 @@
         <f>IF(Preliminary!BA23&lt;3,"Winner of Pool C",Preliminary!AY23)</f>
         <v> Brazil</v>
       </c>
-      <c r="D10" s="48"/>
+      <c r="D10" s="48">
+        <v>3</v>
+      </c>
       <c r="E10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="47"/>
+      <c r="F10" s="47">
+        <v>1</v>
+      </c>
       <c r="G10" s="25" t="str">
         <f>IF(Preliminary!BA48&lt;3,"Runners-up of Pool F",Preliminary!AY48)</f>
         <v> Dominican Republic</v>
       </c>
-      <c r="H10" s="28"/>
+      <c r="H10" s="28">
+        <v>18</v>
+      </c>
       <c r="I10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="30"/>
-      <c r="K10" s="28"/>
+      <c r="J10" s="30">
+        <v>25</v>
+      </c>
+      <c r="K10" s="28">
+        <v>25</v>
+      </c>
       <c r="L10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="28"/>
+      <c r="M10" s="30">
+        <v>12</v>
+      </c>
+      <c r="N10" s="28">
+        <v>25</v>
+      </c>
       <c r="O10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="28"/>
+      <c r="P10" s="30">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="28">
+        <v>25</v>
+      </c>
       <c r="R10" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S10" s="30"/>
+      <c r="S10" s="30">
+        <v>12</v>
+      </c>
       <c r="T10" s="28"/>
       <c r="U10" s="29" t="s">
         <v>0</v>
@@ -18557,34 +18617,34 @@
       <c r="V10" s="30"/>
       <c r="W10" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="X10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y10" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="AA10" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="12">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v> Brazil</v>
       </c>
       <c r="AC10" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="7"/>
@@ -18592,7 +18652,7 @@
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="9"/>
@@ -18600,27 +18660,27 @@
       </c>
       <c r="AI10" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="AJ10" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL10" s="12">
+        <v>69</v>
+      </c>
+      <c r="AL10" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v> Dominican Republic</v>
       </c>
       <c r="AM10" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN10" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO10" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP10" s="12">
         <f t="shared" si="16"/>
@@ -18628,7 +18688,7 @@
       </c>
       <c r="AQ10" s="12">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR10" s="12">
         <f t="shared" si="18"/>
@@ -18636,11 +18696,11 @@
       </c>
       <c r="AS10" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="AT10" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18651,35 +18711,55 @@
         <f>IF(Preliminary!BA47&lt;3,"Winner of Pool F",Preliminary!AY47)</f>
         <v> China</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="48">
+        <v>1</v>
+      </c>
       <c r="E11" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="47"/>
+      <c r="F11" s="47">
+        <v>3</v>
+      </c>
       <c r="G11" s="25" t="str">
         <f>IF(Preliminary!BA24&lt;3,"Runners-up of Pool C",Preliminary!AY24)</f>
         <v> France</v>
       </c>
-      <c r="H11" s="28"/>
+      <c r="H11" s="28">
+        <v>20</v>
+      </c>
       <c r="I11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="28"/>
+      <c r="J11" s="30">
+        <v>25</v>
+      </c>
+      <c r="K11" s="28">
+        <v>25</v>
+      </c>
       <c r="L11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="28"/>
+      <c r="M11" s="30">
+        <v>27</v>
+      </c>
+      <c r="N11" s="28">
+        <v>25</v>
+      </c>
       <c r="O11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="28"/>
+      <c r="P11" s="30">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>20</v>
+      </c>
       <c r="R11" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S11" s="30"/>
+      <c r="S11" s="30">
+        <v>25</v>
+      </c>
       <c r="T11" s="28"/>
       <c r="U11" s="29" t="s">
         <v>0</v>
@@ -18687,34 +18767,34 @@
       <c r="V11" s="30"/>
       <c r="W11" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="X11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y11" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AA11" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="12">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v> France</v>
       </c>
       <c r="AC11" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="7"/>
@@ -18722,7 +18802,7 @@
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="9"/>
@@ -18730,27 +18810,27 @@
       </c>
       <c r="AI11" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AJ11" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL11" s="12">
+        <v>90</v>
+      </c>
+      <c r="AL11" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v> China</v>
       </c>
       <c r="AM11" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN11" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO11" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP11" s="12">
         <f t="shared" si="16"/>
@@ -18758,7 +18838,7 @@
       </c>
       <c r="AQ11" s="12">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR11" s="12">
         <f t="shared" si="18"/>
@@ -18766,11 +18846,11 @@
       </c>
       <c r="AS11" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AT11" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="AW11" s="38"/>
       <c r="AX11" s="38"/>
@@ -18797,30 +18877,46 @@
         <f>IF(Preliminary!BA31&lt;3,"Winner of Pool D",Preliminary!AY31)</f>
         <v> United States</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="48">
+        <v>3</v>
+      </c>
       <c r="E12" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="47"/>
+      <c r="F12" s="47">
+        <v>0</v>
+      </c>
       <c r="G12" s="25" t="str">
         <f>IF(Preliminary!BA40&lt;3,"Runners-up of Pool E",Preliminary!AY40)</f>
         <v> Canada</v>
       </c>
-      <c r="H12" s="28"/>
+      <c r="H12" s="28">
+        <v>25</v>
+      </c>
       <c r="I12" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="30"/>
-      <c r="K12" s="28"/>
+      <c r="J12" s="30">
+        <v>18</v>
+      </c>
+      <c r="K12" s="28">
+        <v>25</v>
+      </c>
       <c r="L12" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M12" s="30"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="30">
+        <v>21</v>
+      </c>
+      <c r="N12" s="28">
+        <v>25</v>
+      </c>
       <c r="O12" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="30"/>
+      <c r="P12" s="30">
+        <v>21</v>
+      </c>
       <c r="Q12" s="28"/>
       <c r="R12" s="29" t="s">
         <v>0</v>
@@ -18833,30 +18929,30 @@
       <c r="V12" s="30"/>
       <c r="W12" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y12" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AA12" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v> United States</v>
       </c>
       <c r="AC12" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="6"/>
@@ -18864,7 +18960,7 @@
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="8"/>
@@ -18876,19 +18972,19 @@
       </c>
       <c r="AI12" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AJ12" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL12" s="12">
+        <v>60</v>
+      </c>
+      <c r="AL12" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v> Canada</v>
       </c>
       <c r="AM12" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN12" s="12">
         <f t="shared" si="14"/>
@@ -18896,7 +18992,7 @@
       </c>
       <c r="AO12" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP12" s="12">
         <f t="shared" si="16"/>
@@ -18908,15 +19004,15 @@
       </c>
       <c r="AR12" s="12">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS12" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AT12" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AW12" s="39"/>
       <c r="AX12" s="39"/>
@@ -18943,30 +19039,46 @@
         <f>IF(Preliminary!BA39&lt;3,"Winner of Pool E",Preliminary!AY39)</f>
         <v> Turkey</v>
       </c>
-      <c r="D13" s="48"/>
+      <c r="D13" s="48">
+        <v>3</v>
+      </c>
       <c r="E13" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="47"/>
+      <c r="F13" s="47">
+        <v>0</v>
+      </c>
       <c r="G13" s="25" t="str">
         <f>IF(Preliminary!BA32&lt;3,"Runners-up of Pool D",Preliminary!AY32)</f>
         <v> Slovenia</v>
       </c>
-      <c r="H13" s="28"/>
+      <c r="H13" s="28">
+        <v>30</v>
+      </c>
       <c r="I13" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="28"/>
+      <c r="J13" s="30">
+        <v>28</v>
+      </c>
+      <c r="K13" s="28">
+        <v>25</v>
+      </c>
       <c r="L13" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="28"/>
+      <c r="M13" s="30">
+        <v>13</v>
+      </c>
+      <c r="N13" s="28">
+        <v>29</v>
+      </c>
       <c r="O13" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P13" s="30"/>
+      <c r="P13" s="30">
+        <v>27</v>
+      </c>
       <c r="Q13" s="28"/>
       <c r="R13" s="29" t="s">
         <v>0</v>
@@ -18979,30 +19091,30 @@
       <c r="V13" s="30"/>
       <c r="W13" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y13" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="AA13" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v> Turkey</v>
       </c>
       <c r="AC13" s="12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="6"/>
@@ -19010,7 +19122,7 @@
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="8"/>
@@ -19022,19 +19134,19 @@
       </c>
       <c r="AI13" s="12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="AJ13" s="12">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AL13" s="12">
+        <v>68</v>
+      </c>
+      <c r="AL13" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v> Slovenia</v>
       </c>
       <c r="AM13" s="12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN13" s="12">
         <f t="shared" si="14"/>
@@ -19042,7 +19154,7 @@
       </c>
       <c r="AO13" s="12">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP13" s="12">
         <f t="shared" si="16"/>
@@ -19054,15 +19166,15 @@
       </c>
       <c r="AR13" s="12">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS13" s="12">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="AT13" s="12">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="AW13" s="39"/>
       <c r="AX13" s="39"/>
@@ -19126,52 +19238,52 @@
       <c r="W15" s="77"/>
       <c r="X15" s="77"/>
       <c r="Y15" s="77"/>
-      <c r="AU15" s="62" t="s">
+      <c r="AU15" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="AV15" s="62"/>
+      <c r="AV15" s="64"/>
     </row>
     <row r="16" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
       <c r="G16" s="36"/>
-      <c r="H16" s="57" t="s">
+      <c r="H16" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="57" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57" t="s">
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="57" t="s">
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="57" t="s">
+      <c r="R16" s="74"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" s="74"/>
+      <c r="Y16" s="74"/>
       <c r="AA16" s="12" t="s">
         <v>23</v>
       </c>
@@ -19229,10 +19341,10 @@
       <c r="AT16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AU16" s="63" t="s">
+      <c r="AU16" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="AV16" s="64"/>
+      <c r="AV16" s="66"/>
     </row>
     <row r="17" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23">
@@ -19363,10 +19475,10 @@
         <f>IF(D17&lt;F17,SUM(J17,M17,P17,S17,V17),SUM(H17,K17,N17,Q17,T17))</f>
         <v>0</v>
       </c>
-      <c r="AU17" s="65" t="s">
+      <c r="AU17" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="AV17" s="66"/>
+      <c r="AV17" s="68"/>
     </row>
     <row r="18" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
@@ -19374,7 +19486,7 @@
       </c>
       <c r="C18" s="24" t="str">
         <f>IF(AB8=0,"Winner R3",AB8)</f>
-        <v>Winner R3</v>
+        <v> Italy</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="49" t="s">
@@ -19383,7 +19495,7 @@
       <c r="F18" s="47"/>
       <c r="G18" s="25" t="str">
         <f>IF(AB9=0,"Winner R4",AB9)</f>
-        <v>Winner R4</v>
+        <v> Poland</v>
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="29" t="s">
@@ -19497,10 +19609,10 @@
         <f t="shared" ref="AT18:AT20" si="39">IF(D18&lt;F18,SUM(J18,M18,P18,S18,V18),SUM(H18,K18,N18,Q18,T18))</f>
         <v>0</v>
       </c>
-      <c r="AU18" s="65" t="s">
+      <c r="AU18" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="AV18" s="66"/>
+      <c r="AV18" s="68"/>
     </row>
     <row r="19" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23">
@@ -19508,7 +19620,7 @@
       </c>
       <c r="C19" s="24" t="str">
         <f>IF(AB10=0,"Winner R5",AB10)</f>
-        <v>Winner R5</v>
+        <v> Brazil</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="49" t="s">
@@ -19517,7 +19629,7 @@
       <c r="F19" s="47"/>
       <c r="G19" s="25" t="str">
         <f>IF(AB11=0,"Winner R6",AB11)</f>
-        <v>Winner R6</v>
+        <v> France</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="29" t="s">
@@ -19631,10 +19743,10 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AU19" s="65" t="s">
+      <c r="AU19" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="AV19" s="66"/>
+      <c r="AV19" s="68"/>
     </row>
     <row r="20" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23">
@@ -19642,7 +19754,7 @@
       </c>
       <c r="C20" s="24" t="str">
         <f>IF(AB12=0,"Winner R7",AB12)</f>
-        <v>Winner R7</v>
+        <v> United States</v>
       </c>
       <c r="D20" s="48"/>
       <c r="E20" s="49" t="s">
@@ -19651,7 +19763,7 @@
       <c r="F20" s="47"/>
       <c r="G20" s="25" t="str">
         <f>IF(AB13=0,"Winner R8",AB13)</f>
-        <v>Winner R8</v>
+        <v> Turkey</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="29" t="s">
@@ -19765,10 +19877,10 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AU20" s="67" t="s">
+      <c r="AU20" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="AV20" s="68"/>
+      <c r="AV20" s="70"/>
     </row>
     <row r="21" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -19804,42 +19916,42 @@
         <v>86</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="57" t="s">
+      <c r="H23" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="57" t="s">
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="57" t="s">
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="57" t="s">
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="R23" s="56"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="57" t="s">
+      <c r="R23" s="74"/>
+      <c r="S23" s="74"/>
+      <c r="T23" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="56"/>
+      <c r="U23" s="74"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="74"/>
+      <c r="Y23" s="74"/>
       <c r="AA23" s="12" t="s">
         <v>23</v>
       </c>
@@ -20211,42 +20323,42 @@
         <v>86</v>
       </c>
       <c r="C29" s="35"/>
-      <c r="D29" s="58" t="s">
+      <c r="D29" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
       <c r="G29" s="36"/>
-      <c r="H29" s="57" t="s">
+      <c r="H29" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="57" t="s">
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="57" t="s">
+      <c r="L29" s="74"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="57" t="s">
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="57" t="s">
+      <c r="R29" s="74"/>
+      <c r="S29" s="74"/>
+      <c r="T29" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="56"/>
-      <c r="Y29" s="56"/>
+      <c r="U29" s="74"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="74"/>
+      <c r="Y29" s="74"/>
       <c r="AA29" s="12" t="s">
         <v>23</v>
       </c>
@@ -20508,42 +20620,42 @@
         <v>86</v>
       </c>
       <c r="C34" s="35"/>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="57" t="s">
+      <c r="H34" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="57" t="s">
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="57" t="s">
+      <c r="L34" s="74"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="57" t="s">
+      <c r="O34" s="74"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="R34" s="56"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="57" t="s">
+      <c r="R34" s="74"/>
+      <c r="S34" s="74"/>
+      <c r="T34" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="X34" s="56"/>
-      <c r="Y34" s="56"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="X34" s="74"/>
+      <c r="Y34" s="74"/>
       <c r="AA34" s="12" t="s">
         <v>23</v>
       </c>
@@ -20861,22 +20973,22 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="48">
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="W34:Y34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="B2:AV2"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="W16:Y16"/>
+    <mergeCell ref="B22:Y22"/>
+    <mergeCell ref="B28:Y28"/>
+    <mergeCell ref="B15:Y15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T23:V23"/>
+    <mergeCell ref="W23:Y23"/>
+    <mergeCell ref="AU18:AV18"/>
+    <mergeCell ref="AU19:AV19"/>
+    <mergeCell ref="AU20:AV20"/>
     <mergeCell ref="B33:Y33"/>
     <mergeCell ref="AU15:AV15"/>
     <mergeCell ref="T29:V29"/>
@@ -20893,22 +21005,22 @@
     <mergeCell ref="Q29:S29"/>
     <mergeCell ref="AU16:AV16"/>
     <mergeCell ref="AU17:AV17"/>
-    <mergeCell ref="B2:AV2"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="W16:Y16"/>
-    <mergeCell ref="B22:Y22"/>
-    <mergeCell ref="B28:Y28"/>
-    <mergeCell ref="B15:Y15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="T23:V23"/>
-    <mergeCell ref="W23:Y23"/>
-    <mergeCell ref="AU18:AV18"/>
-    <mergeCell ref="AU19:AV19"/>
-    <mergeCell ref="AU20:AV20"/>
+    <mergeCell ref="W34:Y34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <conditionalFormatting sqref="BM18:XFD18 BM22:XFD23 BM20:XFD20 A18:A20 Z18:Z20 A41:A1048576 B53:Y1048576 B38:Y47 B37 D37:Y37 Z41:AT1048576 BM41:XFD1048576 A3:XFD3 BM6:XFD15 A4:A15 B4:XFD4 Z22:AT22 AA5:AT13 Z26:AT28 Z23:Z25 Z29:Z30 B36:AT36 Z34:Z35 BM25:XFD36 A22:A36 Z31:AT33 Z5:XFD5 B14:AT15 B21:Y22 B28:Y28 B33:Y33 Z6:Z13 AW24:BL1048576 AU21:AV1048576">
     <cfRule type="cellIs" dxfId="31" priority="79" operator="equal">
@@ -21083,6 +21195,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -21315,24 +21444,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1A4F3B6-8EF3-43FC-AA6E-56F4B11E76F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21349,29 +21486,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att Quarterfinals day 1 complete
</commit_message>
<xml_diff>
--- a/2025 FIVB Women's Volleyball World Championship.xlsx
+++ b/2025 FIVB Women's Volleyball World Championship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3FDF2D4-9AB6-4FA5-A737-AA5296B46BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C74E7559-C176-49CE-8522-E8DF5FE8FBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC01" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="2" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
@@ -863,28 +863,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -912,22 +906,28 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5393,11 +5393,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:X1"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A31:A34"/>
@@ -5406,6 +5401,11 @@
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A22"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:X1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5478,74 +5478,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:67" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="56"/>
-      <c r="AW2" s="56"/>
-      <c r="AX2" s="56"/>
-      <c r="AY2" s="56"/>
-      <c r="AZ2" s="56"/>
-      <c r="BA2" s="56"/>
-      <c r="BB2" s="56"/>
-      <c r="BC2" s="56"/>
-      <c r="BD2" s="56"/>
-      <c r="BE2" s="56"/>
-      <c r="BF2" s="56"/>
-      <c r="BG2" s="56"/>
-      <c r="BH2" s="56"/>
-      <c r="BI2" s="56"/>
-      <c r="BJ2" s="56"/>
-      <c r="BK2" s="56"/>
-      <c r="BL2" s="56"/>
-      <c r="BM2" s="56"/>
-      <c r="BN2" s="56"/>
-      <c r="BO2" s="56"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="75"/>
+      <c r="AW2" s="75"/>
+      <c r="AX2" s="75"/>
+      <c r="AY2" s="75"/>
+      <c r="AZ2" s="75"/>
+      <c r="BA2" s="75"/>
+      <c r="BB2" s="75"/>
+      <c r="BC2" s="75"/>
+      <c r="BD2" s="75"/>
+      <c r="BE2" s="75"/>
+      <c r="BF2" s="75"/>
+      <c r="BG2" s="75"/>
+      <c r="BH2" s="75"/>
+      <c r="BI2" s="75"/>
+      <c r="BJ2" s="75"/>
+      <c r="BK2" s="75"/>
+      <c r="BL2" s="75"/>
+      <c r="BM2" s="75"/>
+      <c r="BN2" s="75"/>
+      <c r="BO2" s="75"/>
     </row>
     <row r="3" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AX3" s="33"/>
@@ -5568,116 +5568,116 @@
       <c r="BO3" s="33"/>
     </row>
     <row r="4" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="57"/>
-      <c r="AO4" s="57"/>
-      <c r="AP4" s="57"/>
-      <c r="AQ4" s="57"/>
-      <c r="AR4" s="57"/>
-      <c r="AS4" s="57"/>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="57"/>
-      <c r="AV4" s="57"/>
-      <c r="AW4" s="57"/>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="57"/>
-      <c r="AZ4" s="57"/>
-      <c r="BA4" s="57"/>
-      <c r="BB4" s="57"/>
-      <c r="BC4" s="57"/>
-      <c r="BD4" s="57"/>
-      <c r="BE4" s="57"/>
-      <c r="BF4" s="57"/>
-      <c r="BG4" s="57"/>
-      <c r="BH4" s="57"/>
-      <c r="BI4" s="57"/>
-      <c r="BJ4" s="57"/>
-      <c r="BK4" s="57"/>
-      <c r="BL4" s="57"/>
-      <c r="BM4" s="57"/>
-      <c r="BN4" s="57"/>
-      <c r="BO4" s="57"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="76"/>
+      <c r="AU4" s="76"/>
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="76"/>
+      <c r="BB4" s="76"/>
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="76"/>
+      <c r="BF4" s="76"/>
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="76"/>
+      <c r="BI4" s="76"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="76"/>
+      <c r="BM4" s="76"/>
+      <c r="BN4" s="76"/>
+      <c r="BO4" s="76"/>
     </row>
     <row r="5" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75" t="s">
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="75" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="75" t="s">
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
       <c r="AD5" s="12" t="s">
         <v>23</v>
       </c>
@@ -5735,34 +5735,34 @@
       <c r="AW5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX5" s="61" t="s">
+      <c r="AX5" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="AY5" s="62"/>
-      <c r="AZ5" s="63"/>
-      <c r="BA5" s="61" t="s">
+      <c r="AY5" s="73"/>
+      <c r="AZ5" s="74"/>
+      <c r="BA5" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="BB5" s="62"/>
-      <c r="BC5" s="63"/>
-      <c r="BD5" s="61" t="s">
+      <c r="BB5" s="73"/>
+      <c r="BC5" s="74"/>
+      <c r="BD5" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="BE5" s="62"/>
-      <c r="BF5" s="62"/>
-      <c r="BG5" s="62"/>
-      <c r="BH5" s="62"/>
-      <c r="BI5" s="63"/>
-      <c r="BJ5" s="61" t="s">
+      <c r="BE5" s="73"/>
+      <c r="BF5" s="73"/>
+      <c r="BG5" s="73"/>
+      <c r="BH5" s="73"/>
+      <c r="BI5" s="74"/>
+      <c r="BJ5" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="BK5" s="62"/>
-      <c r="BL5" s="63"/>
-      <c r="BM5" s="61" t="s">
+      <c r="BK5" s="73"/>
+      <c r="BL5" s="74"/>
+      <c r="BM5" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="BN5" s="62"/>
-      <c r="BO5" s="63"/>
+      <c r="BN5" s="73"/>
+      <c r="BO5" s="74"/>
     </row>
     <row r="6" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B6" s="23">
@@ -7031,116 +7031,116 @@
       </c>
     </row>
     <row r="12" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="57"/>
-      <c r="AA12" s="57"/>
-      <c r="AB12" s="57"/>
-      <c r="AC12" s="57"/>
-      <c r="AD12" s="57"/>
-      <c r="AE12" s="57"/>
-      <c r="AF12" s="57"/>
-      <c r="AG12" s="57"/>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="57"/>
-      <c r="AJ12" s="57"/>
-      <c r="AK12" s="57"/>
-      <c r="AL12" s="57"/>
-      <c r="AM12" s="57"/>
-      <c r="AN12" s="57"/>
-      <c r="AO12" s="57"/>
-      <c r="AP12" s="57"/>
-      <c r="AQ12" s="57"/>
-      <c r="AR12" s="57"/>
-      <c r="AS12" s="57"/>
-      <c r="AT12" s="57"/>
-      <c r="AU12" s="57"/>
-      <c r="AV12" s="57"/>
-      <c r="AW12" s="57"/>
-      <c r="AX12" s="57"/>
-      <c r="AY12" s="57"/>
-      <c r="AZ12" s="57"/>
-      <c r="BA12" s="57"/>
-      <c r="BB12" s="57"/>
-      <c r="BC12" s="57"/>
-      <c r="BD12" s="57"/>
-      <c r="BE12" s="57"/>
-      <c r="BF12" s="57"/>
-      <c r="BG12" s="57"/>
-      <c r="BH12" s="57"/>
-      <c r="BI12" s="57"/>
-      <c r="BJ12" s="57"/>
-      <c r="BK12" s="57"/>
-      <c r="BL12" s="57"/>
-      <c r="BM12" s="57"/>
-      <c r="BN12" s="57"/>
-      <c r="BO12" s="57"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="76"/>
+      <c r="R12" s="76"/>
+      <c r="S12" s="76"/>
+      <c r="T12" s="76"/>
+      <c r="U12" s="76"/>
+      <c r="V12" s="76"/>
+      <c r="W12" s="76"/>
+      <c r="X12" s="76"/>
+      <c r="Y12" s="76"/>
+      <c r="Z12" s="76"/>
+      <c r="AA12" s="76"/>
+      <c r="AB12" s="76"/>
+      <c r="AC12" s="76"/>
+      <c r="AD12" s="76"/>
+      <c r="AE12" s="76"/>
+      <c r="AF12" s="76"/>
+      <c r="AG12" s="76"/>
+      <c r="AH12" s="76"/>
+      <c r="AI12" s="76"/>
+      <c r="AJ12" s="76"/>
+      <c r="AK12" s="76"/>
+      <c r="AL12" s="76"/>
+      <c r="AM12" s="76"/>
+      <c r="AN12" s="76"/>
+      <c r="AO12" s="76"/>
+      <c r="AP12" s="76"/>
+      <c r="AQ12" s="76"/>
+      <c r="AR12" s="76"/>
+      <c r="AS12" s="76"/>
+      <c r="AT12" s="76"/>
+      <c r="AU12" s="76"/>
+      <c r="AV12" s="76"/>
+      <c r="AW12" s="76"/>
+      <c r="AX12" s="76"/>
+      <c r="AY12" s="76"/>
+      <c r="AZ12" s="76"/>
+      <c r="BA12" s="76"/>
+      <c r="BB12" s="76"/>
+      <c r="BC12" s="76"/>
+      <c r="BD12" s="76"/>
+      <c r="BE12" s="76"/>
+      <c r="BF12" s="76"/>
+      <c r="BG12" s="76"/>
+      <c r="BH12" s="76"/>
+      <c r="BI12" s="76"/>
+      <c r="BJ12" s="76"/>
+      <c r="BK12" s="76"/>
+      <c r="BL12" s="76"/>
+      <c r="BM12" s="76"/>
+      <c r="BN12" s="76"/>
+      <c r="BO12" s="76"/>
     </row>
     <row r="13" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="21"/>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="72" t="s">
+      <c r="H13" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="72" t="s">
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="72" t="s">
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="72" t="s">
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R13" s="73"/>
-      <c r="S13" s="73"/>
-      <c r="T13" s="72" t="s">
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U13" s="73"/>
-      <c r="V13" s="73"/>
-      <c r="W13" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X13" s="73"/>
-      <c r="Y13" s="73"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="59"/>
       <c r="AD13" s="12" t="s">
         <v>23</v>
       </c>
@@ -7198,34 +7198,34 @@
       <c r="AW13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX13" s="58" t="s">
+      <c r="AX13" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY13" s="59"/>
-      <c r="AZ13" s="60"/>
-      <c r="BA13" s="58" t="s">
+      <c r="AY13" s="70"/>
+      <c r="AZ13" s="71"/>
+      <c r="BA13" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB13" s="59"/>
-      <c r="BC13" s="60"/>
-      <c r="BD13" s="58" t="s">
+      <c r="BB13" s="70"/>
+      <c r="BC13" s="71"/>
+      <c r="BD13" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE13" s="59"/>
-      <c r="BF13" s="59"/>
-      <c r="BG13" s="59"/>
-      <c r="BH13" s="59"/>
-      <c r="BI13" s="60"/>
-      <c r="BJ13" s="58" t="s">
+      <c r="BE13" s="70"/>
+      <c r="BF13" s="70"/>
+      <c r="BG13" s="70"/>
+      <c r="BH13" s="70"/>
+      <c r="BI13" s="71"/>
+      <c r="BJ13" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK13" s="59"/>
-      <c r="BL13" s="60"/>
-      <c r="BM13" s="58" t="s">
+      <c r="BK13" s="70"/>
+      <c r="BL13" s="71"/>
+      <c r="BM13" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN13" s="59"/>
-      <c r="BO13" s="60"/>
+      <c r="BN13" s="70"/>
+      <c r="BO13" s="71"/>
     </row>
     <row r="14" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -8478,116 +8478,116 @@
       </c>
     </row>
     <row r="20" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="57"/>
-      <c r="V20" s="57"/>
-      <c r="W20" s="57"/>
-      <c r="X20" s="57"/>
-      <c r="Y20" s="57"/>
-      <c r="Z20" s="57"/>
-      <c r="AA20" s="57"/>
-      <c r="AB20" s="57"/>
-      <c r="AC20" s="57"/>
-      <c r="AD20" s="57"/>
-      <c r="AE20" s="57"/>
-      <c r="AF20" s="57"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="57"/>
-      <c r="AK20" s="57"/>
-      <c r="AL20" s="57"/>
-      <c r="AM20" s="57"/>
-      <c r="AN20" s="57"/>
-      <c r="AO20" s="57"/>
-      <c r="AP20" s="57"/>
-      <c r="AQ20" s="57"/>
-      <c r="AR20" s="57"/>
-      <c r="AS20" s="57"/>
-      <c r="AT20" s="57"/>
-      <c r="AU20" s="57"/>
-      <c r="AV20" s="57"/>
-      <c r="AW20" s="57"/>
-      <c r="AX20" s="57"/>
-      <c r="AY20" s="57"/>
-      <c r="AZ20" s="57"/>
-      <c r="BA20" s="57"/>
-      <c r="BB20" s="57"/>
-      <c r="BC20" s="57"/>
-      <c r="BD20" s="57"/>
-      <c r="BE20" s="57"/>
-      <c r="BF20" s="57"/>
-      <c r="BG20" s="57"/>
-      <c r="BH20" s="57"/>
-      <c r="BI20" s="57"/>
-      <c r="BJ20" s="57"/>
-      <c r="BK20" s="57"/>
-      <c r="BL20" s="57"/>
-      <c r="BM20" s="57"/>
-      <c r="BN20" s="57"/>
-      <c r="BO20" s="57"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
+      <c r="P20" s="76"/>
+      <c r="Q20" s="76"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
+      <c r="T20" s="76"/>
+      <c r="U20" s="76"/>
+      <c r="V20" s="76"/>
+      <c r="W20" s="76"/>
+      <c r="X20" s="76"/>
+      <c r="Y20" s="76"/>
+      <c r="Z20" s="76"/>
+      <c r="AA20" s="76"/>
+      <c r="AB20" s="76"/>
+      <c r="AC20" s="76"/>
+      <c r="AD20" s="76"/>
+      <c r="AE20" s="76"/>
+      <c r="AF20" s="76"/>
+      <c r="AG20" s="76"/>
+      <c r="AH20" s="76"/>
+      <c r="AI20" s="76"/>
+      <c r="AJ20" s="76"/>
+      <c r="AK20" s="76"/>
+      <c r="AL20" s="76"/>
+      <c r="AM20" s="76"/>
+      <c r="AN20" s="76"/>
+      <c r="AO20" s="76"/>
+      <c r="AP20" s="76"/>
+      <c r="AQ20" s="76"/>
+      <c r="AR20" s="76"/>
+      <c r="AS20" s="76"/>
+      <c r="AT20" s="76"/>
+      <c r="AU20" s="76"/>
+      <c r="AV20" s="76"/>
+      <c r="AW20" s="76"/>
+      <c r="AX20" s="76"/>
+      <c r="AY20" s="76"/>
+      <c r="AZ20" s="76"/>
+      <c r="BA20" s="76"/>
+      <c r="BB20" s="76"/>
+      <c r="BC20" s="76"/>
+      <c r="BD20" s="76"/>
+      <c r="BE20" s="76"/>
+      <c r="BF20" s="76"/>
+      <c r="BG20" s="76"/>
+      <c r="BH20" s="76"/>
+      <c r="BI20" s="76"/>
+      <c r="BJ20" s="76"/>
+      <c r="BK20" s="76"/>
+      <c r="BL20" s="76"/>
+      <c r="BM20" s="76"/>
+      <c r="BN20" s="76"/>
+      <c r="BO20" s="76"/>
     </row>
     <row r="21" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="71" t="s">
+      <c r="D21" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="72" t="s">
+      <c r="H21" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="72" t="s">
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="72" t="s">
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O21" s="73"/>
-      <c r="P21" s="73"/>
-      <c r="Q21" s="72" t="s">
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R21" s="73"/>
-      <c r="S21" s="73"/>
-      <c r="T21" s="72" t="s">
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U21" s="73"/>
-      <c r="V21" s="73"/>
-      <c r="W21" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X21" s="73"/>
-      <c r="Y21" s="73"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="59"/>
+      <c r="Y21" s="59"/>
       <c r="AD21" s="12" t="s">
         <v>23</v>
       </c>
@@ -8645,34 +8645,34 @@
       <c r="AW21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX21" s="58" t="s">
+      <c r="AX21" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY21" s="59"/>
-      <c r="AZ21" s="60"/>
-      <c r="BA21" s="58" t="s">
+      <c r="AY21" s="70"/>
+      <c r="AZ21" s="71"/>
+      <c r="BA21" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB21" s="59"/>
-      <c r="BC21" s="60"/>
-      <c r="BD21" s="58" t="s">
+      <c r="BB21" s="70"/>
+      <c r="BC21" s="71"/>
+      <c r="BD21" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE21" s="59"/>
-      <c r="BF21" s="59"/>
-      <c r="BG21" s="59"/>
-      <c r="BH21" s="59"/>
-      <c r="BI21" s="60"/>
-      <c r="BJ21" s="58" t="s">
+      <c r="BE21" s="70"/>
+      <c r="BF21" s="70"/>
+      <c r="BG21" s="70"/>
+      <c r="BH21" s="70"/>
+      <c r="BI21" s="71"/>
+      <c r="BJ21" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK21" s="59"/>
-      <c r="BL21" s="60"/>
-      <c r="BM21" s="58" t="s">
+      <c r="BK21" s="70"/>
+      <c r="BL21" s="71"/>
+      <c r="BM21" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN21" s="59"/>
-      <c r="BO21" s="60"/>
+      <c r="BN21" s="70"/>
+      <c r="BO21" s="71"/>
     </row>
     <row r="22" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
@@ -9937,116 +9937,116 @@
       </c>
     </row>
     <row r="28" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
-      <c r="V28" s="57"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="57"/>
-      <c r="Y28" s="57"/>
-      <c r="Z28" s="57"/>
-      <c r="AA28" s="57"/>
-      <c r="AB28" s="57"/>
-      <c r="AC28" s="57"/>
-      <c r="AD28" s="57"/>
-      <c r="AE28" s="57"/>
-      <c r="AF28" s="57"/>
-      <c r="AG28" s="57"/>
-      <c r="AH28" s="57"/>
-      <c r="AI28" s="57"/>
-      <c r="AJ28" s="57"/>
-      <c r="AK28" s="57"/>
-      <c r="AL28" s="57"/>
-      <c r="AM28" s="57"/>
-      <c r="AN28" s="57"/>
-      <c r="AO28" s="57"/>
-      <c r="AP28" s="57"/>
-      <c r="AQ28" s="57"/>
-      <c r="AR28" s="57"/>
-      <c r="AS28" s="57"/>
-      <c r="AT28" s="57"/>
-      <c r="AU28" s="57"/>
-      <c r="AV28" s="57"/>
-      <c r="AW28" s="57"/>
-      <c r="AX28" s="57"/>
-      <c r="AY28" s="57"/>
-      <c r="AZ28" s="57"/>
-      <c r="BA28" s="57"/>
-      <c r="BB28" s="57"/>
-      <c r="BC28" s="57"/>
-      <c r="BD28" s="57"/>
-      <c r="BE28" s="57"/>
-      <c r="BF28" s="57"/>
-      <c r="BG28" s="57"/>
-      <c r="BH28" s="57"/>
-      <c r="BI28" s="57"/>
-      <c r="BJ28" s="57"/>
-      <c r="BK28" s="57"/>
-      <c r="BL28" s="57"/>
-      <c r="BM28" s="57"/>
-      <c r="BN28" s="57"/>
-      <c r="BO28" s="57"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="76"/>
+      <c r="P28" s="76"/>
+      <c r="Q28" s="76"/>
+      <c r="R28" s="76"/>
+      <c r="S28" s="76"/>
+      <c r="T28" s="76"/>
+      <c r="U28" s="76"/>
+      <c r="V28" s="76"/>
+      <c r="W28" s="76"/>
+      <c r="X28" s="76"/>
+      <c r="Y28" s="76"/>
+      <c r="Z28" s="76"/>
+      <c r="AA28" s="76"/>
+      <c r="AB28" s="76"/>
+      <c r="AC28" s="76"/>
+      <c r="AD28" s="76"/>
+      <c r="AE28" s="76"/>
+      <c r="AF28" s="76"/>
+      <c r="AG28" s="76"/>
+      <c r="AH28" s="76"/>
+      <c r="AI28" s="76"/>
+      <c r="AJ28" s="76"/>
+      <c r="AK28" s="76"/>
+      <c r="AL28" s="76"/>
+      <c r="AM28" s="76"/>
+      <c r="AN28" s="76"/>
+      <c r="AO28" s="76"/>
+      <c r="AP28" s="76"/>
+      <c r="AQ28" s="76"/>
+      <c r="AR28" s="76"/>
+      <c r="AS28" s="76"/>
+      <c r="AT28" s="76"/>
+      <c r="AU28" s="76"/>
+      <c r="AV28" s="76"/>
+      <c r="AW28" s="76"/>
+      <c r="AX28" s="76"/>
+      <c r="AY28" s="76"/>
+      <c r="AZ28" s="76"/>
+      <c r="BA28" s="76"/>
+      <c r="BB28" s="76"/>
+      <c r="BC28" s="76"/>
+      <c r="BD28" s="76"/>
+      <c r="BE28" s="76"/>
+      <c r="BF28" s="76"/>
+      <c r="BG28" s="76"/>
+      <c r="BH28" s="76"/>
+      <c r="BI28" s="76"/>
+      <c r="BJ28" s="76"/>
+      <c r="BK28" s="76"/>
+      <c r="BL28" s="76"/>
+      <c r="BM28" s="76"/>
+      <c r="BN28" s="76"/>
+      <c r="BO28" s="76"/>
     </row>
     <row r="29" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="21"/>
-      <c r="D29" s="71" t="s">
+      <c r="D29" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="72" t="s">
+      <c r="H29" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="72" t="s">
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="72" t="s">
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="72" t="s">
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="73"/>
-      <c r="S29" s="73"/>
-      <c r="T29" s="72" t="s">
+      <c r="R29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U29" s="73"/>
-      <c r="V29" s="73"/>
-      <c r="W29" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="73"/>
-      <c r="Y29" s="73"/>
+      <c r="U29" s="59"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="59"/>
+      <c r="Y29" s="59"/>
       <c r="AD29" s="12" t="s">
         <v>23</v>
       </c>
@@ -10104,34 +10104,34 @@
       <c r="AW29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX29" s="58" t="s">
+      <c r="AX29" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY29" s="59"/>
-      <c r="AZ29" s="60"/>
-      <c r="BA29" s="58" t="s">
+      <c r="AY29" s="70"/>
+      <c r="AZ29" s="71"/>
+      <c r="BA29" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB29" s="59"/>
-      <c r="BC29" s="60"/>
-      <c r="BD29" s="58" t="s">
+      <c r="BB29" s="70"/>
+      <c r="BC29" s="71"/>
+      <c r="BD29" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE29" s="59"/>
-      <c r="BF29" s="59"/>
-      <c r="BG29" s="59"/>
-      <c r="BH29" s="59"/>
-      <c r="BI29" s="60"/>
-      <c r="BJ29" s="58" t="s">
+      <c r="BE29" s="70"/>
+      <c r="BF29" s="70"/>
+      <c r="BG29" s="70"/>
+      <c r="BH29" s="70"/>
+      <c r="BI29" s="71"/>
+      <c r="BJ29" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK29" s="59"/>
-      <c r="BL29" s="60"/>
-      <c r="BM29" s="58" t="s">
+      <c r="BK29" s="70"/>
+      <c r="BL29" s="71"/>
+      <c r="BM29" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN29" s="59"/>
-      <c r="BO29" s="60"/>
+      <c r="BN29" s="70"/>
+      <c r="BO29" s="71"/>
     </row>
     <row r="30" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
@@ -11396,120 +11396,120 @@
       </c>
     </row>
     <row r="36" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
-      <c r="S36" s="57"/>
-      <c r="T36" s="57"/>
-      <c r="U36" s="57"/>
-      <c r="V36" s="57"/>
-      <c r="W36" s="57"/>
-      <c r="X36" s="57"/>
-      <c r="Y36" s="57"/>
-      <c r="Z36" s="57"/>
-      <c r="AA36" s="57"/>
-      <c r="AB36" s="57"/>
-      <c r="AC36" s="57"/>
-      <c r="AD36" s="57"/>
-      <c r="AE36" s="57"/>
-      <c r="AF36" s="57"/>
-      <c r="AG36" s="57"/>
-      <c r="AH36" s="57"/>
-      <c r="AI36" s="57"/>
-      <c r="AJ36" s="57"/>
-      <c r="AK36" s="57"/>
-      <c r="AL36" s="57"/>
-      <c r="AM36" s="57"/>
-      <c r="AN36" s="57"/>
-      <c r="AO36" s="57"/>
-      <c r="AP36" s="57"/>
-      <c r="AQ36" s="57"/>
-      <c r="AR36" s="57"/>
-      <c r="AS36" s="57"/>
-      <c r="AT36" s="57"/>
-      <c r="AU36" s="57"/>
-      <c r="AV36" s="57"/>
-      <c r="AW36" s="57"/>
-      <c r="AX36" s="57"/>
-      <c r="AY36" s="57"/>
-      <c r="AZ36" s="57"/>
-      <c r="BA36" s="57"/>
-      <c r="BB36" s="57"/>
-      <c r="BC36" s="57"/>
-      <c r="BD36" s="57"/>
-      <c r="BE36" s="57"/>
-      <c r="BF36" s="57"/>
-      <c r="BG36" s="57"/>
-      <c r="BH36" s="57"/>
-      <c r="BI36" s="57"/>
-      <c r="BJ36" s="57"/>
-      <c r="BK36" s="57"/>
-      <c r="BL36" s="57"/>
-      <c r="BM36" s="57"/>
-      <c r="BN36" s="57"/>
-      <c r="BO36" s="57"/>
-      <c r="BQ36" s="64" t="s">
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="76"/>
+      <c r="O36" s="76"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="76"/>
+      <c r="R36" s="76"/>
+      <c r="S36" s="76"/>
+      <c r="T36" s="76"/>
+      <c r="U36" s="76"/>
+      <c r="V36" s="76"/>
+      <c r="W36" s="76"/>
+      <c r="X36" s="76"/>
+      <c r="Y36" s="76"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="76"/>
+      <c r="AB36" s="76"/>
+      <c r="AC36" s="76"/>
+      <c r="AD36" s="76"/>
+      <c r="AE36" s="76"/>
+      <c r="AF36" s="76"/>
+      <c r="AG36" s="76"/>
+      <c r="AH36" s="76"/>
+      <c r="AI36" s="76"/>
+      <c r="AJ36" s="76"/>
+      <c r="AK36" s="76"/>
+      <c r="AL36" s="76"/>
+      <c r="AM36" s="76"/>
+      <c r="AN36" s="76"/>
+      <c r="AO36" s="76"/>
+      <c r="AP36" s="76"/>
+      <c r="AQ36" s="76"/>
+      <c r="AR36" s="76"/>
+      <c r="AS36" s="76"/>
+      <c r="AT36" s="76"/>
+      <c r="AU36" s="76"/>
+      <c r="AV36" s="76"/>
+      <c r="AW36" s="76"/>
+      <c r="AX36" s="76"/>
+      <c r="AY36" s="76"/>
+      <c r="AZ36" s="76"/>
+      <c r="BA36" s="76"/>
+      <c r="BB36" s="76"/>
+      <c r="BC36" s="76"/>
+      <c r="BD36" s="76"/>
+      <c r="BE36" s="76"/>
+      <c r="BF36" s="76"/>
+      <c r="BG36" s="76"/>
+      <c r="BH36" s="76"/>
+      <c r="BI36" s="76"/>
+      <c r="BJ36" s="76"/>
+      <c r="BK36" s="76"/>
+      <c r="BL36" s="76"/>
+      <c r="BM36" s="76"/>
+      <c r="BN36" s="76"/>
+      <c r="BO36" s="76"/>
+      <c r="BQ36" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="BR36" s="64"/>
+      <c r="BR36" s="62"/>
     </row>
     <row r="37" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="21"/>
-      <c r="D37" s="71" t="s">
+      <c r="D37" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="72" t="s">
+      <c r="H37" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="73"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="72" t="s">
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L37" s="73"/>
-      <c r="M37" s="73"/>
-      <c r="N37" s="72" t="s">
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O37" s="73"/>
-      <c r="P37" s="73"/>
-      <c r="Q37" s="72" t="s">
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R37" s="73"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="72" t="s">
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X37" s="73"/>
-      <c r="Y37" s="73"/>
+      <c r="U37" s="59"/>
+      <c r="V37" s="59"/>
+      <c r="W37" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
       <c r="AD37" s="12" t="s">
         <v>23</v>
       </c>
@@ -11567,38 +11567,38 @@
       <c r="AW37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX37" s="58" t="s">
+      <c r="AX37" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY37" s="59"/>
-      <c r="AZ37" s="60"/>
-      <c r="BA37" s="58" t="s">
+      <c r="AY37" s="70"/>
+      <c r="AZ37" s="71"/>
+      <c r="BA37" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB37" s="59"/>
-      <c r="BC37" s="60"/>
-      <c r="BD37" s="58" t="s">
+      <c r="BB37" s="70"/>
+      <c r="BC37" s="71"/>
+      <c r="BD37" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE37" s="59"/>
-      <c r="BF37" s="59"/>
-      <c r="BG37" s="59"/>
-      <c r="BH37" s="59"/>
-      <c r="BI37" s="60"/>
-      <c r="BJ37" s="58" t="s">
+      <c r="BE37" s="70"/>
+      <c r="BF37" s="70"/>
+      <c r="BG37" s="70"/>
+      <c r="BH37" s="70"/>
+      <c r="BI37" s="71"/>
+      <c r="BJ37" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK37" s="59"/>
-      <c r="BL37" s="60"/>
-      <c r="BM37" s="58" t="s">
+      <c r="BK37" s="70"/>
+      <c r="BL37" s="71"/>
+      <c r="BM37" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN37" s="59"/>
-      <c r="BO37" s="60"/>
-      <c r="BQ37" s="65" t="s">
+      <c r="BN37" s="70"/>
+      <c r="BO37" s="71"/>
+      <c r="BQ37" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="BR37" s="66"/>
+      <c r="BR37" s="64"/>
     </row>
     <row r="38" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B38" s="23">
@@ -11809,10 +11809,10 @@
       <c r="BO38" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="BQ38" s="67" t="s">
+      <c r="BQ38" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="BR38" s="68"/>
+      <c r="BR38" s="66"/>
     </row>
     <row r="39" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B39" s="23">
@@ -12036,10 +12036,10 @@
         <f>VLOOKUP($AX39,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>1297.1428571428571</v>
       </c>
-      <c r="BQ39" s="67" t="s">
+      <c r="BQ39" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="BR39" s="68"/>
+      <c r="BR39" s="66"/>
     </row>
     <row r="40" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B40" s="23">
@@ -12271,10 +12271,10 @@
         <f>VLOOKUP($AX40,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>1026.5151515151515</v>
       </c>
-      <c r="BQ40" s="67" t="s">
+      <c r="BQ40" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="BR40" s="68"/>
+      <c r="BR40" s="66"/>
     </row>
     <row r="41" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B41" s="23">
@@ -12498,10 +12498,10 @@
         <f>VLOOKUP($AX41,Dummy!$B$19:$S$22,18,FALSE)</f>
         <v>973.88059701492534</v>
       </c>
-      <c r="BQ41" s="69" t="s">
+      <c r="BQ41" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="BR41" s="70"/>
+      <c r="BR41" s="68"/>
     </row>
     <row r="42" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B42" s="23">
@@ -12875,116 +12875,116 @@
       </c>
     </row>
     <row r="44" spans="2:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
-      <c r="R44" s="57"/>
-      <c r="S44" s="57"/>
-      <c r="T44" s="57"/>
-      <c r="U44" s="57"/>
-      <c r="V44" s="57"/>
-      <c r="W44" s="57"/>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="57"/>
-      <c r="Z44" s="57"/>
-      <c r="AA44" s="57"/>
-      <c r="AB44" s="57"/>
-      <c r="AC44" s="57"/>
-      <c r="AD44" s="57"/>
-      <c r="AE44" s="57"/>
-      <c r="AF44" s="57"/>
-      <c r="AG44" s="57"/>
-      <c r="AH44" s="57"/>
-      <c r="AI44" s="57"/>
-      <c r="AJ44" s="57"/>
-      <c r="AK44" s="57"/>
-      <c r="AL44" s="57"/>
-      <c r="AM44" s="57"/>
-      <c r="AN44" s="57"/>
-      <c r="AO44" s="57"/>
-      <c r="AP44" s="57"/>
-      <c r="AQ44" s="57"/>
-      <c r="AR44" s="57"/>
-      <c r="AS44" s="57"/>
-      <c r="AT44" s="57"/>
-      <c r="AU44" s="57"/>
-      <c r="AV44" s="57"/>
-      <c r="AW44" s="57"/>
-      <c r="AX44" s="57"/>
-      <c r="AY44" s="57"/>
-      <c r="AZ44" s="57"/>
-      <c r="BA44" s="57"/>
-      <c r="BB44" s="57"/>
-      <c r="BC44" s="57"/>
-      <c r="BD44" s="57"/>
-      <c r="BE44" s="57"/>
-      <c r="BF44" s="57"/>
-      <c r="BG44" s="57"/>
-      <c r="BH44" s="57"/>
-      <c r="BI44" s="57"/>
-      <c r="BJ44" s="57"/>
-      <c r="BK44" s="57"/>
-      <c r="BL44" s="57"/>
-      <c r="BM44" s="57"/>
-      <c r="BN44" s="57"/>
-      <c r="BO44" s="57"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="76"/>
+      <c r="P44" s="76"/>
+      <c r="Q44" s="76"/>
+      <c r="R44" s="76"/>
+      <c r="S44" s="76"/>
+      <c r="T44" s="76"/>
+      <c r="U44" s="76"/>
+      <c r="V44" s="76"/>
+      <c r="W44" s="76"/>
+      <c r="X44" s="76"/>
+      <c r="Y44" s="76"/>
+      <c r="Z44" s="76"/>
+      <c r="AA44" s="76"/>
+      <c r="AB44" s="76"/>
+      <c r="AC44" s="76"/>
+      <c r="AD44" s="76"/>
+      <c r="AE44" s="76"/>
+      <c r="AF44" s="76"/>
+      <c r="AG44" s="76"/>
+      <c r="AH44" s="76"/>
+      <c r="AI44" s="76"/>
+      <c r="AJ44" s="76"/>
+      <c r="AK44" s="76"/>
+      <c r="AL44" s="76"/>
+      <c r="AM44" s="76"/>
+      <c r="AN44" s="76"/>
+      <c r="AO44" s="76"/>
+      <c r="AP44" s="76"/>
+      <c r="AQ44" s="76"/>
+      <c r="AR44" s="76"/>
+      <c r="AS44" s="76"/>
+      <c r="AT44" s="76"/>
+      <c r="AU44" s="76"/>
+      <c r="AV44" s="76"/>
+      <c r="AW44" s="76"/>
+      <c r="AX44" s="76"/>
+      <c r="AY44" s="76"/>
+      <c r="AZ44" s="76"/>
+      <c r="BA44" s="76"/>
+      <c r="BB44" s="76"/>
+      <c r="BC44" s="76"/>
+      <c r="BD44" s="76"/>
+      <c r="BE44" s="76"/>
+      <c r="BF44" s="76"/>
+      <c r="BG44" s="76"/>
+      <c r="BH44" s="76"/>
+      <c r="BI44" s="76"/>
+      <c r="BJ44" s="76"/>
+      <c r="BK44" s="76"/>
+      <c r="BL44" s="76"/>
+      <c r="BM44" s="76"/>
+      <c r="BN44" s="76"/>
+      <c r="BO44" s="76"/>
     </row>
     <row r="45" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B45" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C45" s="21"/>
-      <c r="D45" s="71" t="s">
+      <c r="D45" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="71"/>
-      <c r="F45" s="71"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
       <c r="G45" s="22"/>
-      <c r="H45" s="72" t="s">
+      <c r="H45" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="72" t="s">
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L45" s="73"/>
-      <c r="M45" s="73"/>
-      <c r="N45" s="72" t="s">
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O45" s="73"/>
-      <c r="P45" s="73"/>
-      <c r="Q45" s="72" t="s">
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73"/>
-      <c r="T45" s="72" t="s">
+      <c r="R45" s="59"/>
+      <c r="S45" s="59"/>
+      <c r="T45" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U45" s="73"/>
-      <c r="V45" s="73"/>
-      <c r="W45" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X45" s="73"/>
-      <c r="Y45" s="73"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="59"/>
+      <c r="W45" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
       <c r="AD45" s="12" t="s">
         <v>23</v>
       </c>
@@ -13042,34 +13042,34 @@
       <c r="AW45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX45" s="58" t="s">
+      <c r="AX45" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY45" s="59"/>
-      <c r="AZ45" s="60"/>
-      <c r="BA45" s="58" t="s">
+      <c r="AY45" s="70"/>
+      <c r="AZ45" s="71"/>
+      <c r="BA45" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB45" s="59"/>
-      <c r="BC45" s="60"/>
-      <c r="BD45" s="58" t="s">
+      <c r="BB45" s="70"/>
+      <c r="BC45" s="71"/>
+      <c r="BD45" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE45" s="59"/>
-      <c r="BF45" s="59"/>
-      <c r="BG45" s="59"/>
-      <c r="BH45" s="59"/>
-      <c r="BI45" s="60"/>
-      <c r="BJ45" s="58" t="s">
+      <c r="BE45" s="70"/>
+      <c r="BF45" s="70"/>
+      <c r="BG45" s="70"/>
+      <c r="BH45" s="70"/>
+      <c r="BI45" s="71"/>
+      <c r="BJ45" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK45" s="59"/>
-      <c r="BL45" s="60"/>
-      <c r="BM45" s="58" t="s">
+      <c r="BK45" s="70"/>
+      <c r="BL45" s="71"/>
+      <c r="BM45" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN45" s="59"/>
-      <c r="BO45" s="60"/>
+      <c r="BN45" s="70"/>
+      <c r="BO45" s="71"/>
     </row>
     <row r="46" spans="2:70" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
@@ -14330,116 +14330,116 @@
       </c>
     </row>
     <row r="52" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="57"/>
-      <c r="Q52" s="57"/>
-      <c r="R52" s="57"/>
-      <c r="S52" s="57"/>
-      <c r="T52" s="57"/>
-      <c r="U52" s="57"/>
-      <c r="V52" s="57"/>
-      <c r="W52" s="57"/>
-      <c r="X52" s="57"/>
-      <c r="Y52" s="57"/>
-      <c r="Z52" s="57"/>
-      <c r="AA52" s="57"/>
-      <c r="AB52" s="57"/>
-      <c r="AC52" s="57"/>
-      <c r="AD52" s="57"/>
-      <c r="AE52" s="57"/>
-      <c r="AF52" s="57"/>
-      <c r="AG52" s="57"/>
-      <c r="AH52" s="57"/>
-      <c r="AI52" s="57"/>
-      <c r="AJ52" s="57"/>
-      <c r="AK52" s="57"/>
-      <c r="AL52" s="57"/>
-      <c r="AM52" s="57"/>
-      <c r="AN52" s="57"/>
-      <c r="AO52" s="57"/>
-      <c r="AP52" s="57"/>
-      <c r="AQ52" s="57"/>
-      <c r="AR52" s="57"/>
-      <c r="AS52" s="57"/>
-      <c r="AT52" s="57"/>
-      <c r="AU52" s="57"/>
-      <c r="AV52" s="57"/>
-      <c r="AW52" s="57"/>
-      <c r="AX52" s="57"/>
-      <c r="AY52" s="57"/>
-      <c r="AZ52" s="57"/>
-      <c r="BA52" s="57"/>
-      <c r="BB52" s="57"/>
-      <c r="BC52" s="57"/>
-      <c r="BD52" s="57"/>
-      <c r="BE52" s="57"/>
-      <c r="BF52" s="57"/>
-      <c r="BG52" s="57"/>
-      <c r="BH52" s="57"/>
-      <c r="BI52" s="57"/>
-      <c r="BJ52" s="57"/>
-      <c r="BK52" s="57"/>
-      <c r="BL52" s="57"/>
-      <c r="BM52" s="57"/>
-      <c r="BN52" s="57"/>
-      <c r="BO52" s="57"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="76"/>
+      <c r="M52" s="76"/>
+      <c r="N52" s="76"/>
+      <c r="O52" s="76"/>
+      <c r="P52" s="76"/>
+      <c r="Q52" s="76"/>
+      <c r="R52" s="76"/>
+      <c r="S52" s="76"/>
+      <c r="T52" s="76"/>
+      <c r="U52" s="76"/>
+      <c r="V52" s="76"/>
+      <c r="W52" s="76"/>
+      <c r="X52" s="76"/>
+      <c r="Y52" s="76"/>
+      <c r="Z52" s="76"/>
+      <c r="AA52" s="76"/>
+      <c r="AB52" s="76"/>
+      <c r="AC52" s="76"/>
+      <c r="AD52" s="76"/>
+      <c r="AE52" s="76"/>
+      <c r="AF52" s="76"/>
+      <c r="AG52" s="76"/>
+      <c r="AH52" s="76"/>
+      <c r="AI52" s="76"/>
+      <c r="AJ52" s="76"/>
+      <c r="AK52" s="76"/>
+      <c r="AL52" s="76"/>
+      <c r="AM52" s="76"/>
+      <c r="AN52" s="76"/>
+      <c r="AO52" s="76"/>
+      <c r="AP52" s="76"/>
+      <c r="AQ52" s="76"/>
+      <c r="AR52" s="76"/>
+      <c r="AS52" s="76"/>
+      <c r="AT52" s="76"/>
+      <c r="AU52" s="76"/>
+      <c r="AV52" s="76"/>
+      <c r="AW52" s="76"/>
+      <c r="AX52" s="76"/>
+      <c r="AY52" s="76"/>
+      <c r="AZ52" s="76"/>
+      <c r="BA52" s="76"/>
+      <c r="BB52" s="76"/>
+      <c r="BC52" s="76"/>
+      <c r="BD52" s="76"/>
+      <c r="BE52" s="76"/>
+      <c r="BF52" s="76"/>
+      <c r="BG52" s="76"/>
+      <c r="BH52" s="76"/>
+      <c r="BI52" s="76"/>
+      <c r="BJ52" s="76"/>
+      <c r="BK52" s="76"/>
+      <c r="BL52" s="76"/>
+      <c r="BM52" s="76"/>
+      <c r="BN52" s="76"/>
+      <c r="BO52" s="76"/>
     </row>
     <row r="53" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B53" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="71" t="s">
+      <c r="D53" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E53" s="71"/>
-      <c r="F53" s="71"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
       <c r="G53" s="22"/>
-      <c r="H53" s="72" t="s">
+      <c r="H53" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I53" s="73"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="72" t="s">
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L53" s="73"/>
-      <c r="M53" s="73"/>
-      <c r="N53" s="72" t="s">
+      <c r="L53" s="59"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O53" s="73"/>
-      <c r="P53" s="73"/>
-      <c r="Q53" s="72" t="s">
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R53" s="73"/>
-      <c r="S53" s="73"/>
-      <c r="T53" s="72" t="s">
+      <c r="R53" s="59"/>
+      <c r="S53" s="59"/>
+      <c r="T53" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U53" s="73"/>
-      <c r="V53" s="73"/>
-      <c r="W53" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X53" s="73"/>
-      <c r="Y53" s="73"/>
+      <c r="U53" s="59"/>
+      <c r="V53" s="59"/>
+      <c r="W53" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X53" s="59"/>
+      <c r="Y53" s="59"/>
       <c r="AD53" s="12" t="s">
         <v>23</v>
       </c>
@@ -14497,34 +14497,34 @@
       <c r="AW53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX53" s="58" t="s">
+      <c r="AX53" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY53" s="59"/>
-      <c r="AZ53" s="60"/>
-      <c r="BA53" s="58" t="s">
+      <c r="AY53" s="70"/>
+      <c r="AZ53" s="71"/>
+      <c r="BA53" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB53" s="59"/>
-      <c r="BC53" s="60"/>
-      <c r="BD53" s="58" t="s">
+      <c r="BB53" s="70"/>
+      <c r="BC53" s="71"/>
+      <c r="BD53" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE53" s="59"/>
-      <c r="BF53" s="59"/>
-      <c r="BG53" s="59"/>
-      <c r="BH53" s="59"/>
-      <c r="BI53" s="60"/>
-      <c r="BJ53" s="58" t="s">
+      <c r="BE53" s="70"/>
+      <c r="BF53" s="70"/>
+      <c r="BG53" s="70"/>
+      <c r="BH53" s="70"/>
+      <c r="BI53" s="71"/>
+      <c r="BJ53" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK53" s="59"/>
-      <c r="BL53" s="60"/>
-      <c r="BM53" s="58" t="s">
+      <c r="BK53" s="70"/>
+      <c r="BL53" s="71"/>
+      <c r="BM53" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN53" s="59"/>
-      <c r="BO53" s="60"/>
+      <c r="BN53" s="70"/>
+      <c r="BO53" s="71"/>
     </row>
     <row r="54" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B54" s="23">
@@ -15785,116 +15785,116 @@
       </c>
     </row>
     <row r="60" spans="2:67" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="57" t="s">
+      <c r="B60" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="57"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="57"/>
-      <c r="R60" s="57"/>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
-      <c r="U60" s="57"/>
-      <c r="V60" s="57"/>
-      <c r="W60" s="57"/>
-      <c r="X60" s="57"/>
-      <c r="Y60" s="57"/>
-      <c r="Z60" s="57"/>
-      <c r="AA60" s="57"/>
-      <c r="AB60" s="57"/>
-      <c r="AC60" s="57"/>
-      <c r="AD60" s="57"/>
-      <c r="AE60" s="57"/>
-      <c r="AF60" s="57"/>
-      <c r="AG60" s="57"/>
-      <c r="AH60" s="57"/>
-      <c r="AI60" s="57"/>
-      <c r="AJ60" s="57"/>
-      <c r="AK60" s="57"/>
-      <c r="AL60" s="57"/>
-      <c r="AM60" s="57"/>
-      <c r="AN60" s="57"/>
-      <c r="AO60" s="57"/>
-      <c r="AP60" s="57"/>
-      <c r="AQ60" s="57"/>
-      <c r="AR60" s="57"/>
-      <c r="AS60" s="57"/>
-      <c r="AT60" s="57"/>
-      <c r="AU60" s="57"/>
-      <c r="AV60" s="57"/>
-      <c r="AW60" s="57"/>
-      <c r="AX60" s="57"/>
-      <c r="AY60" s="57"/>
-      <c r="AZ60" s="57"/>
-      <c r="BA60" s="57"/>
-      <c r="BB60" s="57"/>
-      <c r="BC60" s="57"/>
-      <c r="BD60" s="57"/>
-      <c r="BE60" s="57"/>
-      <c r="BF60" s="57"/>
-      <c r="BG60" s="57"/>
-      <c r="BH60" s="57"/>
-      <c r="BI60" s="57"/>
-      <c r="BJ60" s="57"/>
-      <c r="BK60" s="57"/>
-      <c r="BL60" s="57"/>
-      <c r="BM60" s="57"/>
-      <c r="BN60" s="57"/>
-      <c r="BO60" s="57"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="76"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="76"/>
+      <c r="O60" s="76"/>
+      <c r="P60" s="76"/>
+      <c r="Q60" s="76"/>
+      <c r="R60" s="76"/>
+      <c r="S60" s="76"/>
+      <c r="T60" s="76"/>
+      <c r="U60" s="76"/>
+      <c r="V60" s="76"/>
+      <c r="W60" s="76"/>
+      <c r="X60" s="76"/>
+      <c r="Y60" s="76"/>
+      <c r="Z60" s="76"/>
+      <c r="AA60" s="76"/>
+      <c r="AB60" s="76"/>
+      <c r="AC60" s="76"/>
+      <c r="AD60" s="76"/>
+      <c r="AE60" s="76"/>
+      <c r="AF60" s="76"/>
+      <c r="AG60" s="76"/>
+      <c r="AH60" s="76"/>
+      <c r="AI60" s="76"/>
+      <c r="AJ60" s="76"/>
+      <c r="AK60" s="76"/>
+      <c r="AL60" s="76"/>
+      <c r="AM60" s="76"/>
+      <c r="AN60" s="76"/>
+      <c r="AO60" s="76"/>
+      <c r="AP60" s="76"/>
+      <c r="AQ60" s="76"/>
+      <c r="AR60" s="76"/>
+      <c r="AS60" s="76"/>
+      <c r="AT60" s="76"/>
+      <c r="AU60" s="76"/>
+      <c r="AV60" s="76"/>
+      <c r="AW60" s="76"/>
+      <c r="AX60" s="76"/>
+      <c r="AY60" s="76"/>
+      <c r="AZ60" s="76"/>
+      <c r="BA60" s="76"/>
+      <c r="BB60" s="76"/>
+      <c r="BC60" s="76"/>
+      <c r="BD60" s="76"/>
+      <c r="BE60" s="76"/>
+      <c r="BF60" s="76"/>
+      <c r="BG60" s="76"/>
+      <c r="BH60" s="76"/>
+      <c r="BI60" s="76"/>
+      <c r="BJ60" s="76"/>
+      <c r="BK60" s="76"/>
+      <c r="BL60" s="76"/>
+      <c r="BM60" s="76"/>
+      <c r="BN60" s="76"/>
+      <c r="BO60" s="76"/>
     </row>
     <row r="61" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B61" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C61" s="21"/>
-      <c r="D61" s="71" t="s">
+      <c r="D61" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E61" s="71"/>
-      <c r="F61" s="71"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="72" t="s">
+      <c r="H61" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="I61" s="73"/>
-      <c r="J61" s="73"/>
-      <c r="K61" s="72" t="s">
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L61" s="73"/>
-      <c r="M61" s="73"/>
-      <c r="N61" s="72" t="s">
+      <c r="L61" s="59"/>
+      <c r="M61" s="59"/>
+      <c r="N61" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="O61" s="73"/>
-      <c r="P61" s="73"/>
-      <c r="Q61" s="72" t="s">
+      <c r="O61" s="59"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="R61" s="73"/>
-      <c r="S61" s="73"/>
-      <c r="T61" s="72" t="s">
+      <c r="R61" s="59"/>
+      <c r="S61" s="59"/>
+      <c r="T61" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="U61" s="73"/>
-      <c r="V61" s="73"/>
-      <c r="W61" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="X61" s="73"/>
-      <c r="Y61" s="73"/>
+      <c r="U61" s="59"/>
+      <c r="V61" s="59"/>
+      <c r="W61" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="X61" s="59"/>
+      <c r="Y61" s="59"/>
       <c r="AD61" s="12" t="s">
         <v>23</v>
       </c>
@@ -15952,34 +15952,34 @@
       <c r="AW61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AX61" s="58" t="s">
+      <c r="AX61" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="AY61" s="59"/>
-      <c r="AZ61" s="60"/>
-      <c r="BA61" s="58" t="s">
+      <c r="AY61" s="70"/>
+      <c r="AZ61" s="71"/>
+      <c r="BA61" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="BB61" s="59"/>
-      <c r="BC61" s="60"/>
-      <c r="BD61" s="58" t="s">
+      <c r="BB61" s="70"/>
+      <c r="BC61" s="71"/>
+      <c r="BD61" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="BE61" s="59"/>
-      <c r="BF61" s="59"/>
-      <c r="BG61" s="59"/>
-      <c r="BH61" s="59"/>
-      <c r="BI61" s="60"/>
-      <c r="BJ61" s="58" t="s">
+      <c r="BE61" s="70"/>
+      <c r="BF61" s="70"/>
+      <c r="BG61" s="70"/>
+      <c r="BH61" s="70"/>
+      <c r="BI61" s="71"/>
+      <c r="BJ61" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BK61" s="59"/>
-      <c r="BL61" s="60"/>
-      <c r="BM61" s="58" t="s">
+      <c r="BK61" s="70"/>
+      <c r="BL61" s="71"/>
+      <c r="BM61" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="BN61" s="59"/>
-      <c r="BO61" s="60"/>
+      <c r="BN61" s="70"/>
+      <c r="BO61" s="71"/>
     </row>
     <row r="62" spans="2:67" x14ac:dyDescent="0.25">
       <c r="B62" s="11">
@@ -17238,93 +17238,6 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="111">
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:S21"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:Y21"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="Q37:S37"/>
-    <mergeCell ref="T37:V37"/>
-    <mergeCell ref="W37:Y37"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="T61:V61"/>
-    <mergeCell ref="W61:Y61"/>
-    <mergeCell ref="W45:Y45"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="T53:V53"/>
-    <mergeCell ref="W53:Y53"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="K45:M45"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="Q45:S45"/>
-    <mergeCell ref="T45:V45"/>
-    <mergeCell ref="BQ36:BR36"/>
-    <mergeCell ref="BQ37:BR37"/>
-    <mergeCell ref="BQ38:BR38"/>
-    <mergeCell ref="BQ39:BR39"/>
-    <mergeCell ref="BQ40:BR40"/>
-    <mergeCell ref="BQ41:BR41"/>
-    <mergeCell ref="AX29:AZ29"/>
-    <mergeCell ref="BA29:BC29"/>
-    <mergeCell ref="BD29:BI29"/>
-    <mergeCell ref="BJ29:BL29"/>
-    <mergeCell ref="BM29:BO29"/>
-    <mergeCell ref="AX37:AZ37"/>
-    <mergeCell ref="BA37:BC37"/>
-    <mergeCell ref="BD37:BI37"/>
-    <mergeCell ref="BJ37:BL37"/>
-    <mergeCell ref="BM37:BO37"/>
-    <mergeCell ref="BJ21:BL21"/>
-    <mergeCell ref="BM21:BO21"/>
-    <mergeCell ref="AX61:AZ61"/>
-    <mergeCell ref="BA61:BC61"/>
-    <mergeCell ref="BD61:BI61"/>
-    <mergeCell ref="BJ61:BL61"/>
-    <mergeCell ref="BM61:BO61"/>
-    <mergeCell ref="AX45:AZ45"/>
-    <mergeCell ref="BA5:BC5"/>
-    <mergeCell ref="BD5:BI5"/>
-    <mergeCell ref="BJ5:BL5"/>
-    <mergeCell ref="BM5:BO5"/>
-    <mergeCell ref="AX5:AZ5"/>
-    <mergeCell ref="BA13:BC13"/>
-    <mergeCell ref="BD13:BI13"/>
     <mergeCell ref="B2:BO2"/>
     <mergeCell ref="B4:BO4"/>
     <mergeCell ref="B12:BO12"/>
@@ -17349,6 +17262,93 @@
     <mergeCell ref="AX21:AZ21"/>
     <mergeCell ref="BA21:BC21"/>
     <mergeCell ref="BD21:BI21"/>
+    <mergeCell ref="BJ21:BL21"/>
+    <mergeCell ref="BM21:BO21"/>
+    <mergeCell ref="AX61:AZ61"/>
+    <mergeCell ref="BA61:BC61"/>
+    <mergeCell ref="BD61:BI61"/>
+    <mergeCell ref="BJ61:BL61"/>
+    <mergeCell ref="BM61:BO61"/>
+    <mergeCell ref="AX45:AZ45"/>
+    <mergeCell ref="BA5:BC5"/>
+    <mergeCell ref="BD5:BI5"/>
+    <mergeCell ref="BJ5:BL5"/>
+    <mergeCell ref="BM5:BO5"/>
+    <mergeCell ref="AX5:AZ5"/>
+    <mergeCell ref="BA13:BC13"/>
+    <mergeCell ref="BD13:BI13"/>
+    <mergeCell ref="BQ36:BR36"/>
+    <mergeCell ref="BQ37:BR37"/>
+    <mergeCell ref="BQ38:BR38"/>
+    <mergeCell ref="BQ39:BR39"/>
+    <mergeCell ref="BQ40:BR40"/>
+    <mergeCell ref="BQ41:BR41"/>
+    <mergeCell ref="AX29:AZ29"/>
+    <mergeCell ref="BA29:BC29"/>
+    <mergeCell ref="BD29:BI29"/>
+    <mergeCell ref="BJ29:BL29"/>
+    <mergeCell ref="BM29:BO29"/>
+    <mergeCell ref="AX37:AZ37"/>
+    <mergeCell ref="BA37:BC37"/>
+    <mergeCell ref="BD37:BI37"/>
+    <mergeCell ref="BJ37:BL37"/>
+    <mergeCell ref="BM37:BO37"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="T61:V61"/>
+    <mergeCell ref="W61:Y61"/>
+    <mergeCell ref="W45:Y45"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="T53:V53"/>
+    <mergeCell ref="W53:Y53"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="K45:M45"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="T45:V45"/>
+    <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="T37:V37"/>
+    <mergeCell ref="W37:Y37"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:Y21"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T13:V13"/>
   </mergeCells>
   <conditionalFormatting sqref="T6:V11 T22:V27 T54:V59">
     <cfRule type="expression" dxfId="95" priority="472">
@@ -17687,7 +17687,7 @@
   <dimension ref="B1:BO48"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17756,55 +17756,55 @@
       <c r="Y1" s="18"/>
     </row>
     <row r="2" spans="2:67" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="56"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
+      <c r="AQ2" s="75"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
+      <c r="AT2" s="75"/>
+      <c r="AU2" s="75"/>
+      <c r="AV2" s="75"/>
       <c r="AW2" s="46"/>
       <c r="AX2" s="46"/>
       <c r="AY2" s="46"/>
@@ -17858,42 +17858,42 @@
         <v>86</v>
       </c>
       <c r="C5" s="35"/>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75" t="s">
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75" t="s">
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="75" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="74"/>
-      <c r="S5" s="74"/>
-      <c r="T5" s="75" t="s">
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="56"/>
       <c r="AA5" s="12" t="s">
         <v>23</v>
       </c>
@@ -19238,52 +19238,52 @@
       <c r="W15" s="77"/>
       <c r="X15" s="77"/>
       <c r="Y15" s="77"/>
-      <c r="AU15" s="64" t="s">
+      <c r="AU15" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="AV15" s="64"/>
+      <c r="AV15" s="62"/>
     </row>
     <row r="16" spans="2:67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
       <c r="G16" s="36"/>
-      <c r="H16" s="75" t="s">
+      <c r="H16" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="75" t="s">
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="75" t="s">
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="75" t="s">
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R16" s="74"/>
-      <c r="S16" s="74"/>
-      <c r="T16" s="75" t="s">
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U16" s="74"/>
-      <c r="V16" s="74"/>
-      <c r="W16" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X16" s="74"/>
-      <c r="Y16" s="74"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="56"/>
       <c r="AA16" s="12" t="s">
         <v>23</v>
       </c>
@@ -19341,10 +19341,10 @@
       <c r="AT16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AU16" s="65" t="s">
+      <c r="AU16" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AV16" s="66"/>
+      <c r="AV16" s="64"/>
     </row>
     <row r="17" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23">
@@ -19354,70 +19354,94 @@
         <f>IF(AB6=0,"Winner R1",AB6)</f>
         <v> Netherlands</v>
       </c>
-      <c r="D17" s="48"/>
+      <c r="D17" s="48">
+        <v>2</v>
+      </c>
       <c r="E17" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="47"/>
+      <c r="F17" s="47">
+        <v>3</v>
+      </c>
       <c r="G17" s="25" t="str">
         <f>IF(AB7=0,"Winner R2",AB7)</f>
         <v> Japan</v>
       </c>
-      <c r="H17" s="28"/>
+      <c r="H17" s="28">
+        <v>25</v>
+      </c>
       <c r="I17" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="28"/>
+      <c r="J17" s="30">
+        <v>20</v>
+      </c>
+      <c r="K17" s="28">
+        <v>20</v>
+      </c>
       <c r="L17" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M17" s="30"/>
-      <c r="N17" s="28"/>
+      <c r="M17" s="30">
+        <v>25</v>
+      </c>
+      <c r="N17" s="28">
+        <v>25</v>
+      </c>
       <c r="O17" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="28"/>
+      <c r="P17" s="30">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="28">
+        <v>22</v>
+      </c>
       <c r="R17" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S17" s="30"/>
-      <c r="T17" s="28"/>
+      <c r="S17" s="30">
+        <v>25</v>
+      </c>
+      <c r="T17" s="28">
+        <v>12</v>
+      </c>
       <c r="U17" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="V17" s="30"/>
+      <c r="V17" s="30">
+        <v>15</v>
+      </c>
       <c r="W17" s="31">
         <f>SUM(H17,K17,N17,Q17,T17)</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="X17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y17" s="32">
         <f>SUM(J17,M17,P17,S17,V17)</f>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="AA17" s="12">
         <f>AD17+AE17</f>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="12">
+        <v>5</v>
+      </c>
+      <c r="AB17" s="12" t="str">
         <f>IF(OR(D17="",F17=""),0,IF(D17&gt;F17,C17,G17))</f>
-        <v>0</v>
+        <v> Japan</v>
       </c>
       <c r="AC17" s="12">
         <f>IF(OR(D17="",F17=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD17" s="12">
         <f>IF(OR(D17="",F17=""),0,IF(D17&gt;F17,D17,F17))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE17" s="12">
         <f>IF(OR(D17="",F17=""),0,IF(D17&gt;F17,F17,D17))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF17" s="12">
         <f>IF(AND(AD17=3,AE17=0),1,0)</f>
@@ -19429,35 +19453,35 @@
       </c>
       <c r="AH17" s="12">
         <f>IF(AND(AD17=3,AE17=2),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" s="12">
         <f>IF(D17&gt;F17,SUM(H17,K17,N17,Q17,T17,),SUM(J17,M17,P17,S17,V17))</f>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="AJ17" s="12">
         <f>IF(D17&gt;F17,SUM(J17,M17,P17,S17,V17),SUM(H17,K17,N17,Q17,T17))</f>
-        <v>0</v>
-      </c>
-      <c r="AL17" s="12">
+        <v>104</v>
+      </c>
+      <c r="AL17" s="12" t="str">
         <f>IF(OR(D17="",F17=""),0,IF(D17&lt;F17,C17,G17))</f>
-        <v>0</v>
+        <v> Netherlands</v>
       </c>
       <c r="AM17" s="12">
         <f>IF(OR(D17="",F17=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN17" s="12">
         <f>IF(OR(D17="",F17=""),0,IF(D17&lt;F17,D17,F17))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO17" s="12">
         <f>IF(OR(D17="",F17=""),0,IF(D17&lt;F17,F17,D17))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP17" s="12">
         <f>IF(AND(AN17=2,AO17=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ17" s="12">
         <f>IF(AND(AN17=1,AO17=3),1,0)</f>
@@ -19469,16 +19493,16 @@
       </c>
       <c r="AS17" s="12">
         <f>IF(D17&lt;F17,SUM(H17,K17,N17,Q17,T17,),SUM(J17,M17,P17,S17,V17))</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="AT17" s="12">
         <f>IF(D17&lt;F17,SUM(J17,M17,P17,S17,V17),SUM(H17,K17,N17,Q17,T17))</f>
-        <v>0</v>
-      </c>
-      <c r="AU17" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU17" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="AV17" s="68"/>
+      <c r="AV17" s="66"/>
     </row>
     <row r="18" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
@@ -19488,30 +19512,46 @@
         <f>IF(AB8=0,"Winner R3",AB8)</f>
         <v> Italy</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="48">
+        <v>3</v>
+      </c>
       <c r="E18" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="47"/>
+      <c r="F18" s="47">
+        <v>0</v>
+      </c>
       <c r="G18" s="25" t="str">
         <f>IF(AB9=0,"Winner R4",AB9)</f>
         <v> Poland</v>
       </c>
-      <c r="H18" s="28"/>
+      <c r="H18" s="28">
+        <v>25</v>
+      </c>
       <c r="I18" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="28"/>
+      <c r="J18" s="30">
+        <v>17</v>
+      </c>
+      <c r="K18" s="28">
+        <v>25</v>
+      </c>
       <c r="L18" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M18" s="30"/>
-      <c r="N18" s="28"/>
+      <c r="M18" s="30">
+        <v>21</v>
+      </c>
+      <c r="N18" s="28">
+        <v>25</v>
+      </c>
       <c r="O18" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P18" s="30"/>
+      <c r="P18" s="30">
+        <v>18</v>
+      </c>
       <c r="Q18" s="28"/>
       <c r="R18" s="29" t="s">
         <v>0</v>
@@ -19524,30 +19564,30 @@
       <c r="V18" s="30"/>
       <c r="W18" s="31">
         <f>SUM(H18,K18,N18,Q18,T18)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="X18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y18" s="32">
         <f>SUM(J18,M18,P18,S18,V18)</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AA18" s="12">
         <f t="shared" ref="AA18:AA20" si="21">AD18+AE18</f>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="12" t="str">
         <f t="shared" ref="AB18:AB20" si="22">IF(OR(D18="",F18=""),0,IF(D18&gt;F18,C18,G18))</f>
-        <v>0</v>
+        <v> Italy</v>
       </c>
       <c r="AC18" s="12">
         <f t="shared" ref="AC18:AC20" si="23">IF(OR(D18="",F18=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD18" s="12">
         <f t="shared" ref="AD18:AD20" si="24">IF(OR(D18="",F18=""),0,IF(D18&gt;F18,D18,F18))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" ref="AE18:AE20" si="25">IF(OR(D18="",F18=""),0,IF(D18&gt;F18,F18,D18))</f>
@@ -19555,7 +19595,7 @@
       </c>
       <c r="AF18" s="12">
         <f t="shared" ref="AF18:AF20" si="26">IF(AND(AD18=3,AE18=0),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" ref="AG18:AG20" si="27">IF(AND(AD18=3,AE18=1),1,0)</f>
@@ -19567,19 +19607,19 @@
       </c>
       <c r="AI18" s="12">
         <f t="shared" ref="AI18:AI20" si="29">IF(D18&gt;F18,SUM(H18,K18,N18,Q18,T18,),SUM(J18,M18,P18,S18,V18))</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AJ18" s="12">
         <f t="shared" ref="AJ18:AJ20" si="30">IF(D18&gt;F18,SUM(J18,M18,P18,S18,V18),SUM(H18,K18,N18,Q18,T18))</f>
-        <v>0</v>
-      </c>
-      <c r="AL18" s="12">
+        <v>56</v>
+      </c>
+      <c r="AL18" s="12" t="str">
         <f t="shared" ref="AL18:AL20" si="31">IF(OR(D18="",F18=""),0,IF(D18&lt;F18,C18,G18))</f>
-        <v>0</v>
+        <v> Poland</v>
       </c>
       <c r="AM18" s="12">
         <f t="shared" ref="AM18:AM20" si="32">IF(OR(D18="",F18=""),0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="12">
         <f t="shared" ref="AN18:AN20" si="33">IF(OR(D18="",F18=""),0,IF(D18&lt;F18,D18,F18))</f>
@@ -19587,7 +19627,7 @@
       </c>
       <c r="AO18" s="12">
         <f t="shared" ref="AO18:AO20" si="34">IF(OR(D18="",F18=""),0,IF(D18&lt;F18,F18,D18))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP18" s="12">
         <f t="shared" ref="AP18:AP20" si="35">IF(AND(AN18=2,AO18=3),1,0)</f>
@@ -19599,20 +19639,20 @@
       </c>
       <c r="AR18" s="12">
         <f t="shared" ref="AR18:AR20" si="37">IF(AND(AN18=0,AO18=3),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS18" s="12">
         <f t="shared" ref="AS18:AS20" si="38">IF(D18&lt;F18,SUM(H18,K18,N18,Q18,T18,),SUM(J18,M18,P18,S18,V18))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AT18" s="12">
         <f t="shared" ref="AT18:AT20" si="39">IF(D18&lt;F18,SUM(J18,M18,P18,S18,V18),SUM(H18,K18,N18,Q18,T18))</f>
-        <v>0</v>
-      </c>
-      <c r="AU18" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU18" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="AV18" s="68"/>
+      <c r="AV18" s="66"/>
     </row>
     <row r="19" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23">
@@ -19743,10 +19783,10 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AU19" s="67" t="s">
+      <c r="AU19" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="AV19" s="68"/>
+      <c r="AV19" s="66"/>
     </row>
     <row r="20" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23">
@@ -19877,10 +19917,10 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AU20" s="69" t="s">
+      <c r="AU20" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="AV20" s="70"/>
+      <c r="AV20" s="68"/>
     </row>
     <row r="21" spans="2:64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -19916,42 +19956,42 @@
         <v>86</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="76" t="s">
+      <c r="D23" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
       <c r="G23" s="36"/>
-      <c r="H23" s="75" t="s">
+      <c r="H23" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="75" t="s">
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="75" t="s">
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="75" t="s">
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R23" s="74"/>
-      <c r="S23" s="74"/>
-      <c r="T23" s="75" t="s">
+      <c r="R23" s="56"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U23" s="74"/>
-      <c r="V23" s="74"/>
-      <c r="W23" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X23" s="74"/>
-      <c r="Y23" s="74"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="56"/>
       <c r="AA23" s="12" t="s">
         <v>23</v>
       </c>
@@ -20016,7 +20056,7 @@
       </c>
       <c r="C24" s="24" t="str">
         <f>IF(AB17=0,"Winner Q1",AB17)</f>
-        <v>Winner Q1</v>
+        <v> Japan</v>
       </c>
       <c r="D24" s="48"/>
       <c r="E24" s="49" t="s">
@@ -20146,7 +20186,7 @@
       </c>
       <c r="C25" s="24" t="str">
         <f>IF(AB18=0,"Winner Q2",AB18)</f>
-        <v>Winner Q2</v>
+        <v> Italy</v>
       </c>
       <c r="D25" s="48"/>
       <c r="E25" s="49" t="s">
@@ -20323,42 +20363,42 @@
         <v>86</v>
       </c>
       <c r="C29" s="35"/>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
       <c r="G29" s="36"/>
-      <c r="H29" s="75" t="s">
+      <c r="H29" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="75" t="s">
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="75" t="s">
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="75" t="s">
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R29" s="74"/>
-      <c r="S29" s="74"/>
-      <c r="T29" s="75" t="s">
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U29" s="74"/>
-      <c r="V29" s="74"/>
-      <c r="W29" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="74"/>
-      <c r="Y29" s="74"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="56"/>
+      <c r="Y29" s="56"/>
       <c r="AA29" s="12" t="s">
         <v>23</v>
       </c>
@@ -20620,42 +20660,42 @@
         <v>86</v>
       </c>
       <c r="C34" s="35"/>
-      <c r="D34" s="76" t="s">
+      <c r="D34" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
       <c r="G34" s="36"/>
-      <c r="H34" s="75" t="s">
+      <c r="H34" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75" t="s">
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75" t="s">
+      <c r="L34" s="56"/>
+      <c r="M34" s="56"/>
+      <c r="N34" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="O34" s="74"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75" t="s">
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="R34" s="74"/>
-      <c r="S34" s="74"/>
-      <c r="T34" s="75" t="s">
+      <c r="R34" s="56"/>
+      <c r="S34" s="56"/>
+      <c r="T34" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="U34" s="74"/>
-      <c r="V34" s="74"/>
-      <c r="W34" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="X34" s="74"/>
-      <c r="Y34" s="74"/>
+      <c r="U34" s="56"/>
+      <c r="V34" s="56"/>
+      <c r="W34" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="X34" s="56"/>
+      <c r="Y34" s="56"/>
       <c r="AA34" s="12" t="s">
         <v>23</v>
       </c>
@@ -20973,6 +21013,38 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="48">
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="W34:Y34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="B33:Y33"/>
+    <mergeCell ref="AU15:AV15"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="AU16:AV16"/>
+    <mergeCell ref="AU17:AV17"/>
     <mergeCell ref="B2:AV2"/>
     <mergeCell ref="T16:V16"/>
     <mergeCell ref="W16:Y16"/>
@@ -20989,38 +21061,6 @@
     <mergeCell ref="AU18:AV18"/>
     <mergeCell ref="AU19:AV19"/>
     <mergeCell ref="AU20:AV20"/>
-    <mergeCell ref="B33:Y33"/>
-    <mergeCell ref="AU15:AV15"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="AU16:AV16"/>
-    <mergeCell ref="AU17:AV17"/>
-    <mergeCell ref="W34:Y34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="B4:Y4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W5:Y5"/>
   </mergeCells>
   <conditionalFormatting sqref="BM18:XFD18 BM22:XFD23 BM20:XFD20 A18:A20 Z18:Z20 A41:A1048576 B53:Y1048576 B38:Y47 B37 D37:Y37 Z41:AT1048576 BM41:XFD1048576 A3:XFD3 BM6:XFD15 A4:A15 B4:XFD4 Z22:AT22 AA5:AT13 Z26:AT28 Z23:Z25 Z29:Z30 B36:AT36 Z34:Z35 BM25:XFD36 A22:A36 Z31:AT33 Z5:XFD5 B14:AT15 B21:Y22 B28:Y28 B33:Y33 Z6:Z13 AW24:BL1048576 AU21:AV1048576">
     <cfRule type="cellIs" dxfId="31" priority="79" operator="equal">
@@ -21195,23 +21235,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -21444,32 +21467,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1A4F3B6-8EF3-43FC-AA6E-56F4B11E76F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21486,4 +21501,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5079BA11-B2F9-4F45-9320-B0ECAAE97A1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att Quarterfinals complete results
3th place on rank was incorrect
</commit_message>
<xml_diff>
--- a/2025 FIVB Women's Volleyball World Championship.xlsx
+++ b/2025 FIVB Women's Volleyball World Championship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C74E7559-C176-49CE-8522-E8DF5FE8FBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76048C2A-EA21-45D2-A56C-C624D1894FA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CC01" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" firstSheet="1" activeTab="2" xr2:uid="{701403F6-3112-456D-B33A-FC5595D41656}"/>
@@ -17687,7 +17687,7 @@
   <dimension ref="B1:BO48"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17715,21 +17715,19 @@
     <col min="25" max="25" width="4.7109375" style="12" customWidth="1"/>
     <col min="26" max="26" width="9.140625" style="12" customWidth="1"/>
     <col min="27" max="27" width="6.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" style="12" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="2.28515625" style="12" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="5.5703125" style="12" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="5.42578125" style="12" hidden="1" customWidth="1"/>
     <col min="32" max="34" width="4.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="3.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="3.42578125" style="12" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="2.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="21.140625" style="12" hidden="1" customWidth="1"/>
+    <col min="35" max="36" width="4.42578125" style="12" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="3.42578125" style="12" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="2.85546875" style="12" hidden="1" customWidth="1"/>
     <col min="39" max="39" width="2.28515625" style="12" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="5.5703125" style="12" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="5.42578125" style="12" hidden="1" customWidth="1"/>
     <col min="42" max="44" width="4.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="3.28515625" style="12" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="3.42578125" style="12" hidden="1" customWidth="1"/>
+    <col min="45" max="46" width="4.42578125" style="12" hidden="1" customWidth="1"/>
     <col min="47" max="47" width="4.7109375" style="12" customWidth="1"/>
     <col min="48" max="48" width="22.7109375" style="12" customWidth="1"/>
     <col min="49" max="49" width="4.7109375" style="12" customWidth="1"/>
@@ -19662,30 +19660,46 @@
         <f>IF(AB10=0,"Winner R5",AB10)</f>
         <v> Brazil</v>
       </c>
-      <c r="D19" s="48"/>
+      <c r="D19" s="48">
+        <v>3</v>
+      </c>
       <c r="E19" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="47"/>
+      <c r="F19" s="47">
+        <v>0</v>
+      </c>
       <c r="G19" s="25" t="str">
         <f>IF(AB11=0,"Winner R6",AB11)</f>
         <v> France</v>
       </c>
-      <c r="H19" s="28"/>
+      <c r="H19" s="28">
+        <v>27</v>
+      </c>
       <c r="I19" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J19" s="30"/>
-      <c r="K19" s="28"/>
+      <c r="J19" s="30">
+        <v>25</v>
+      </c>
+      <c r="K19" s="28">
+        <v>33</v>
+      </c>
       <c r="L19" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M19" s="30"/>
-      <c r="N19" s="28"/>
+      <c r="M19" s="30">
+        <v>31</v>
+      </c>
+      <c r="N19" s="28">
+        <v>25</v>
+      </c>
       <c r="O19" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P19" s="30"/>
+      <c r="P19" s="30">
+        <v>19</v>
+      </c>
       <c r="Q19" s="28"/>
       <c r="R19" s="29" t="s">
         <v>0</v>
@@ -19698,30 +19712,30 @@
       <c r="V19" s="30"/>
       <c r="W19" s="31">
         <f>SUM(H19,K19,N19,Q19,T19)</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="X19" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y19" s="32">
         <f>SUM(J19,M19,P19,S19,V19)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AA19" s="12">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="12" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v> Brazil</v>
       </c>
       <c r="AC19" s="12">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="25"/>
@@ -19729,7 +19743,7 @@
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="27"/>
@@ -19741,19 +19755,19 @@
       </c>
       <c r="AI19" s="12">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AJ19" s="12">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="AL19" s="12">
+        <v>75</v>
+      </c>
+      <c r="AL19" s="12" t="str">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v> France</v>
       </c>
       <c r="AM19" s="12">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN19" s="12">
         <f t="shared" si="33"/>
@@ -19761,7 +19775,7 @@
       </c>
       <c r="AO19" s="12">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP19" s="12">
         <f t="shared" si="35"/>
@@ -19773,15 +19787,15 @@
       </c>
       <c r="AR19" s="12">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS19" s="12">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AT19" s="12">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AU19" s="65" t="s">
         <v>44</v>
@@ -19796,35 +19810,55 @@
         <f>IF(AB12=0,"Winner R7",AB12)</f>
         <v> United States</v>
       </c>
-      <c r="D20" s="48"/>
+      <c r="D20" s="48">
+        <v>1</v>
+      </c>
       <c r="E20" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="47"/>
+      <c r="F20" s="47">
+        <v>3</v>
+      </c>
       <c r="G20" s="25" t="str">
         <f>IF(AB13=0,"Winner R8",AB13)</f>
         <v> Turkey</v>
       </c>
-      <c r="H20" s="28"/>
+      <c r="H20" s="28">
+        <v>14</v>
+      </c>
       <c r="I20" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="28"/>
+      <c r="J20" s="30">
+        <v>25</v>
+      </c>
+      <c r="K20" s="28">
+        <v>25</v>
+      </c>
       <c r="L20" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="M20" s="30"/>
-      <c r="N20" s="28"/>
+      <c r="M20" s="30">
+        <v>22</v>
+      </c>
+      <c r="N20" s="28">
+        <v>14</v>
+      </c>
       <c r="O20" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="28"/>
+      <c r="P20" s="30">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="28">
+        <v>23</v>
+      </c>
       <c r="R20" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="S20" s="30"/>
+      <c r="S20" s="30">
+        <v>25</v>
+      </c>
       <c r="T20" s="28"/>
       <c r="U20" s="29" t="s">
         <v>0</v>
@@ -19832,34 +19866,34 @@
       <c r="V20" s="30"/>
       <c r="W20" s="31">
         <f>SUM(H20,K20,N20,Q20,T20)</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="X20" s="29" t="s">
         <v>0</v>
       </c>
       <c r="Y20" s="32">
         <f>SUM(J20,M20,P20,S20,V20)</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AA20" s="12">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="12">
+        <v>4</v>
+      </c>
+      <c r="AB20" s="12" t="str">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v> Turkey</v>
       </c>
       <c r="AC20" s="12">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="26"/>
@@ -19867,7 +19901,7 @@
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH20" s="12">
         <f t="shared" si="28"/>
@@ -19875,27 +19909,27 @@
       </c>
       <c r="AI20" s="12">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AJ20" s="12">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="AL20" s="12">
+        <v>76</v>
+      </c>
+      <c r="AL20" s="12" t="str">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v> United States</v>
       </c>
       <c r="AM20" s="12">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN20" s="12">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO20" s="12">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP20" s="12">
         <f t="shared" si="35"/>
@@ -19903,7 +19937,7 @@
       </c>
       <c r="AQ20" s="12">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR20" s="12">
         <f t="shared" si="37"/>
@@ -19911,11 +19945,11 @@
       </c>
       <c r="AS20" s="12">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="AT20" s="12">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AU20" s="67" t="s">
         <v>45</v>
@@ -20065,7 +20099,7 @@
       <c r="F24" s="47"/>
       <c r="G24" s="25" t="str">
         <f>IF(AB20=0,"Winner Q4",AB20)</f>
-        <v>Winner Q4</v>
+        <v> Turkey</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="29" t="s">
@@ -20195,7 +20229,7 @@
       <c r="F25" s="47"/>
       <c r="G25" s="25" t="str">
         <f>IF(AB19=0,"Winner Q3",AB19)</f>
-        <v>Winner Q3</v>
+        <v> Brazil</v>
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="29" t="s">
@@ -20917,7 +20951,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="53" t="str">
-        <f>IF(AB25=0,"Champion",AB25)</f>
+        <f>IF(AB35=0,"Champion",AB35)</f>
         <v>Champion</v>
       </c>
       <c r="D38" s="43"/>
@@ -20948,7 +20982,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="54" t="str">
-        <f>IF(AL25=0,"Runner Up",AL25)</f>
+        <f>IF(AL35=0,"Runner Up",AL35)</f>
         <v>Runner Up</v>
       </c>
       <c r="D39" s="43"/>
@@ -20979,7 +21013,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="54" t="str">
-        <f>IF(AB20=0,"3rd",AB20)</f>
+        <f>IF(AB30=0,"3rd",AB30)</f>
         <v>3rd</v>
       </c>
       <c r="D40" s="43"/>
@@ -21514,16 +21548,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0F6A83-8A20-4128-AC08-526BDD0F4F5D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>